<commit_message>
Finish array pointer blog, prepare for func pointer
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="40200" yWindow="108" windowWidth="3720" windowHeight="6096"/>
+    <workbookView xWindow="41976" yWindow="108" windowWidth="3720" windowHeight="6096"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="115">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -408,6 +408,10 @@
   </si>
   <si>
     <t>20220323</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220325</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -876,7 +880,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1636,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>

</xml_diff>

<commit_message>
Finish Eulerian circuit and LeetCode 332
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED90B23-FD72-482C-8F59-A1B7FF7626A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48192" yWindow="108" windowWidth="3720" windowHeight="6096"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="122">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -408,10 +409,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20220401</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20220402</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -425,23 +422,41 @@
   <si>
     <t>20220407</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NP问题与算法思路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220408</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220408</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220409</t>
+  </si>
+  <si>
+    <t>LeetCode经验与技巧</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -450,7 +465,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -459,7 +474,7 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -467,7 +482,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -614,7 +629,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -689,6 +704,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -724,6 +756,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -899,15 +948,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC192"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.77734375" style="1" customWidth="1"/>
@@ -917,7 +966,7 @@
     <col min="6" max="6" width="12.5546875" style="21" customWidth="1"/>
     <col min="7" max="7" width="3" style="19" customWidth="1"/>
     <col min="8" max="8" width="26.77734375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="42" style="1" customWidth="1"/>
+    <col min="9" max="9" width="49.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.44140625" style="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.88671875" style="21" customWidth="1"/>
@@ -925,7 +974,7 @@
     <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -980,7 +1029,7 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" s="1" customFormat="1">
       <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1056,7 @@
       <c r="L2" s="14"/>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29">
       <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1099,7 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="4" customFormat="1">
       <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
@@ -1071,11 +1120,11 @@
         <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="12"/>
+      <c r="M4" s="11"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1093,7 +1142,7 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29">
       <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1185,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" s="22" t="s">
         <v>0</v>
       </c>
@@ -1179,7 +1228,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="A7" s="22" t="s">
         <v>0</v>
       </c>
@@ -1187,11 +1236,11 @@
         <v>62</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="25"/>
+        <v>120</v>
+      </c>
+      <c r="D7" s="9"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="24"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="18"/>
       <c r="H7" s="22" t="s">
         <v>3</v>
@@ -1222,7 +1271,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29">
       <c r="A8" s="22" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1314,7 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9" s="22" t="s">
         <v>0</v>
       </c>
@@ -1308,7 +1357,7 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="A10" s="22" t="s">
         <v>0</v>
       </c>
@@ -1326,14 +1375,14 @@
         <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K10" s="9"/>
+        <v>120</v>
+      </c>
+      <c r="K10" s="24"/>
       <c r="L10" s="10"/>
-      <c r="M10" s="11"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1351,7 +1400,7 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29">
       <c r="A11" s="22" t="s">
         <v>0</v>
       </c>
@@ -1369,13 +1418,13 @@
         <v>3</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K11" s="9"/>
-      <c r="L11" s="3"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="11"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1394,7 +1443,7 @@
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29">
       <c r="A12" s="22" t="s">
         <v>0</v>
       </c>
@@ -1409,16 +1458,16 @@
       <c r="F12" s="12"/>
       <c r="G12" s="18"/>
       <c r="H12" s="22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="11"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1437,7 +1486,7 @@
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29">
       <c r="A13" s="22" t="s">
         <v>0</v>
       </c>
@@ -1451,14 +1500,14 @@
       <c r="E13" s="10"/>
       <c r="F13" s="12"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="22" t="s">
-        <v>6</v>
+      <c r="H13" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="10"/>
@@ -1480,7 +1529,7 @@
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29">
       <c r="A14" s="22" t="s">
         <v>0</v>
       </c>
@@ -1494,14 +1543,14 @@
       <c r="E14" s="10"/>
       <c r="F14" s="12"/>
       <c r="G14" s="18"/>
-      <c r="H14" s="22" t="s">
-        <v>6</v>
+      <c r="H14" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="10"/>
@@ -1523,7 +1572,7 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29">
       <c r="A15" s="22" t="s">
         <v>0</v>
       </c>
@@ -1531,17 +1580,17 @@
         <v>77</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="18"/>
-      <c r="H15" s="22" t="s">
-        <v>6</v>
+      <c r="H15" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>78</v>
@@ -1566,7 +1615,7 @@
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29">
       <c r="A16" s="22" t="s">
         <v>0</v>
       </c>
@@ -1580,17 +1629,17 @@
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="18"/>
-      <c r="H16" s="22" t="s">
-        <v>6</v>
+      <c r="H16" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K16" s="9"/>
-      <c r="L16" s="10"/>
+      <c r="L16" s="3"/>
       <c r="M16" s="11"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1609,25 +1658,25 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29">
       <c r="A17" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="9"/>
+        <v>118</v>
+      </c>
+      <c r="D17" s="25"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>26</v>
+      <c r="H17" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>78</v>
@@ -1652,28 +1701,28 @@
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29">
       <c r="A18" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="12"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="18"/>
       <c r="H18" s="23" t="s">
         <v>81</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="10"/>
@@ -1695,28 +1744,28 @@
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29">
       <c r="A19" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="12"/>
       <c r="G19" s="18"/>
       <c r="H19" s="23" t="s">
         <v>81</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="10"/>
@@ -1738,28 +1787,28 @@
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29">
       <c r="A20" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="11"/>
       <c r="G20" s="18"/>
       <c r="H20" s="23" t="s">
         <v>81</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="3"/>
@@ -1781,31 +1830,31 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29">
       <c r="A21" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="12"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="11"/>
       <c r="G21" s="18"/>
       <c r="H21" s="23" t="s">
         <v>81</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="K21" s="9"/>
-      <c r="L21" s="3"/>
+      <c r="L21" s="10"/>
       <c r="M21" s="11"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1824,28 +1873,28 @@
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
-    <row r="22" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="A22" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="18"/>
       <c r="H22" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>64</v>
+      <c r="I22" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="10"/>
@@ -1867,32 +1916,32 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
     </row>
-    <row r="23" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="A23" s="22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="12"/>
+      <c r="F23" s="11"/>
       <c r="G23" s="18"/>
       <c r="H23" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="K23" s="9"/>
+      <c r="I23" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" s="14"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="11"/>
+      <c r="M23" s="12"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1910,32 +1959,32 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
     </row>
-    <row r="24" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>2</v>
+    <row r="24" spans="1:29" ht="17.399999999999999" customHeight="1">
+      <c r="A24" s="15" t="s">
+        <v>107</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="23" t="s">
-        <v>81</v>
+      <c r="H24" s="22" t="s">
+        <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="11"/>
+      <c r="M24" s="12"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1953,31 +2002,31 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
     </row>
-    <row r="25" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+    <row r="25" spans="1:29" ht="17.399999999999999" customHeight="1">
+      <c r="A25" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="I25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="K25" s="9"/>
-      <c r="L25" s="3"/>
+      <c r="L25" s="10"/>
       <c r="M25" s="11"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1996,28 +2045,16 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
     </row>
-    <row r="26" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11"/>
+    <row r="26" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="G26" s="18"/>
-      <c r="H26" s="23" t="s">
-        <v>81</v>
+      <c r="H26" s="22" t="s">
+        <v>2</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="10"/>
@@ -2039,32 +2076,14 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
     </row>
-    <row r="27" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="12"/>
+    <row r="27" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="G27" s="18"/>
-      <c r="H27" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K27" s="9"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="11"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="12"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -2082,25 +2101,13 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+    <row r="28" spans="1:29">
       <c r="G28" s="18"/>
-      <c r="H28" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>101</v>
-      </c>
+      <c r="H28" s="13"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
       <c r="K28" s="14"/>
-      <c r="L28" s="10"/>
+      <c r="L28" s="14"/>
       <c r="M28" s="12"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -2119,7 +2126,13 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29">
+      <c r="A29" s="15"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="18"/>
       <c r="H29" s="13"/>
       <c r="I29" s="14"/>
@@ -2144,13 +2157,13 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29">
       <c r="G30" s="18"/>
       <c r="H30" s="13"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
+      <c r="L30" s="12"/>
       <c r="M30" s="12"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -2169,13 +2182,13 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
     </row>
-    <row r="31" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="G31" s="18"/>
       <c r="H31" s="13"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
-      <c r="L31" s="12"/>
+      <c r="L31" s="14"/>
       <c r="M31" s="12"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2194,7 +2207,7 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
     </row>
-    <row r="32" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="G32" s="18"/>
       <c r="H32" s="13"/>
       <c r="I32" s="14"/>
@@ -2219,20 +2232,8 @@
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
     </row>
-    <row r="33" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+    <row r="33" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="G33" s="18"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="12"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -2250,7 +2251,7 @@
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
     </row>
-    <row r="34" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="A34" s="13"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -2258,12 +2259,6 @@
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="18"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="12"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -2281,7 +2276,7 @@
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
     </row>
-    <row r="35" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="A35" s="13"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -2289,12 +2284,6 @@
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="18"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -2312,7 +2301,7 @@
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29">
       <c r="A36" s="13"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -2324,7 +2313,7 @@
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
+      <c r="L36" s="12"/>
       <c r="M36" s="12"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -2343,7 +2332,7 @@
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
     </row>
-    <row r="37" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="A37" s="13"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -2355,7 +2344,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
+      <c r="L37" s="12"/>
       <c r="M37" s="12"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -2374,7 +2363,7 @@
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
     </row>
-    <row r="38" spans="1:29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" ht="17.399999999999999" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2382,6 +2371,12 @@
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="18"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -2399,7 +2394,7 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29">
       <c r="A39" s="13"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -2407,6 +2402,12 @@
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="18"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -2424,7 +2425,7 @@
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29">
       <c r="A40" s="13"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -2432,6 +2433,12 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="18"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -2449,7 +2456,7 @@
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29">
       <c r="A41" s="13"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -2480,7 +2487,7 @@
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29">
       <c r="A42" s="13"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -2511,7 +2518,7 @@
       <c r="AB42" s="1"/>
       <c r="AC42" s="1"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29">
       <c r="A43" s="13"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2519,7 +2526,7 @@
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="18"/>
-      <c r="H43" s="15"/>
+      <c r="H43" s="13"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
@@ -2542,7 +2549,7 @@
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29">
       <c r="A44" s="13"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2573,7 +2580,7 @@
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29">
       <c r="A45" s="13"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2604,7 +2611,7 @@
       <c r="AB45" s="1"/>
       <c r="AC45" s="1"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29">
       <c r="A46" s="13"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2635,7 +2642,7 @@
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29">
       <c r="A47" s="13"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -2666,12 +2673,12 @@
       <c r="AB47" s="1"/>
       <c r="AC47" s="1"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29">
       <c r="A48" s="13"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
+      <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="18"/>
       <c r="H48" s="13"/>
@@ -2697,12 +2704,12 @@
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29">
       <c r="A49" s="13"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
-      <c r="E49" s="12"/>
+      <c r="E49" s="14"/>
       <c r="F49" s="12"/>
       <c r="G49" s="18"/>
       <c r="H49" s="13"/>
@@ -2728,7 +2735,7 @@
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29">
       <c r="A50" s="13"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -2759,7 +2766,7 @@
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29">
       <c r="A51" s="13"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -2790,7 +2797,7 @@
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29">
       <c r="A52" s="13"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -2821,19 +2828,19 @@
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29">
       <c r="A53" s="13"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
+      <c r="E53" s="12"/>
       <c r="F53" s="12"/>
       <c r="G53" s="18"/>
       <c r="H53" s="13"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
       <c r="K53" s="14"/>
-      <c r="L53" s="12"/>
+      <c r="L53" s="14"/>
       <c r="M53" s="12"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2852,12 +2859,12 @@
       <c r="AB53" s="1"/>
       <c r="AC53" s="1"/>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29">
       <c r="A54" s="13"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
-      <c r="E54" s="12"/>
+      <c r="E54" s="14"/>
       <c r="F54" s="12"/>
       <c r="G54" s="18"/>
       <c r="H54" s="13"/>
@@ -2883,7 +2890,7 @@
       <c r="AB54" s="1"/>
       <c r="AC54" s="1"/>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29">
       <c r="A55" s="13"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -2914,7 +2921,7 @@
       <c r="AB55" s="1"/>
       <c r="AC55" s="1"/>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29">
       <c r="A56" s="13"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -2945,7 +2952,7 @@
       <c r="AB56" s="1"/>
       <c r="AC56" s="1"/>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29">
       <c r="A57" s="13"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -2976,7 +2983,7 @@
       <c r="AB57" s="1"/>
       <c r="AC57" s="1"/>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29">
       <c r="A58" s="13"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
@@ -3007,7 +3014,7 @@
       <c r="AB58" s="1"/>
       <c r="AC58" s="1"/>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29">
       <c r="A59" s="13"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
@@ -3038,7 +3045,7 @@
       <c r="AB59" s="1"/>
       <c r="AC59" s="1"/>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29">
       <c r="A60" s="13"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -3069,8 +3076,8 @@
       <c r="AB60" s="1"/>
       <c r="AC60" s="1"/>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+    <row r="61" spans="1:29">
+      <c r="A61" s="13"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -3100,8 +3107,8 @@
       <c r="AB61" s="1"/>
       <c r="AC61" s="1"/>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
+    <row r="62" spans="1:29">
+      <c r="A62" s="15"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
@@ -3131,7 +3138,7 @@
       <c r="AB62" s="1"/>
       <c r="AC62" s="1"/>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29">
       <c r="A63" s="13"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -3143,7 +3150,7 @@
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
       <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
+      <c r="L63" s="12"/>
       <c r="M63" s="12"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
@@ -3162,8 +3169,8 @@
       <c r="AB63" s="1"/>
       <c r="AC63" s="1"/>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+    <row r="64" spans="1:29">
+      <c r="A64" s="13"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
@@ -3193,13 +3200,13 @@
       <c r="AB64" s="1"/>
       <c r="AC64" s="1"/>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29">
       <c r="A65" s="16"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
       <c r="G65" s="18"/>
       <c r="H65" s="13"/>
       <c r="I65" s="14"/>
@@ -3224,7 +3231,7 @@
       <c r="AB65" s="1"/>
       <c r="AC65" s="1"/>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29">
       <c r="A66" s="16"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
@@ -3255,7 +3262,7 @@
       <c r="AB66" s="1"/>
       <c r="AC66" s="1"/>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29">
       <c r="A67" s="16"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -3263,7 +3270,7 @@
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
       <c r="G67" s="18"/>
-      <c r="H67" s="13"/>
+      <c r="H67" s="15"/>
       <c r="I67" s="14"/>
       <c r="J67" s="14"/>
       <c r="K67" s="14"/>
@@ -3286,7 +3293,7 @@
       <c r="AB67" s="1"/>
       <c r="AC67" s="1"/>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29">
       <c r="A68" s="16"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
@@ -3317,7 +3324,7 @@
       <c r="AB68" s="1"/>
       <c r="AC68" s="1"/>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29">
       <c r="A69" s="16"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -3348,7 +3355,7 @@
       <c r="AB69" s="1"/>
       <c r="AC69" s="1"/>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29">
       <c r="A70" s="16"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -3356,12 +3363,8 @@
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
       <c r="G70" s="18"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="12"/>
-      <c r="M70" s="12"/>
+      <c r="H70" s="5"/>
+      <c r="J70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
@@ -3379,7 +3382,7 @@
       <c r="AB70" s="1"/>
       <c r="AC70" s="1"/>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29">
       <c r="A71" s="16"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -3387,12 +3390,8 @@
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
       <c r="G71" s="18"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="12"/>
-      <c r="M71" s="12"/>
+      <c r="H71" s="5"/>
+      <c r="J71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
@@ -3410,7 +3409,7 @@
       <c r="AB71" s="1"/>
       <c r="AC71" s="1"/>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29">
       <c r="A72" s="16"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
@@ -3418,12 +3417,8 @@
       <c r="E72" s="20"/>
       <c r="F72" s="20"/>
       <c r="G72" s="18"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-      <c r="K72" s="14"/>
-      <c r="L72" s="12"/>
-      <c r="M72" s="12"/>
+      <c r="H72" s="5"/>
+      <c r="J72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -3441,7 +3436,7 @@
       <c r="AB72" s="1"/>
       <c r="AC72" s="1"/>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29">
       <c r="A73" s="16"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -3449,12 +3444,8 @@
       <c r="E73" s="20"/>
       <c r="F73" s="20"/>
       <c r="G73" s="18"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="L73" s="12"/>
-      <c r="M73" s="12"/>
+      <c r="H73" s="5"/>
+      <c r="J73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -3472,7 +3463,7 @@
       <c r="AB73" s="1"/>
       <c r="AC73" s="1"/>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29">
       <c r="A74" s="16"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
@@ -3480,12 +3471,8 @@
       <c r="E74" s="20"/>
       <c r="F74" s="20"/>
       <c r="G74" s="18"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14"/>
-      <c r="L74" s="12"/>
-      <c r="M74" s="12"/>
+      <c r="H74" s="5"/>
+      <c r="J74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
@@ -3503,7 +3490,7 @@
       <c r="AB74" s="1"/>
       <c r="AC74" s="1"/>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29">
       <c r="A75" s="16"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -3530,7 +3517,7 @@
       <c r="AB75" s="1"/>
       <c r="AC75" s="1"/>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29">
       <c r="A76" s="16"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
@@ -3557,7 +3544,7 @@
       <c r="AB76" s="1"/>
       <c r="AC76" s="1"/>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29">
       <c r="A77" s="16"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
@@ -3584,7 +3571,7 @@
       <c r="AB77" s="1"/>
       <c r="AC77" s="1"/>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29">
       <c r="A78" s="16"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
@@ -3611,7 +3598,7 @@
       <c r="AB78" s="1"/>
       <c r="AC78" s="1"/>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29">
       <c r="A79" s="16"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
@@ -3638,7 +3625,7 @@
       <c r="AB79" s="1"/>
       <c r="AC79" s="1"/>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29">
       <c r="A80" s="16"/>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
@@ -3665,7 +3652,7 @@
       <c r="AB80" s="1"/>
       <c r="AC80" s="1"/>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29">
       <c r="A81" s="16"/>
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
@@ -3692,7 +3679,7 @@
       <c r="AB81" s="1"/>
       <c r="AC81" s="1"/>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29">
       <c r="A82" s="16"/>
       <c r="B82" s="14"/>
       <c r="C82" s="14"/>
@@ -3719,7 +3706,7 @@
       <c r="AB82" s="1"/>
       <c r="AC82" s="1"/>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29">
       <c r="A83" s="16"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
@@ -3746,7 +3733,7 @@
       <c r="AB83" s="1"/>
       <c r="AC83" s="1"/>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29">
       <c r="A84" s="16"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
@@ -3773,7 +3760,7 @@
       <c r="AB84" s="1"/>
       <c r="AC84" s="1"/>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29">
       <c r="A85" s="16"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
@@ -3800,7 +3787,7 @@
       <c r="AB85" s="1"/>
       <c r="AC85" s="1"/>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29">
       <c r="A86" s="16"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -3827,7 +3814,7 @@
       <c r="AB86" s="1"/>
       <c r="AC86" s="1"/>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29">
       <c r="A87" s="16"/>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
@@ -3854,7 +3841,7 @@
       <c r="AB87" s="1"/>
       <c r="AC87" s="1"/>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:29">
       <c r="A88" s="16"/>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
@@ -3881,7 +3868,7 @@
       <c r="AB88" s="1"/>
       <c r="AC88" s="1"/>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:29">
       <c r="A89" s="16"/>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
@@ -3908,7 +3895,7 @@
       <c r="AB89" s="1"/>
       <c r="AC89" s="1"/>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:29">
       <c r="A90" s="16"/>
       <c r="B90" s="14"/>
       <c r="C90" s="14"/>
@@ -3935,7 +3922,7 @@
       <c r="AB90" s="1"/>
       <c r="AC90" s="1"/>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:29">
       <c r="A91" s="16"/>
       <c r="B91" s="14"/>
       <c r="C91" s="14"/>
@@ -3962,7 +3949,7 @@
       <c r="AB91" s="1"/>
       <c r="AC91" s="1"/>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:29">
       <c r="A92" s="16"/>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
@@ -3989,7 +3976,7 @@
       <c r="AB92" s="1"/>
       <c r="AC92" s="1"/>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:29">
       <c r="A93" s="16"/>
       <c r="B93" s="14"/>
       <c r="C93" s="14"/>
@@ -4016,7 +4003,7 @@
       <c r="AB93" s="1"/>
       <c r="AC93" s="1"/>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:29">
       <c r="A94" s="16"/>
       <c r="B94" s="14"/>
       <c r="C94" s="14"/>
@@ -4043,7 +4030,7 @@
       <c r="AB94" s="1"/>
       <c r="AC94" s="1"/>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:29">
       <c r="A95" s="16"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
@@ -4070,7 +4057,7 @@
       <c r="AB95" s="1"/>
       <c r="AC95" s="1"/>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29">
       <c r="A96" s="16"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
@@ -4097,7 +4084,7 @@
       <c r="AB96" s="1"/>
       <c r="AC96" s="1"/>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:29">
       <c r="A97" s="16"/>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>
@@ -4124,7 +4111,7 @@
       <c r="AB97" s="1"/>
       <c r="AC97" s="1"/>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:29">
       <c r="A98" s="16"/>
       <c r="B98" s="14"/>
       <c r="C98" s="14"/>
@@ -4151,7 +4138,7 @@
       <c r="AB98" s="1"/>
       <c r="AC98" s="1"/>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:29">
       <c r="A99" s="16"/>
       <c r="B99" s="14"/>
       <c r="C99" s="14"/>
@@ -4178,7 +4165,7 @@
       <c r="AB99" s="1"/>
       <c r="AC99" s="1"/>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:29">
       <c r="A100" s="16"/>
       <c r="B100" s="14"/>
       <c r="C100" s="14"/>
@@ -4205,7 +4192,7 @@
       <c r="AB100" s="1"/>
       <c r="AC100" s="1"/>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:29">
       <c r="A101" s="16"/>
       <c r="B101" s="14"/>
       <c r="C101" s="14"/>
@@ -4232,7 +4219,7 @@
       <c r="AB101" s="1"/>
       <c r="AC101" s="1"/>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:29">
       <c r="A102" s="16"/>
       <c r="B102" s="14"/>
       <c r="C102" s="14"/>
@@ -4259,7 +4246,7 @@
       <c r="AB102" s="1"/>
       <c r="AC102" s="1"/>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:29">
       <c r="A103" s="16"/>
       <c r="B103" s="14"/>
       <c r="C103" s="14"/>
@@ -4286,7 +4273,7 @@
       <c r="AB103" s="1"/>
       <c r="AC103" s="1"/>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:29">
       <c r="A104" s="16"/>
       <c r="B104" s="14"/>
       <c r="C104" s="14"/>
@@ -4313,7 +4300,7 @@
       <c r="AB104" s="1"/>
       <c r="AC104" s="1"/>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:29">
       <c r="A105" s="16"/>
       <c r="B105" s="14"/>
       <c r="C105" s="14"/>
@@ -4340,7 +4327,7 @@
       <c r="AB105" s="1"/>
       <c r="AC105" s="1"/>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:29">
       <c r="A106" s="16"/>
       <c r="B106" s="14"/>
       <c r="C106" s="14"/>
@@ -4367,7 +4354,7 @@
       <c r="AB106" s="1"/>
       <c r="AC106" s="1"/>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:29">
       <c r="A107" s="16"/>
       <c r="B107" s="14"/>
       <c r="C107" s="14"/>
@@ -4394,7 +4381,7 @@
       <c r="AB107" s="1"/>
       <c r="AC107" s="1"/>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:29">
       <c r="A108" s="16"/>
       <c r="B108" s="14"/>
       <c r="C108" s="14"/>
@@ -4421,7 +4408,7 @@
       <c r="AB108" s="1"/>
       <c r="AC108" s="1"/>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:29">
       <c r="A109" s="16"/>
       <c r="B109" s="14"/>
       <c r="C109" s="14"/>
@@ -4448,7 +4435,7 @@
       <c r="AB109" s="1"/>
       <c r="AC109" s="1"/>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:29">
       <c r="A110" s="16"/>
       <c r="B110" s="14"/>
       <c r="C110" s="14"/>
@@ -4475,7 +4462,7 @@
       <c r="AB110" s="1"/>
       <c r="AC110" s="1"/>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:29">
       <c r="A111" s="16"/>
       <c r="B111" s="14"/>
       <c r="C111" s="14"/>
@@ -4502,7 +4489,7 @@
       <c r="AB111" s="1"/>
       <c r="AC111" s="1"/>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:29">
       <c r="A112" s="16"/>
       <c r="B112" s="14"/>
       <c r="C112" s="14"/>
@@ -4529,7 +4516,7 @@
       <c r="AB112" s="1"/>
       <c r="AC112" s="1"/>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:29">
       <c r="A113" s="16"/>
       <c r="B113" s="14"/>
       <c r="C113" s="14"/>
@@ -4556,7 +4543,7 @@
       <c r="AB113" s="1"/>
       <c r="AC113" s="1"/>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:29">
       <c r="A114" s="16"/>
       <c r="B114" s="14"/>
       <c r="C114" s="14"/>
@@ -4583,7 +4570,7 @@
       <c r="AB114" s="1"/>
       <c r="AC114" s="1"/>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:29">
       <c r="A115" s="16"/>
       <c r="B115" s="14"/>
       <c r="C115" s="14"/>
@@ -4610,7 +4597,7 @@
       <c r="AB115" s="1"/>
       <c r="AC115" s="1"/>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:29">
       <c r="A116" s="16"/>
       <c r="B116" s="14"/>
       <c r="C116" s="14"/>
@@ -4637,7 +4624,7 @@
       <c r="AB116" s="1"/>
       <c r="AC116" s="1"/>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:29">
       <c r="A117" s="16"/>
       <c r="B117" s="14"/>
       <c r="C117" s="14"/>
@@ -4664,7 +4651,7 @@
       <c r="AB117" s="1"/>
       <c r="AC117" s="1"/>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:29">
       <c r="A118" s="16"/>
       <c r="B118" s="14"/>
       <c r="C118" s="14"/>
@@ -4691,7 +4678,7 @@
       <c r="AB118" s="1"/>
       <c r="AC118" s="1"/>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:29">
       <c r="A119" s="16"/>
       <c r="B119" s="14"/>
       <c r="C119" s="14"/>
@@ -4718,7 +4705,7 @@
       <c r="AB119" s="1"/>
       <c r="AC119" s="1"/>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:29">
       <c r="A120" s="16"/>
       <c r="B120" s="14"/>
       <c r="C120" s="14"/>
@@ -4745,7 +4732,7 @@
       <c r="AB120" s="1"/>
       <c r="AC120" s="1"/>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:29">
       <c r="A121" s="16"/>
       <c r="B121" s="14"/>
       <c r="C121" s="14"/>
@@ -4772,7 +4759,7 @@
       <c r="AB121" s="1"/>
       <c r="AC121" s="1"/>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:29">
       <c r="A122" s="16"/>
       <c r="B122" s="14"/>
       <c r="C122" s="14"/>
@@ -4799,7 +4786,7 @@
       <c r="AB122" s="1"/>
       <c r="AC122" s="1"/>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:29">
       <c r="A123" s="16"/>
       <c r="B123" s="14"/>
       <c r="C123" s="14"/>
@@ -4826,7 +4813,7 @@
       <c r="AB123" s="1"/>
       <c r="AC123" s="1"/>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:29">
       <c r="A124" s="16"/>
       <c r="B124" s="14"/>
       <c r="C124" s="14"/>
@@ -4853,10 +4840,10 @@
       <c r="AB124" s="1"/>
       <c r="AC124" s="1"/>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:29">
       <c r="A125" s="16"/>
       <c r="B125" s="14"/>
-      <c r="C125" s="17"/>
+      <c r="C125" s="14"/>
       <c r="D125" s="20"/>
       <c r="E125" s="20"/>
       <c r="F125" s="20"/>
@@ -4880,7 +4867,7 @@
       <c r="AB125" s="1"/>
       <c r="AC125" s="1"/>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:29">
       <c r="A126" s="16"/>
       <c r="B126" s="14"/>
       <c r="C126" s="17"/>
@@ -4907,7 +4894,7 @@
       <c r="AB126" s="1"/>
       <c r="AC126" s="1"/>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:29">
       <c r="A127" s="16"/>
       <c r="B127" s="14"/>
       <c r="C127" s="17"/>
@@ -4934,7 +4921,7 @@
       <c r="AB127" s="1"/>
       <c r="AC127" s="1"/>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:29">
       <c r="A128" s="16"/>
       <c r="B128" s="14"/>
       <c r="C128" s="17"/>
@@ -4961,7 +4948,7 @@
       <c r="AB128" s="1"/>
       <c r="AC128" s="1"/>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:29">
       <c r="A129" s="16"/>
       <c r="B129" s="14"/>
       <c r="C129" s="17"/>
@@ -4988,7 +4975,7 @@
       <c r="AB129" s="1"/>
       <c r="AC129" s="1"/>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:29">
       <c r="A130" s="16"/>
       <c r="B130" s="14"/>
       <c r="C130" s="17"/>
@@ -4997,7 +4984,6 @@
       <c r="F130" s="20"/>
       <c r="G130" s="18"/>
       <c r="H130" s="5"/>
-      <c r="J130" s="1"/>
       <c r="N130" s="1"/>
       <c r="O130" s="1"/>
       <c r="P130" s="1"/>
@@ -5015,7 +5001,7 @@
       <c r="AB130" s="1"/>
       <c r="AC130" s="1"/>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:29">
       <c r="A131" s="16"/>
       <c r="B131" s="14"/>
       <c r="C131" s="17"/>
@@ -5024,7 +5010,6 @@
       <c r="F131" s="20"/>
       <c r="G131" s="18"/>
       <c r="H131" s="5"/>
-      <c r="J131" s="1"/>
       <c r="N131" s="1"/>
       <c r="O131" s="1"/>
       <c r="P131" s="1"/>
@@ -5042,7 +5027,7 @@
       <c r="AB131" s="1"/>
       <c r="AC131" s="1"/>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:29">
       <c r="A132" s="16"/>
       <c r="B132" s="14"/>
       <c r="C132" s="17"/>
@@ -5051,7 +5036,6 @@
       <c r="F132" s="20"/>
       <c r="G132" s="18"/>
       <c r="H132" s="5"/>
-      <c r="J132" s="1"/>
       <c r="N132" s="1"/>
       <c r="O132" s="1"/>
       <c r="P132" s="1"/>
@@ -5069,7 +5053,7 @@
       <c r="AB132" s="1"/>
       <c r="AC132" s="1"/>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:29">
       <c r="A133" s="16"/>
       <c r="B133" s="14"/>
       <c r="C133" s="17"/>
@@ -5078,7 +5062,6 @@
       <c r="F133" s="20"/>
       <c r="G133" s="18"/>
       <c r="H133" s="5"/>
-      <c r="J133" s="1"/>
       <c r="N133" s="1"/>
       <c r="O133" s="1"/>
       <c r="P133" s="1"/>
@@ -5096,7 +5079,7 @@
       <c r="AB133" s="1"/>
       <c r="AC133" s="1"/>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:29">
       <c r="A134" s="16"/>
       <c r="B134" s="14"/>
       <c r="C134" s="17"/>
@@ -5105,7 +5088,6 @@
       <c r="F134" s="20"/>
       <c r="G134" s="18"/>
       <c r="H134" s="5"/>
-      <c r="J134" s="1"/>
       <c r="N134" s="1"/>
       <c r="O134" s="1"/>
       <c r="P134" s="1"/>
@@ -5123,7 +5105,7 @@
       <c r="AB134" s="1"/>
       <c r="AC134" s="1"/>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:29">
       <c r="A135" s="16"/>
       <c r="B135" s="14"/>
       <c r="C135" s="17"/>
@@ -5132,7 +5114,7 @@
       <c r="F135" s="20"/>
       <c r="H135" s="5"/>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:29">
       <c r="A136" s="16"/>
       <c r="B136" s="14"/>
       <c r="C136" s="17"/>
@@ -5141,7 +5123,7 @@
       <c r="F136" s="20"/>
       <c r="H136" s="5"/>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:29">
       <c r="A137" s="16"/>
       <c r="B137" s="14"/>
       <c r="C137" s="17"/>
@@ -5150,7 +5132,7 @@
       <c r="F137" s="20"/>
       <c r="H137" s="5"/>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:29">
       <c r="A138" s="16"/>
       <c r="B138" s="14"/>
       <c r="C138" s="17"/>
@@ -5159,7 +5141,7 @@
       <c r="F138" s="20"/>
       <c r="H138" s="5"/>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:29">
       <c r="A139" s="16"/>
       <c r="B139" s="14"/>
       <c r="C139" s="17"/>
@@ -5168,7 +5150,7 @@
       <c r="F139" s="20"/>
       <c r="H139" s="5"/>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:29">
       <c r="A140" s="16"/>
       <c r="B140" s="14"/>
       <c r="C140" s="17"/>
@@ -5177,7 +5159,7 @@
       <c r="F140" s="20"/>
       <c r="H140" s="5"/>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:29">
       <c r="A141" s="16"/>
       <c r="B141" s="14"/>
       <c r="C141" s="17"/>
@@ -5186,7 +5168,7 @@
       <c r="F141" s="20"/>
       <c r="H141" s="5"/>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:29">
       <c r="A142" s="16"/>
       <c r="B142" s="14"/>
       <c r="C142" s="17"/>
@@ -5195,7 +5177,7 @@
       <c r="F142" s="20"/>
       <c r="H142" s="5"/>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:29">
       <c r="A143" s="16"/>
       <c r="B143" s="14"/>
       <c r="C143" s="17"/>
@@ -5204,7 +5186,7 @@
       <c r="F143" s="20"/>
       <c r="H143" s="5"/>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:29">
       <c r="A144" s="16"/>
       <c r="B144" s="14"/>
       <c r="C144" s="17"/>
@@ -5213,7 +5195,7 @@
       <c r="F144" s="20"/>
       <c r="H144" s="5"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8">
       <c r="A145" s="16"/>
       <c r="B145" s="14"/>
       <c r="C145" s="17"/>
@@ -5222,7 +5204,7 @@
       <c r="F145" s="20"/>
       <c r="H145" s="5"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8">
       <c r="A146" s="16"/>
       <c r="B146" s="14"/>
       <c r="C146" s="17"/>
@@ -5231,7 +5213,7 @@
       <c r="F146" s="20"/>
       <c r="H146" s="5"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8">
       <c r="A147" s="16"/>
       <c r="B147" s="14"/>
       <c r="C147" s="17"/>
@@ -5240,7 +5222,7 @@
       <c r="F147" s="20"/>
       <c r="H147" s="5"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8">
       <c r="A148" s="16"/>
       <c r="B148" s="14"/>
       <c r="C148" s="17"/>
@@ -5249,7 +5231,7 @@
       <c r="F148" s="20"/>
       <c r="H148" s="5"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8">
       <c r="A149" s="16"/>
       <c r="B149" s="14"/>
       <c r="C149" s="17"/>
@@ -5258,7 +5240,7 @@
       <c r="F149" s="20"/>
       <c r="H149" s="5"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8">
       <c r="A150" s="16"/>
       <c r="B150" s="14"/>
       <c r="C150" s="17"/>
@@ -5267,7 +5249,7 @@
       <c r="F150" s="20"/>
       <c r="H150" s="5"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8">
       <c r="A151" s="16"/>
       <c r="B151" s="14"/>
       <c r="C151" s="17"/>
@@ -5276,7 +5258,7 @@
       <c r="F151" s="20"/>
       <c r="H151" s="5"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8">
       <c r="A152" s="16"/>
       <c r="B152" s="14"/>
       <c r="C152" s="17"/>
@@ -5285,7 +5267,7 @@
       <c r="F152" s="20"/>
       <c r="H152" s="5"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8">
       <c r="A153" s="16"/>
       <c r="B153" s="14"/>
       <c r="C153" s="17"/>
@@ -5294,7 +5276,7 @@
       <c r="F153" s="20"/>
       <c r="H153" s="5"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8">
       <c r="A154" s="16"/>
       <c r="B154" s="14"/>
       <c r="C154" s="17"/>
@@ -5303,7 +5285,7 @@
       <c r="F154" s="20"/>
       <c r="H154" s="5"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8">
       <c r="A155" s="16"/>
       <c r="B155" s="14"/>
       <c r="C155" s="17"/>
@@ -5312,7 +5294,7 @@
       <c r="F155" s="20"/>
       <c r="H155" s="5"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8">
       <c r="A156" s="16"/>
       <c r="B156" s="14"/>
       <c r="C156" s="17"/>
@@ -5321,7 +5303,7 @@
       <c r="F156" s="20"/>
       <c r="H156" s="5"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8">
       <c r="A157" s="16"/>
       <c r="B157" s="14"/>
       <c r="C157" s="17"/>
@@ -5330,7 +5312,7 @@
       <c r="F157" s="20"/>
       <c r="H157" s="5"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8">
       <c r="A158" s="16"/>
       <c r="B158" s="14"/>
       <c r="C158" s="17"/>
@@ -5339,7 +5321,7 @@
       <c r="F158" s="20"/>
       <c r="H158" s="5"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8">
       <c r="A159" s="16"/>
       <c r="B159" s="14"/>
       <c r="C159" s="17"/>
@@ -5348,8 +5330,8 @@
       <c r="F159" s="20"/>
       <c r="H159" s="5"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A160" s="5"/>
+    <row r="160" spans="1:8">
+      <c r="A160" s="16"/>
       <c r="B160" s="14"/>
       <c r="C160" s="17"/>
       <c r="D160" s="20"/>
@@ -5357,125 +5339,116 @@
       <c r="F160" s="20"/>
       <c r="H160" s="5"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8">
       <c r="A161" s="5"/>
+      <c r="B161" s="14"/>
+      <c r="C161" s="17"/>
+      <c r="D161" s="20"/>
+      <c r="E161" s="20"/>
+      <c r="F161" s="20"/>
       <c r="H161" s="5"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8">
       <c r="A162" s="5"/>
       <c r="H162" s="5"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8">
       <c r="A163" s="5"/>
       <c r="H163" s="5"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8">
       <c r="A164" s="5"/>
       <c r="H164" s="5"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8">
       <c r="A165" s="5"/>
       <c r="H165" s="5"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8">
       <c r="A166" s="5"/>
       <c r="H166" s="5"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8">
       <c r="A167" s="5"/>
       <c r="H167" s="5"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8">
       <c r="A168" s="5"/>
       <c r="H168" s="5"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8">
       <c r="A169" s="5"/>
       <c r="H169" s="5"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8">
       <c r="A170" s="5"/>
       <c r="H170" s="5"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8">
       <c r="A171" s="5"/>
       <c r="H171" s="5"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8">
       <c r="A172" s="5"/>
       <c r="H172" s="5"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8">
       <c r="A173" s="5"/>
       <c r="H173" s="5"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8">
       <c r="A174" s="5"/>
       <c r="H174" s="5"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8">
       <c r="A175" s="5"/>
       <c r="H175" s="5"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8">
       <c r="A176" s="5"/>
       <c r="H176" s="5"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8">
       <c r="A177" s="5"/>
       <c r="H177" s="5"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8">
       <c r="A178" s="5"/>
       <c r="H178" s="5"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8">
       <c r="A179" s="5"/>
       <c r="H179" s="5"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8">
       <c r="A180" s="5"/>
       <c r="H180" s="5"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8">
       <c r="A181" s="5"/>
       <c r="H181" s="5"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8">
+      <c r="A182" s="5"/>
       <c r="H182" s="5"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8">
       <c r="H183" s="5"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8">
       <c r="H184" s="5"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8">
       <c r="H185" s="5"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8">
       <c r="H186" s="5"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8">
       <c r="H187" s="5"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H188" s="5"/>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H189" s="5"/>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H190" s="5"/>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H191" s="5"/>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H192" s="5"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:F43">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F43">
     <sortCondition ref="A2:A43"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5485,14 +5458,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F176"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="28" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" style="1" customWidth="1"/>
@@ -5502,7 +5475,7 @@
     <col min="6" max="6" width="13.109375" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -5522,7 +5495,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="23" t="s">
         <v>82</v>
       </c>
@@ -5536,7 +5509,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="23" t="s">
         <v>82</v>
       </c>
@@ -5550,7 +5523,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="23" t="s">
         <v>82</v>
       </c>
@@ -5564,7 +5537,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="23" t="s">
         <v>82</v>
       </c>
@@ -5578,7 +5551,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="23" t="s">
         <v>82</v>
       </c>
@@ -5592,7 +5565,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="23" t="s">
         <v>82</v>
       </c>
@@ -5606,7 +5579,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="23" t="s">
         <v>82</v>
       </c>
@@ -5620,7 +5593,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="23" t="s">
         <v>83</v>
       </c>
@@ -5634,7 +5607,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="23" t="s">
         <v>83</v>
       </c>
@@ -5648,7 +5621,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="23" t="s">
         <v>83</v>
       </c>
@@ -5662,7 +5635,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="23" t="s">
         <v>83</v>
       </c>
@@ -5676,7 +5649,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="23" t="s">
         <v>83</v>
       </c>
@@ -5690,7 +5663,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="23" t="s">
         <v>83</v>
       </c>
@@ -5704,7 +5677,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="23" t="s">
         <v>83</v>
       </c>
@@ -5718,7 +5691,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="23" t="s">
         <v>83</v>
       </c>
@@ -5732,7 +5705,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="23" t="s">
         <v>83</v>
       </c>
@@ -5746,7 +5719,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="23" t="s">
         <v>83</v>
       </c>
@@ -5760,7 +5733,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="23" t="s">
         <v>83</v>
       </c>
@@ -5774,7 +5747,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="23" t="s">
         <v>83</v>
       </c>
@@ -5788,7 +5761,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="23" t="s">
         <v>83</v>
       </c>
@@ -5802,7 +5775,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="23" t="s">
         <v>84</v>
       </c>
@@ -5816,7 +5789,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="23" t="s">
         <v>84</v>
       </c>
@@ -5830,7 +5803,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="23" t="s">
         <v>84</v>
       </c>
@@ -5844,55 +5817,91 @@
       <c r="E24" s="3"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
+      <c r="A25" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -5900,7 +5909,7 @@
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="13"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -5908,7 +5917,7 @@
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="13"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -5916,7 +5925,7 @@
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="13"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -5924,7 +5933,7 @@
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="13"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -5932,7 +5941,7 @@
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="13"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -5940,7 +5949,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="13"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -5948,7 +5957,7 @@
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="13"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -5956,7 +5965,7 @@
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="13"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -5964,7 +5973,7 @@
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="13"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -5972,7 +5981,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="13"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -5980,7 +5989,7 @@
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="13"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -5988,7 +5997,7 @@
       <c r="E42" s="14"/>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="13"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -5996,7 +6005,7 @@
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="13"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -6004,7 +6013,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="13"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -6012,7 +6021,7 @@
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="13"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -6020,7 +6029,7 @@
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="13"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -6028,7 +6037,7 @@
       <c r="E47" s="14"/>
       <c r="F47" s="12"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="13"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -6036,7 +6045,7 @@
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="13"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -6044,7 +6053,7 @@
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="13"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -6052,7 +6061,7 @@
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="13"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -6060,7 +6069,7 @@
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="13"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -6068,7 +6077,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="13"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -6076,7 +6085,7 @@
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="13"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -6084,7 +6093,7 @@
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="13"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -6092,7 +6101,7 @@
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="15"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -6100,7 +6109,7 @@
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="13"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -6108,7 +6117,7 @@
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="13"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
@@ -6116,418 +6125,418 @@
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="5"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="5"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="5"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="5"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="5"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="5"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="5"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="5"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="5"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="5"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="5"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="5"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="5"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="5"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="5"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="5"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="5"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="5"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="5"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="5"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="5"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="5"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="5"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="5"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="5"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="5"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="5"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" s="5"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" s="5"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="5"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="5"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" s="5"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" s="5"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" s="5"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" s="5"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" s="5"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" s="5"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="5"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" s="5"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" s="5"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" s="5"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" s="5"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" s="5"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" s="5"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" s="5"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" s="5"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105" s="5"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" s="5"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" s="5"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108" s="5"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109" s="5"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" s="5"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111" s="5"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3">
       <c r="A112" s="5"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113" s="5"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3">
       <c r="A114" s="5"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3">
       <c r="A115" s="5"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3">
       <c r="A116" s="5"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" s="5"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" s="5"/>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" s="5"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" s="5"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" s="5"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3">
       <c r="A122" s="5"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3">
       <c r="A123" s="5"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" s="5"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" s="5"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" s="5"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" s="5"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3">
       <c r="A128" s="5"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1">
       <c r="A129" s="5"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1">
       <c r="A130" s="5"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1">
       <c r="A131" s="5"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1">
       <c r="A132" s="5"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1">
       <c r="A133" s="5"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1">
       <c r="A134" s="5"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1">
       <c r="A135" s="5"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1">
       <c r="A136" s="5"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1">
       <c r="A137" s="5"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1">
       <c r="A138" s="5"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1">
       <c r="A139" s="5"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1">
       <c r="A140" s="5"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1">
       <c r="A141" s="5"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1">
       <c r="A142" s="5"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1">
       <c r="A143" s="5"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1">
       <c r="A144" s="5"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1">
       <c r="A145" s="5"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1">
       <c r="A146" s="5"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1">
       <c r="A147" s="5"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1">
       <c r="A148" s="5"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1">
       <c r="A149" s="5"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1">
       <c r="A150" s="5"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1">
       <c r="A151" s="5"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1">
       <c r="A152" s="5"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1">
       <c r="A153" s="5"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1">
       <c r="A154" s="5"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1">
       <c r="A155" s="5"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1">
       <c r="A156" s="5"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1">
       <c r="A157" s="5"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1">
       <c r="A158" s="5"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1">
       <c r="A159" s="5"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1">
       <c r="A160" s="5"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1">
       <c r="A161" s="5"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1">
       <c r="A162" s="5"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1">
       <c r="A163" s="5"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1">
       <c r="A164" s="5"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1">
       <c r="A165" s="5"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1">
       <c r="A166" s="5"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1">
       <c r="A167" s="5"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1">
       <c r="A168" s="5"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1">
       <c r="A169" s="5"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1">
       <c r="A170" s="5"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1">
       <c r="A171" s="5"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1">
       <c r="A172" s="5"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1">
       <c r="A173" s="5"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1">
       <c r="A174" s="5"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1">
       <c r="A175" s="5"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1">
       <c r="A176" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update GBase System Manage Blog
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2556" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="4332" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="131">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -412,10 +412,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20220412</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ubuntu系统命令（持续更新）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -461,6 +457,18 @@
   </si>
   <si>
     <t>20220707</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220711</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220712</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220713</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -950,7 +958,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -984,7 +992,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>93</v>
@@ -1006,7 +1014,7 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>93</v>
@@ -1355,7 +1363,7 @@
         <v>35</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="26"/>
@@ -1431,7 +1439,7 @@
         <v>63</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="26"/>
@@ -1611,7 +1619,7 @@
         <v>75</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="26"/>
@@ -1701,7 +1709,7 @@
         <v>106</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="25"/>
@@ -1791,12 +1799,12 @@
         <v>111</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="25"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="12"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="18"/>
       <c r="I19" s="23" t="s">
         <v>79</v>
@@ -1892,10 +1900,10 @@
         <v>79</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="12"/>
@@ -1926,7 +1934,7 @@
         <v>113</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" s="1"/>
       <c r="F22" s="10"/>
@@ -1938,7 +1946,7 @@
         <v>97</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="14"/>
@@ -1969,7 +1977,7 @@
         <v>112</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="D23" s="1"/>
       <c r="F23" s="10"/>
@@ -1982,10 +1990,10 @@
         <v>13</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L23" s="9"/>
-      <c r="M23" s="12"/>
+      <c r="M23" s="26"/>
       <c r="N23" s="10"/>
       <c r="O23" s="12"/>
       <c r="P23" s="1"/>
@@ -2010,14 +2018,15 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="12"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="18"/>
       <c r="I24" s="22" t="s">
         <v>2</v>
@@ -2026,7 +2035,7 @@
         <v>14</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="26"/>
@@ -2071,7 +2080,7 @@
         <v>15</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="26"/>
@@ -2113,15 +2122,15 @@
         <v>2</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="12"/>
+        <v>130</v>
+      </c>
+      <c r="L26" s="9"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="11"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -5828,7 +5837,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
New blog: the record of C compile error
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7884" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="8772" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="135">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -477,6 +477,13 @@
   </si>
   <si>
     <t>20220811</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C编译报错原因汇总</t>
+  </si>
+  <si>
+    <t>20220818</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -966,7 +973,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1804,15 +1811,15 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
+        <v>134</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="18"/>
       <c r="I19" s="23" t="s">
         <v>79</v>
@@ -1849,10 +1856,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="26"/>
@@ -1894,14 +1901,14 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="26"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="18"/>
       <c r="I21" s="23" t="s">
@@ -1939,13 +1946,15 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="F22" s="10"/>
+        <v>76</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="18"/>
       <c r="I22" s="23" t="s">
         <v>79</v>
@@ -1982,14 +1991,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D23" s="1"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="12"/>
       <c r="H23" s="18"/>
       <c r="I23" s="22" t="s">
         <v>2</v>
@@ -2026,15 +2034,14 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="26"/>
+        <v>128</v>
+      </c>
+      <c r="D24" s="1"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="11"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="18"/>
       <c r="I24" s="22" t="s">
         <v>2</v>
@@ -2071,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="26"/>
@@ -2112,14 +2119,14 @@
       <c r="AE25" s="1"/>
     </row>
     <row r="26" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>101</v>
+      <c r="A26" s="22" t="s">
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="26"/>
@@ -2160,16 +2167,16 @@
       <c r="A27" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="B27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="26"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="12"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="18"/>
       <c r="I27" s="13"/>
       <c r="J27" s="14"/>
@@ -2199,14 +2206,16 @@
       <c r="A28" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="1"/>
+      <c r="B28" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="10"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="18"/>
       <c r="I28" s="13"/>
       <c r="J28" s="14"/>
@@ -2236,15 +2245,13 @@
         <v>101</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="26"/>
+        <v>109</v>
+      </c>
+      <c r="D29" s="1"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="11"/>
       <c r="H29" s="18"/>
       <c r="I29" s="13"/>
       <c r="J29" s="14"/>
@@ -2270,6 +2277,19 @@
       <c r="AE29" s="1"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="11"/>
       <c r="H30" s="18"/>
       <c r="I30" s="13"/>
       <c r="J30" s="14"/>
@@ -2296,13 +2316,6 @@
       <c r="AE30" s="1"/>
     </row>
     <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
       <c r="H31" s="18"/>
       <c r="I31" s="13"/>
       <c r="J31" s="14"/>
@@ -2328,6 +2341,13 @@
       <c r="AE31" s="1"/>
     </row>
     <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
       <c r="H32" s="18"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -2411,13 +2431,6 @@
       <c r="AE35" s="1"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
       <c r="H36" s="18"/>
       <c r="I36" s="13"/>
       <c r="J36" s="14"/>
@@ -2911,7 +2924,7 @@
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="18"/>
       <c r="I51" s="13"/>
@@ -2944,7 +2957,7 @@
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
-      <c r="F52" s="12"/>
+      <c r="F52" s="14"/>
       <c r="G52" s="12"/>
       <c r="H52" s="18"/>
       <c r="I52" s="13"/>
@@ -3076,7 +3089,7 @@
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
+      <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="18"/>
       <c r="I56" s="13"/>
@@ -3109,7 +3122,7 @@
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
-      <c r="F57" s="12"/>
+      <c r="F57" s="14"/>
       <c r="G57" s="12"/>
       <c r="H57" s="18"/>
       <c r="I57" s="13"/>
@@ -3335,7 +3348,7 @@
       <c r="AE63" s="1"/>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
+      <c r="A64" s="13"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
@@ -3368,7 +3381,7 @@
       <c r="AE64" s="1"/>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+      <c r="A65" s="15"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
@@ -3434,7 +3447,7 @@
       <c r="AE66" s="1"/>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
+      <c r="A67" s="13"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
@@ -3471,9 +3484,9 @@
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="20"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
       <c r="H68" s="18"/>
       <c r="I68" s="13"/>
       <c r="J68" s="14"/>
@@ -5213,8 +5226,8 @@
     <row r="128" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A128" s="16"/>
       <c r="B128" s="14"/>
-      <c r="C128" s="17"/>
-      <c r="D128" s="17"/>
+      <c r="C128" s="14"/>
+      <c r="D128" s="14"/>
       <c r="E128" s="20"/>
       <c r="F128" s="20"/>
       <c r="G128" s="20"/>
@@ -5716,7 +5729,7 @@
       <c r="L162" s="17"/>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A163" s="5"/>
+      <c r="A163" s="16"/>
       <c r="B163" s="14"/>
       <c r="C163" s="17"/>
       <c r="D163" s="17"/>
@@ -5727,6 +5740,12 @@
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
+      <c r="B164" s="14"/>
+      <c r="C164" s="17"/>
+      <c r="D164" s="17"/>
+      <c r="E164" s="20"/>
+      <c r="F164" s="20"/>
+      <c r="G164" s="20"/>
       <c r="I164" s="5"/>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.25">
@@ -5810,6 +5829,7 @@
       <c r="I184" s="5"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185" s="5"/>
       <c r="I185" s="5"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -5823,7 +5843,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C28" numberStoredAsText="1"/>
+    <ignoredError sqref="C29" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New blog: serach optimize
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8772" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="9660" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="137">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -484,6 +484,14 @@
   </si>
   <si>
     <t>20220818</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索优化集锦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220819</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -972,8 +980,8 @@
   <dimension ref="A1:AE186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1766,15 +1774,15 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="26"/>
+        <v>136</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="25"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="11"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="18"/>
       <c r="I18" s="23" t="s">
         <v>79</v>
@@ -1808,18 +1816,18 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="24"/>
+        <v>92</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="18"/>
       <c r="I19" s="23" t="s">
         <v>79</v>
@@ -1856,15 +1864,15 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
+        <v>134</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="18"/>
       <c r="I20" s="23" t="s">
         <v>79</v>
@@ -1901,10 +1909,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="26"/>
@@ -1946,14 +1954,14 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="26"/>
-      <c r="F22" s="3"/>
+      <c r="F22" s="10"/>
       <c r="G22" s="11"/>
       <c r="H22" s="18"/>
       <c r="I22" s="23" t="s">
@@ -1991,13 +1999,15 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="F23" s="10"/>
+        <v>76</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="11"/>
       <c r="H23" s="18"/>
       <c r="I23" s="22" t="s">
         <v>2</v>
@@ -2034,14 +2044,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D24" s="1"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="12"/>
       <c r="H24" s="18"/>
       <c r="I24" s="22" t="s">
         <v>2</v>
@@ -2078,15 +2087,14 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="26"/>
+        <v>128</v>
+      </c>
+      <c r="D25" s="1"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="12"/>
       <c r="H25" s="18"/>
       <c r="I25" s="22" t="s">
         <v>2</v>
@@ -2123,10 +2131,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="26"/>
@@ -2164,14 +2172,14 @@
       <c r="AE26" s="1"/>
     </row>
     <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>101</v>
+      <c r="A27" s="22" t="s">
+        <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="26"/>
@@ -2206,16 +2214,16 @@
       <c r="A28" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="B28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="26"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="12"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="18"/>
       <c r="I28" s="13"/>
       <c r="J28" s="14"/>
@@ -2244,14 +2252,16 @@
       <c r="A29" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="1"/>
+      <c r="B29" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="10"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="18"/>
       <c r="I29" s="13"/>
       <c r="J29" s="14"/>
@@ -2281,15 +2291,13 @@
         <v>101</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="26"/>
+        <v>109</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
       <c r="H30" s="18"/>
       <c r="I30" s="13"/>
       <c r="J30" s="14"/>
@@ -2316,6 +2324,19 @@
       <c r="AE30" s="1"/>
     </row>
     <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
       <c r="H31" s="18"/>
       <c r="I31" s="13"/>
       <c r="J31" s="14"/>
@@ -2341,13 +2362,6 @@
       <c r="AE31" s="1"/>
     </row>
     <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
       <c r="H32" s="18"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -2367,6 +2381,13 @@
       <c r="AE32" s="1"/>
     </row>
     <row r="33" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
       <c r="H33" s="18"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
@@ -2457,13 +2478,6 @@
       <c r="AE36" s="1"/>
     </row>
     <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
       <c r="H37" s="18"/>
       <c r="I37" s="15"/>
       <c r="J37" s="14"/>
@@ -2957,7 +2971,7 @@
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="F52" s="12"/>
       <c r="G52" s="12"/>
       <c r="H52" s="18"/>
       <c r="I52" s="13"/>
@@ -2990,7 +3004,7 @@
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
-      <c r="F53" s="12"/>
+      <c r="F53" s="14"/>
       <c r="G53" s="12"/>
       <c r="H53" s="18"/>
       <c r="I53" s="13"/>
@@ -3122,7 +3136,7 @@
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
+      <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="18"/>
       <c r="I57" s="13"/>
@@ -3155,7 +3169,7 @@
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
-      <c r="F58" s="12"/>
+      <c r="F58" s="14"/>
       <c r="G58" s="12"/>
       <c r="H58" s="18"/>
       <c r="I58" s="13"/>
@@ -3381,7 +3395,7 @@
       <c r="AE64" s="1"/>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
+      <c r="A65" s="13"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
@@ -3414,7 +3428,7 @@
       <c r="AE65" s="1"/>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
@@ -3480,7 +3494,7 @@
       <c r="AE67" s="1"/>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A68" s="16"/>
+      <c r="A68" s="13"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
@@ -3517,9 +3531,9 @@
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="20"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
       <c r="H69" s="18"/>
       <c r="I69" s="5"/>
       <c r="K69" s="1"/>
@@ -5255,8 +5269,8 @@
     <row r="129" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A129" s="16"/>
       <c r="B129" s="14"/>
-      <c r="C129" s="17"/>
-      <c r="D129" s="17"/>
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
       <c r="E129" s="20"/>
       <c r="F129" s="20"/>
       <c r="G129" s="20"/>
@@ -5739,7 +5753,7 @@
       <c r="I163" s="5"/>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A164" s="5"/>
+      <c r="A164" s="16"/>
       <c r="B164" s="14"/>
       <c r="C164" s="17"/>
       <c r="D164" s="17"/>
@@ -5750,6 +5764,12 @@
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
+      <c r="B165" s="14"/>
+      <c r="C165" s="17"/>
+      <c r="D165" s="17"/>
+      <c r="E165" s="20"/>
+      <c r="F165" s="20"/>
+      <c r="G165" s="20"/>
       <c r="I165" s="5"/>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.25">
@@ -5833,6 +5853,7 @@
       <c r="I185" s="5"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" s="5"/>
       <c r="I186" s="5"/>
     </row>
   </sheetData>
@@ -5843,7 +5864,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C29" numberStoredAsText="1"/>
+    <ignoredError sqref="C30" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update on Aug 28
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="10548" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="138">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -449,10 +449,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20220427</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20220707</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -492,6 +488,14 @@
   </si>
   <si>
     <t>20220819</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220828</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -541,7 +545,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,12 +578,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -597,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -664,13 +662,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -980,8 +972,8 @@
   <dimension ref="A1:AE186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1073,10 +1065,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="26"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="10"/>
       <c r="G2" s="11"/>
       <c r="H2" s="18"/>
@@ -1090,7 +1082,7 @@
         <v>78</v>
       </c>
       <c r="L2" s="9"/>
-      <c r="M2" s="26"/>
+      <c r="M2" s="24"/>
       <c r="N2" s="14"/>
       <c r="O2" s="11"/>
     </row>
@@ -1105,7 +1097,7 @@
         <v>90</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="26"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="10"/>
       <c r="G3" s="11"/>
       <c r="H3" s="18"/>
@@ -1119,7 +1111,7 @@
         <v>76</v>
       </c>
       <c r="L3" s="9"/>
-      <c r="M3" s="26"/>
+      <c r="M3" s="24"/>
       <c r="N3" s="3"/>
       <c r="O3" s="11"/>
       <c r="P3" s="1"/>
@@ -1150,7 +1142,7 @@
         <v>76</v>
       </c>
       <c r="D4" s="9"/>
-      <c r="E4" s="26"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="10"/>
       <c r="G4" s="11"/>
       <c r="H4" s="18"/>
@@ -1164,7 +1156,7 @@
         <v>107</v>
       </c>
       <c r="L4" s="9"/>
-      <c r="M4" s="26"/>
+      <c r="M4" s="24"/>
       <c r="N4" s="10"/>
       <c r="O4" s="11"/>
       <c r="P4" s="1"/>
@@ -1209,7 +1201,7 @@
         <v>78</v>
       </c>
       <c r="L5" s="9"/>
-      <c r="M5" s="26"/>
+      <c r="M5" s="24"/>
       <c r="N5" s="14"/>
       <c r="O5" s="11"/>
       <c r="P5" s="1"/>
@@ -1240,7 +1232,7 @@
         <v>76</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="26"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="H6" s="18"/>
@@ -1254,7 +1246,7 @@
         <v>78</v>
       </c>
       <c r="L6" s="9"/>
-      <c r="M6" s="26"/>
+      <c r="M6" s="24"/>
       <c r="N6" s="14"/>
       <c r="O6" s="11"/>
       <c r="P6" s="1"/>
@@ -1285,7 +1277,7 @@
         <v>108</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="26"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="18"/>
@@ -1299,7 +1291,7 @@
         <v>78</v>
       </c>
       <c r="L7" s="9"/>
-      <c r="M7" s="26"/>
+      <c r="M7" s="24"/>
       <c r="N7" s="10"/>
       <c r="O7" s="11"/>
       <c r="P7" s="1"/>
@@ -1330,7 +1322,7 @@
         <v>94</v>
       </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="26"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
       <c r="H8" s="18"/>
@@ -1344,7 +1336,7 @@
         <v>76</v>
       </c>
       <c r="L8" s="9"/>
-      <c r="M8" s="26"/>
+      <c r="M8" s="24"/>
       <c r="N8" s="10"/>
       <c r="O8" s="11"/>
       <c r="P8" s="1"/>
@@ -1389,7 +1381,7 @@
         <v>114</v>
       </c>
       <c r="L9" s="9"/>
-      <c r="M9" s="26"/>
+      <c r="M9" s="24"/>
       <c r="N9" s="10"/>
       <c r="O9" s="11"/>
       <c r="P9" s="1"/>
@@ -1434,7 +1426,7 @@
         <v>76</v>
       </c>
       <c r="L10" s="9"/>
-      <c r="M10" s="26"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="10"/>
       <c r="O10" s="11"/>
       <c r="P10" s="1"/>
@@ -1465,7 +1457,7 @@
         <v>118</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="26"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="10"/>
       <c r="G11" s="12"/>
       <c r="H11" s="18"/>
@@ -1479,7 +1471,7 @@
         <v>76</v>
       </c>
       <c r="L11" s="9"/>
-      <c r="M11" s="26"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="3"/>
       <c r="O11" s="11"/>
       <c r="P11" s="1"/>
@@ -1524,7 +1516,7 @@
         <v>76</v>
       </c>
       <c r="L12" s="9"/>
-      <c r="M12" s="26"/>
+      <c r="M12" s="24"/>
       <c r="N12" s="10"/>
       <c r="O12" s="11"/>
       <c r="P12" s="1"/>
@@ -1569,7 +1561,7 @@
         <v>89</v>
       </c>
       <c r="L13" s="9"/>
-      <c r="M13" s="26"/>
+      <c r="M13" s="24"/>
       <c r="N13" s="10"/>
       <c r="O13" s="11"/>
       <c r="P13" s="1"/>
@@ -1614,7 +1606,7 @@
         <v>76</v>
       </c>
       <c r="L14" s="9"/>
-      <c r="M14" s="26"/>
+      <c r="M14" s="24"/>
       <c r="N14" s="3"/>
       <c r="O14" s="11"/>
       <c r="P14" s="1"/>
@@ -1642,10 +1634,10 @@
         <v>75</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="26"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
       <c r="H15" s="18"/>
@@ -1659,7 +1651,7 @@
         <v>76</v>
       </c>
       <c r="L15" s="9"/>
-      <c r="M15" s="26"/>
+      <c r="M15" s="24"/>
       <c r="N15" s="3"/>
       <c r="O15" s="11"/>
       <c r="P15" s="1"/>
@@ -1690,7 +1682,7 @@
         <v>76</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="26"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
       <c r="H16" s="18"/>
@@ -1704,7 +1696,7 @@
         <v>76</v>
       </c>
       <c r="L16" s="9"/>
-      <c r="M16" s="26"/>
+      <c r="M16" s="24"/>
       <c r="N16" s="10"/>
       <c r="O16" s="11"/>
       <c r="P16" s="1"/>
@@ -1726,7 +1718,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>106</v>
@@ -1734,10 +1726,10 @@
       <c r="C17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="25"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="24"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="18"/>
       <c r="I17" s="23" t="s">
         <v>79</v>
@@ -1749,7 +1741,7 @@
         <v>103</v>
       </c>
       <c r="L17" s="9"/>
-      <c r="M17" s="26"/>
+      <c r="M17" s="24"/>
       <c r="N17" s="10"/>
       <c r="O17" s="11"/>
       <c r="P17" s="1"/>
@@ -1771,18 +1763,18 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="25"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="24"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="18"/>
       <c r="I18" s="23" t="s">
         <v>79</v>
@@ -1794,7 +1786,7 @@
         <v>87</v>
       </c>
       <c r="L18" s="9"/>
-      <c r="M18" s="26"/>
+      <c r="M18" s="24"/>
       <c r="N18" s="10"/>
       <c r="O18" s="11"/>
       <c r="P18" s="1"/>
@@ -1825,7 +1817,7 @@
         <v>92</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="26"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
       <c r="H19" s="18"/>
@@ -1839,7 +1831,7 @@
         <v>89</v>
       </c>
       <c r="L19" s="9"/>
-      <c r="M19" s="26"/>
+      <c r="M19" s="24"/>
       <c r="N19" s="3"/>
       <c r="O19" s="11"/>
       <c r="P19" s="1"/>
@@ -1864,15 +1856,15 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="24"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="18"/>
       <c r="I20" s="23" t="s">
         <v>79</v>
@@ -1884,7 +1876,7 @@
         <v>87</v>
       </c>
       <c r="L20" s="9"/>
-      <c r="M20" s="26"/>
+      <c r="M20" s="24"/>
       <c r="N20" s="10"/>
       <c r="O20" s="11"/>
       <c r="P20" s="1"/>
@@ -1912,10 +1904,10 @@
         <v>111</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="26"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="18"/>
@@ -1926,7 +1918,7 @@
         <v>115</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="12"/>
@@ -1960,7 +1952,7 @@
         <v>76</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="26"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="10"/>
       <c r="G22" s="11"/>
       <c r="H22" s="18"/>
@@ -2005,7 +1997,7 @@
         <v>76</v>
       </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="26"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="3"/>
       <c r="G23" s="11"/>
       <c r="H23" s="18"/>
@@ -2016,7 +2008,7 @@
         <v>13</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="12"/>
@@ -2062,7 +2054,7 @@
         <v>119</v>
       </c>
       <c r="L24" s="9"/>
-      <c r="M24" s="26"/>
+      <c r="M24" s="24"/>
       <c r="N24" s="10"/>
       <c r="O24" s="11"/>
       <c r="P24" s="1"/>
@@ -2090,7 +2082,7 @@
         <v>112</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25" s="1"/>
       <c r="F25" s="10"/>
@@ -2106,7 +2098,7 @@
         <v>120</v>
       </c>
       <c r="L25" s="9"/>
-      <c r="M25" s="26"/>
+      <c r="M25" s="24"/>
       <c r="N25" s="10"/>
       <c r="O25" s="11"/>
       <c r="P25" s="1"/>
@@ -2134,10 +2126,10 @@
         <v>123</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D26" s="9"/>
-      <c r="E26" s="26"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="10"/>
       <c r="G26" s="11"/>
       <c r="H26" s="18"/>
@@ -2148,7 +2140,7 @@
         <v>121</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="12"/>
@@ -2182,7 +2174,7 @@
         <v>99</v>
       </c>
       <c r="D27" s="9"/>
-      <c r="E27" s="26"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="10"/>
       <c r="G27" s="11"/>
       <c r="H27" s="18"/>
@@ -2221,7 +2213,7 @@
         <v>102</v>
       </c>
       <c r="D28" s="9"/>
-      <c r="E28" s="26"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="10"/>
       <c r="G28" s="11"/>
       <c r="H28" s="18"/>
@@ -2328,13 +2320,13 @@
         <v>101</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="D31" s="9"/>
-      <c r="E31" s="26"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="10"/>
       <c r="G31" s="11"/>
       <c r="H31" s="18"/>
@@ -5922,7 +5914,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="26"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="3"/>
       <c r="G2" s="11"/>
     </row>
@@ -5937,7 +5929,7 @@
         <v>68</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="26"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="3"/>
       <c r="G3" s="11"/>
     </row>
@@ -5952,7 +5944,7 @@
         <v>68</v>
       </c>
       <c r="D4" s="9"/>
-      <c r="E4" s="26"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="3"/>
       <c r="G4" s="11"/>
     </row>
@@ -5967,7 +5959,7 @@
         <v>68</v>
       </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="26"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="3"/>
       <c r="G5" s="11"/>
     </row>
@@ -5982,7 +5974,7 @@
         <v>68</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="26"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="3"/>
       <c r="G6" s="11"/>
     </row>
@@ -5997,7 +5989,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="26"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="3"/>
       <c r="G7" s="11"/>
     </row>
@@ -6012,7 +6004,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="26"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="3"/>
       <c r="G8" s="11"/>
     </row>
@@ -6027,7 +6019,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="26"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="3"/>
       <c r="G9" s="11"/>
     </row>
@@ -6042,7 +6034,7 @@
         <v>69</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="26"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="3"/>
       <c r="G10" s="11"/>
     </row>
@@ -6057,7 +6049,7 @@
         <v>68</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="26"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="3"/>
       <c r="G11" s="11"/>
     </row>
@@ -6072,7 +6064,7 @@
         <v>69</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="26"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="3"/>
       <c r="G12" s="11"/>
     </row>
@@ -6087,7 +6079,7 @@
         <v>69</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="26"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="3"/>
       <c r="G13" s="11"/>
     </row>
@@ -6102,7 +6094,7 @@
         <v>68</v>
       </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="26"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="3"/>
       <c r="G14" s="11"/>
     </row>
@@ -6117,7 +6109,7 @@
         <v>69</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="26"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="3"/>
       <c r="G15" s="11"/>
     </row>
@@ -6132,7 +6124,7 @@
         <v>69</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="26"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="3"/>
       <c r="G16" s="11"/>
     </row>
@@ -6147,7 +6139,7 @@
         <v>69</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="26"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="3"/>
       <c r="G17" s="11"/>
     </row>
@@ -6162,7 +6154,7 @@
         <v>69</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="26"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="3"/>
       <c r="G18" s="11"/>
     </row>
@@ -6177,7 +6169,7 @@
         <v>69</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="26"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="3"/>
       <c r="G19" s="11"/>
     </row>
@@ -6192,7 +6184,7 @@
         <v>68</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="26"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="3"/>
       <c r="G20" s="11"/>
     </row>
@@ -6207,7 +6199,7 @@
         <v>68</v>
       </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="26"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="3"/>
       <c r="G21" s="11"/>
     </row>
@@ -6222,7 +6214,7 @@
         <v>76</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="26"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="3"/>
       <c r="G22" s="11"/>
     </row>
@@ -6237,7 +6229,7 @@
         <v>90</v>
       </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="26"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="3"/>
       <c r="G23" s="11"/>
     </row>
@@ -6252,7 +6244,7 @@
         <v>90</v>
       </c>
       <c r="D24" s="9"/>
-      <c r="E24" s="26"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="3"/>
       <c r="G24" s="11"/>
     </row>
@@ -6267,7 +6259,7 @@
         <v>78</v>
       </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="26"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="10"/>
       <c r="G25" s="11"/>
     </row>
@@ -6282,7 +6274,7 @@
         <v>78</v>
       </c>
       <c r="D26" s="9"/>
-      <c r="E26" s="26"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="10"/>
       <c r="G26" s="11"/>
     </row>
@@ -6297,7 +6289,7 @@
         <v>85</v>
       </c>
       <c r="D27" s="9"/>
-      <c r="E27" s="26"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="10"/>
       <c r="G27" s="11"/>
     </row>
@@ -6312,7 +6304,7 @@
         <v>76</v>
       </c>
       <c r="D28" s="9"/>
-      <c r="E28" s="26"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="3"/>
       <c r="G28" s="11"/>
     </row>
@@ -6327,7 +6319,7 @@
         <v>78</v>
       </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="26"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
     </row>
@@ -6342,7 +6334,7 @@
         <v>76</v>
       </c>
       <c r="D30" s="9"/>
-      <c r="E30" s="26"/>
+      <c r="E30" s="24"/>
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
     </row>

</xml_diff>

<commit_message>
Update on 2 Sept
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11436" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="12324" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="139">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -497,6 +497,10 @@
   </si>
   <si>
     <t>数据库系统存储结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20220902</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -974,7 +978,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1518,7 @@
         <v>65</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>75</v>
+        <v>138</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="24"/>
@@ -1922,7 +1926,7 @@
         <v>123</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="M21" s="12"/>
+      <c r="M21" s="24"/>
       <c r="N21" s="10"/>
       <c r="O21" s="11"/>
       <c r="P21" s="1"/>
@@ -2040,10 +2044,12 @@
         <v>111</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="18"/>
       <c r="I24" s="22" t="s">
         <v>2</v>
@@ -5867,7 +5873,7 @@
   <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
GNU & VS Code update
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="9660" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="152">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,9 +95,6 @@
     <t>Windows下cmd使用技巧（持续更新）</t>
   </si>
   <si>
-    <t>编译原理极简笔记（附C/C++编译过程及GNU使用笔记）</t>
-  </si>
-  <si>
     <t>ACM环境下对拍程序的写法</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>Git自学笔记（本地操作）</t>
   </si>
   <si>
-    <t>VS Code 使用技巧及Python/C++（ACM竞赛）环境配置</t>
-  </si>
-  <si>
     <t>Docker入门</t>
   </si>
   <si>
@@ -510,10 +504,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20220921</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20220920</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -540,6 +530,29 @@
   <si>
     <t>TODO：</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL约束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编译原理及GNU使用笔记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>填其他工时表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20221011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20221011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VS Code使用技巧及开发环境配置</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1031,8 @@
   <dimension ref="A1:AE180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1053,16 +1066,16 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H1" s="18"/>
       <c r="I1" s="5" t="s">
@@ -1075,16 +1088,16 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1111,7 +1124,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="24"/>
@@ -1119,13 +1132,13 @@
       <c r="G2" s="11"/>
       <c r="H2" s="18"/>
       <c r="I2" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L2" s="9"/>
       <c r="M2" s="24"/>
@@ -1140,7 +1153,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="24"/>
@@ -1148,13 +1161,13 @@
       <c r="G3" s="11"/>
       <c r="H3" s="18"/>
       <c r="I3" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="24"/>
@@ -1182,10 +1195,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="24"/>
@@ -1193,17 +1206,17 @@
       <c r="G4" s="11"/>
       <c r="H4" s="18"/>
       <c r="I4" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>23</v>
+        <v>147</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="24"/>
-      <c r="N4" s="3"/>
+      <c r="N4" s="10"/>
       <c r="O4" s="11"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1230,7 +1243,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="14"/>
@@ -1238,13 +1251,13 @@
       <c r="G5" s="12"/>
       <c r="H5" s="18"/>
       <c r="I5" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="24"/>
@@ -1272,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="24"/>
@@ -1283,13 +1296,13 @@
       <c r="G6" s="11"/>
       <c r="H6" s="18"/>
       <c r="I6" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="24"/>
@@ -1317,10 +1330,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="24"/>
@@ -1328,13 +1341,13 @@
       <c r="G7" s="11"/>
       <c r="H7" s="18"/>
       <c r="I7" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="24"/>
@@ -1362,10 +1375,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="24"/>
@@ -1373,13 +1386,13 @@
       <c r="G8" s="11"/>
       <c r="H8" s="18"/>
       <c r="I8" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="24"/>
@@ -1407,10 +1420,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
@@ -1418,13 +1431,13 @@
       <c r="G9" s="12"/>
       <c r="H9" s="18"/>
       <c r="I9" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="24"/>
@@ -1452,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -1463,13 +1476,13 @@
       <c r="G10" s="12"/>
       <c r="H10" s="18"/>
       <c r="I10" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="24"/>
@@ -1497,10 +1510,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="24"/>
@@ -1508,13 +1521,13 @@
       <c r="G11" s="12"/>
       <c r="H11" s="18"/>
       <c r="I11" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="24"/>
@@ -1542,10 +1555,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
@@ -1553,13 +1566,13 @@
       <c r="G12" s="12"/>
       <c r="H12" s="18"/>
       <c r="I12" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="14"/>
@@ -1587,10 +1600,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
@@ -1604,7 +1617,7 @@
         <v>13</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="24"/>
@@ -1632,10 +1645,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -1649,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="24"/>
@@ -1677,10 +1690,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="24"/>
@@ -1691,10 +1704,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="24"/>
@@ -1722,10 +1735,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="24"/>
@@ -1736,10 +1749,10 @@
         <v>2</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="24"/>
@@ -1764,13 +1777,13 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8"/>
@@ -1781,10 +1794,10 @@
         <v>1</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="8"/>
@@ -1809,13 +1822,13 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="24"/>
@@ -1826,10 +1839,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="24"/>
@@ -1857,10 +1870,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="24"/>
@@ -1874,7 +1887,7 @@
         <v>9</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="24"/>
@@ -1899,13 +1912,13 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -1919,7 +1932,7 @@
         <v>10</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L20" s="9"/>
       <c r="M20" s="24"/>
@@ -1947,10 +1960,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="24"/>
@@ -1961,10 +1974,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="24"/>
@@ -1989,13 +2002,13 @@
     </row>
     <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="24"/>
@@ -2006,10 +2019,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L22" s="1"/>
       <c r="N22" s="10"/>
@@ -2033,13 +2046,13 @@
     </row>
     <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>97</v>
-      </c>
       <c r="C23" s="14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -2050,10 +2063,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="24"/>
@@ -2078,13 +2091,13 @@
     </row>
     <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D24" s="1"/>
       <c r="F24" s="10"/>
@@ -2093,10 +2106,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="24"/>
@@ -2121,13 +2134,13 @@
     </row>
     <row r="25" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="24"/>
@@ -2160,13 +2173,13 @@
     </row>
     <row r="26" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="24"/>
@@ -2258,7 +2271,10 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="H29" s="18"/>
       <c r="I29" s="13"/>
@@ -2286,6 +2302,9 @@
       <c r="AE29" s="1"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="H30" s="18"/>
       <c r="I30" s="13"/>
       <c r="J30" s="14"/>
@@ -5781,8 +5800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -5807,27 +5826,27 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="24"/>
@@ -5836,13 +5855,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="24"/>
@@ -5851,13 +5870,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="24"/>
@@ -5866,13 +5885,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="24"/>
@@ -5881,13 +5900,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="24"/>
@@ -5896,13 +5915,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="24"/>
@@ -5911,13 +5930,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="24"/>
@@ -5926,13 +5945,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="24"/>
@@ -5941,13 +5960,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="24"/>
@@ -5956,13 +5975,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="24"/>
@@ -5971,13 +5990,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="24"/>
@@ -5986,13 +6005,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="24"/>
@@ -6001,13 +6020,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="24"/>
@@ -6016,13 +6035,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="24"/>
@@ -6031,13 +6050,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="24"/>
@@ -6046,13 +6065,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="24"/>
@@ -6061,13 +6080,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="24"/>
@@ -6076,13 +6095,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="24"/>
@@ -6091,13 +6110,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="24"/>
@@ -6106,13 +6125,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="24"/>
@@ -6121,13 +6140,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="24"/>
@@ -6136,13 +6155,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="24"/>
@@ -6151,13 +6170,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="24"/>
@@ -6169,10 +6188,10 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="24"/>
@@ -6184,10 +6203,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="24"/>
@@ -6202,7 +6221,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="24"/>
@@ -6217,7 +6236,7 @@
         <v>19</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="24"/>
@@ -6232,7 +6251,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="24"/>
@@ -6247,7 +6266,7 @@
         <v>21</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="24"/>
@@ -6259,10 +6278,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="24"/>
@@ -6274,10 +6293,10 @@
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="24"/>
@@ -6289,10 +6308,10 @@
         <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="24"/>
@@ -6304,10 +6323,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="24"/>
@@ -6319,10 +6338,10 @@
         <v>3</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="24"/>
@@ -6334,10 +6353,10 @@
         <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="24"/>
@@ -6349,10 +6368,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="24"/>
@@ -6364,10 +6383,10 @@
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="24"/>
@@ -6379,10 +6398,10 @@
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="24"/>
@@ -6394,10 +6413,10 @@
         <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="24"/>
@@ -6424,10 +6443,10 @@
     </row>
     <row r="43" spans="1:7" ht="52.2" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>

</xml_diff>

<commit_message>
update stack and SQL
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE93902-1F98-4CE4-AB31-611A0159D122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE29BF12-53DA-4102-A13F-E6A7E1DAD3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="152">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -526,10 +526,6 @@
   </si>
   <si>
     <t>编译原理及GNU使用笔记</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>填其他工时表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -571,6 +567,10 @@
   </si>
   <si>
     <t>博客网页转pdf保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20221014</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1085,7 +1085,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1177,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="24"/>
@@ -1265,7 +1265,7 @@
         <v>144</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="24"/>
@@ -1355,7 +1355,7 @@
         <v>57</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="24"/>
@@ -1670,7 +1670,7 @@
         <v>13</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="24"/>
@@ -1791,7 +1791,7 @@
         <v>137</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="24"/>
@@ -2030,7 +2030,7 @@
         <v>103</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="24"/>
@@ -2162,7 +2162,7 @@
         <v>89</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="24"/>
@@ -2325,9 +2325,6 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="H29" s="18"/>
       <c r="I29" s="13"/>
@@ -6448,10 +6445,10 @@
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="24"/>
@@ -6506,10 +6503,10 @@
     </row>
     <row r="44" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>

</xml_diff>

<commit_message>
update string match algorithm blog
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07936D90-7701-4C22-BEEA-815AB2BC1ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366F1BCC-25C8-44F9-A796-93F450DFF637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="160">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -600,6 +600,10 @@
   </si>
   <si>
     <t>20230131</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230201</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1089,7 +1093,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -2065,12 +2069,12 @@
         <v>157</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+        <v>159</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="8"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="12"/>
       <c r="I22" s="10" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
update C time.h function
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366F1BCC-25C8-44F9-A796-93F450DFF637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580B19DF-A8A2-46CF-807A-68DDB94E8313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,7 @@
     <sheet name="暂时不管" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -599,11 +600,11 @@
     <t>简单高效的字符串匹配算法</t>
   </si>
   <si>
-    <t>20230131</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20230201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230202</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1093,7 +1094,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -2069,7 +2070,7 @@
         <v>157</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="15"/>
@@ -2307,7 +2308,7 @@
         <v>86</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L27" s="7"/>
       <c r="M27" s="15"/>

</xml_diff>

<commit_message>
update DQL syntax: instr()
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580B19DF-A8A2-46CF-807A-68DDB94E8313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51498C75-2062-4EC1-AC30-1B0CBEF273CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,12 +12,11 @@
     <sheet name="暂时不管" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="162">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -526,10 +525,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20221114</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SQL笔记（DQL语句）</t>
   </si>
   <si>
@@ -605,6 +600,18 @@
   </si>
   <si>
     <t>20230202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发布39篇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230203</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1094,7 +1101,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1371,7 @@
         <v>55</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="15"/>
@@ -1392,10 +1399,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="15"/>
@@ -1440,7 +1447,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
@@ -1589,7 +1596,7 @@
         <v>136</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="15"/>
@@ -1679,7 +1686,7 @@
         <v>75</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="15"/>
@@ -1721,13 +1728,13 @@
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="L14" s="7"/>
-      <c r="M14" s="15"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="8"/>
       <c r="O14" s="3"/>
       <c r="P14" s="1"/>
@@ -1755,7 +1762,7 @@
         <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="15"/>
@@ -1766,10 +1773,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="15"/>
@@ -1890,7 +1897,7 @@
         <v>113</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="15"/>
@@ -1901,10 +1908,10 @@
         <v>2</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="15"/>
@@ -1935,7 +1942,7 @@
         <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="15"/>
@@ -1949,7 +1956,7 @@
         <v>98</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="15"/>
@@ -1977,10 +1984,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1994,7 +2001,7 @@
         <v>106</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="3"/>
@@ -2022,10 +2029,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -2067,10 +2074,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="15"/>
@@ -2112,10 +2119,10 @@
         <v>89</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -2294,7 +2301,7 @@
         <v>109</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
@@ -2308,7 +2315,7 @@
         <v>86</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L27" s="7"/>
       <c r="M27" s="15"/>
@@ -5340,10 +5347,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -5974,42 +5981,46 @@
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="C42" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>130</v>
-      </c>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="3"/>
+      <c r="F43" s="1"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>126</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -6017,7 +6028,6 @@
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -6029,7 +6039,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -6037,7 +6047,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="3"/>
+      <c r="F48" s="1"/>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -6097,7 +6107,7 @@
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
+      <c r="A56" s="10"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -6105,7 +6115,7 @@
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
+      <c r="A57" s="11"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -6121,9 +6131,12 @@
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
+      <c r="A59" s="10"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
@@ -6422,6 +6435,8 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
@@ -6593,6 +6608,9 @@
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update c/c++ io blogs
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1302F3-E892-42EF-AD72-A82BFD1B6C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5813553-B856-4198-9A46-4D4A811962C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -540,80 +540,89 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>C（C++）文件读写笔记</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20230228</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>C++ Primer Plus拾遗</t>
+  </si>
+  <si>
+    <t>LeetCode贪心算法合集</t>
+  </si>
+  <si>
+    <t>20230301</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>函数模板（书8.5）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命名空间（书9.3）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++面向对象笔记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230303</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows下PostgreSQL编译调试笔记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230314</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230324</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.1-11.5运算符重载与友元函数暂时跳过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230324</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230325</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230329</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230330</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230331</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230404</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>C（C++）字符串操作笔记</t>
-  </si>
-  <si>
-    <t>C++ Primer Plus拾遗</t>
-  </si>
-  <si>
-    <t>LeetCode贪心算法合集</t>
-  </si>
-  <si>
-    <t>20230301</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>函数模板（书8.5）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>命名空间（书9.3）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C++面向对象笔记</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230303</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230309</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Windows下PostgreSQL编译调试笔记</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230314</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230324</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.1-11.5运算符重载与友元函数暂时跳过</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230324</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230325</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230329</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230330</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230331</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C读写笔记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++读写笔记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230407</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1099,11 +1108,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE176"/>
+  <dimension ref="A1:AE177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1449,7 +1458,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
@@ -1553,10 +1562,10 @@
         <v>120</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="L10" s="7"/>
-      <c r="M10" s="3"/>
+      <c r="M10" s="15"/>
       <c r="N10" s="8"/>
       <c r="O10" s="9"/>
       <c r="P10" s="1"/>
@@ -1629,7 +1638,7 @@
         <v>53</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3"/>
@@ -1688,7 +1697,7 @@
         <v>122</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="3"/>
@@ -1733,7 +1742,7 @@
         <v>123</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="3"/>
@@ -1865,7 +1874,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>126</v>
@@ -1899,7 +1908,7 @@
         <v>101</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="15"/>
@@ -2003,7 +2012,7 @@
         <v>86</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="15"/>
@@ -2045,10 +2054,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="3"/>
@@ -2076,10 +2085,10 @@
         <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="15"/>
@@ -2090,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="15"/>
@@ -2135,12 +2144,13 @@
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L23" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
       <c r="N23" s="8"/>
       <c r="O23" s="3"/>
       <c r="P23" s="1"/>
@@ -2179,15 +2189,14 @@
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L24" s="7"/>
-      <c r="M24" s="15"/>
+        <v>162</v>
+      </c>
+      <c r="L24" s="1"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="9"/>
+      <c r="O24" s="3"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -2211,10 +2220,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
       <c r="L25" s="7"/>
       <c r="M25" s="15"/>
@@ -2243,15 +2252,15 @@
         <v>1</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="L26" s="7"/>
+      <c r="M26" s="15"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="3"/>
+      <c r="O26" s="9"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -2274,14 +2283,21 @@
         <v>106</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="10"/>
-      <c r="K27" s="1"/>
+      <c r="I27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-      <c r="N27" s="3"/>
+      <c r="N27" s="8"/>
       <c r="O27" s="3"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -2302,10 +2318,10 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="11"/>
+      <c r="I28" s="10"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2331,7 +2347,7 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2339,7 +2355,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="10"/>
+      <c r="I29" s="11"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2396,7 +2412,7 @@
     <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2430,7 +2446,7 @@
     <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2752,7 +2768,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
@@ -2783,7 +2799,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
-      <c r="N43" s="3"/>
+      <c r="N43" s="1"/>
       <c r="O43" s="3"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
@@ -2907,7 +2923,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
+      <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
@@ -2938,7 +2954,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="N48" s="3"/>
+      <c r="N48" s="1"/>
       <c r="O48" s="3"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
@@ -3182,7 +3198,7 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="12"/>
-      <c r="I56" s="11"/>
+      <c r="I56" s="10"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -3213,7 +3229,7 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="12"/>
-      <c r="I57" s="10"/>
+      <c r="I57" s="11"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -3275,9 +3291,12 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="5"/>
+      <c r="I59" s="10"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
@@ -4727,6 +4746,7 @@
       <c r="H117" s="12"/>
       <c r="I117" s="5"/>
       <c r="K117" s="1"/>
+      <c r="L117" s="1"/>
       <c r="P117" s="1"/>
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
@@ -4774,6 +4794,7 @@
       <c r="D119" s="1"/>
       <c r="H119" s="12"/>
       <c r="I119" s="5"/>
+      <c r="K119" s="1"/>
       <c r="P119" s="1"/>
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
@@ -5256,6 +5277,9 @@
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="I176" s="5"/>
+    </row>
+    <row r="177" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I177" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F40">

</xml_diff>

<commit_message>
update gdb and sql notes
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5813553-B856-4198-9A46-4D4A811962C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0481755-7DED-4EA3-A17F-8DF2F8E39296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>HTML自学笔记#2</t>
-  </si>
-  <si>
-    <t>B树与B+树</t>
   </si>
   <si>
     <t>gdb调试笔记</t>
@@ -479,10 +476,6 @@
     <t>经典动态规划算法合集</t>
   </si>
   <si>
-    <t>20221122</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20221124</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -602,10 +595,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230331</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20230404</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -623,6 +612,18 @@
   </si>
   <si>
     <t>20230407</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230412</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230414</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B树与B+树</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1112,7 +1113,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1146,16 +1147,16 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="5" t="s">
@@ -1168,16 +1169,16 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1204,7 +1205,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="15"/>
@@ -1212,13 +1213,13 @@
       <c r="G2" s="9"/>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="15"/>
@@ -1233,7 +1234,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="15"/>
@@ -1241,13 +1242,13 @@
       <c r="G3" s="9"/>
       <c r="H3" s="12"/>
       <c r="I3" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="15"/>
@@ -1275,10 +1276,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="15"/>
@@ -1286,13 +1287,13 @@
       <c r="G4" s="9"/>
       <c r="H4" s="12"/>
       <c r="I4" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="15"/>
@@ -1323,7 +1324,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="1"/>
@@ -1331,13 +1332,13 @@
       <c r="G5" s="3"/>
       <c r="H5" s="12"/>
       <c r="I5" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="15"/>
@@ -1365,10 +1366,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="15"/>
@@ -1376,13 +1377,13 @@
       <c r="G6" s="9"/>
       <c r="H6" s="12"/>
       <c r="I6" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="15"/>
@@ -1410,10 +1411,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="15"/>
@@ -1421,13 +1422,13 @@
       <c r="G7" s="9"/>
       <c r="H7" s="12"/>
       <c r="I7" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="15"/>
@@ -1455,10 +1456,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
@@ -1466,13 +1467,13 @@
       <c r="G8" s="9"/>
       <c r="H8" s="12"/>
       <c r="I8" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="15"/>
@@ -1500,10 +1501,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
@@ -1511,13 +1512,13 @@
       <c r="G9" s="3"/>
       <c r="H9" s="12"/>
       <c r="I9" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="15"/>
@@ -1545,10 +1546,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>
@@ -1556,13 +1557,13 @@
       <c r="G10" s="3"/>
       <c r="H10" s="12"/>
       <c r="I10" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="15"/>
@@ -1590,10 +1591,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="15"/>
@@ -1601,13 +1602,13 @@
       <c r="G11" s="3"/>
       <c r="H11" s="12"/>
       <c r="I11" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="15"/>
@@ -1635,10 +1636,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3"/>
@@ -1646,13 +1647,13 @@
       <c r="G12" s="3"/>
       <c r="H12" s="12"/>
       <c r="I12" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="15"/>
@@ -1680,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="3"/>
@@ -1694,10 +1695,10 @@
         <v>2</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="3"/>
@@ -1725,10 +1726,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
@@ -1739,10 +1740,10 @@
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="3"/>
@@ -1770,10 +1771,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="15"/>
@@ -1787,7 +1788,7 @@
         <v>11</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="15"/>
@@ -1815,10 +1816,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="15"/>
@@ -1829,10 +1830,10 @@
         <v>2</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="15"/>
@@ -1860,10 +1861,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
@@ -1874,10 +1875,10 @@
         <v>2</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="15"/>
@@ -1902,13 +1903,13 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="15"/>
@@ -1919,10 +1920,10 @@
         <v>2</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="15"/>
@@ -1950,10 +1951,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1964,10 +1965,10 @@
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="3"/>
@@ -1995,10 +1996,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="15"/>
@@ -2009,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="15"/>
@@ -2037,13 +2038,13 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -2054,10 +2055,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="3"/>
@@ -2082,13 +2083,13 @@
     </row>
     <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="15"/>
@@ -2099,10 +2100,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="15"/>
@@ -2127,13 +2128,13 @@
     </row>
     <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="15"/>
@@ -2144,10 +2145,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -2172,13 +2173,13 @@
     </row>
     <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
@@ -2189,10 +2190,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L24" s="1"/>
       <c r="N24" s="8"/>
@@ -2220,10 +2221,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="L25" s="7"/>
       <c r="M25" s="15"/>
@@ -2252,10 +2253,10 @@
         <v>1</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="15"/>
@@ -2280,20 +2281,20 @@
     </row>
     <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2318,7 +2319,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="10"/>
@@ -2347,7 +2348,7 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2412,7 +2413,7 @@
     <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2446,7 +2447,7 @@
     <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -5295,8 +5296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -5321,27 +5322,27 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="15"/>
@@ -5350,13 +5351,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="15"/>
@@ -5365,13 +5366,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="15"/>
@@ -5380,13 +5381,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="15"/>
@@ -5395,13 +5396,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="15"/>
@@ -5410,13 +5411,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="15"/>
@@ -5425,13 +5426,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
@@ -5440,13 +5441,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="15"/>
@@ -5455,13 +5456,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="15"/>
@@ -5470,13 +5471,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="15"/>
@@ -5485,13 +5486,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="15"/>
@@ -5500,13 +5501,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="15"/>
@@ -5515,13 +5516,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="15"/>
@@ -5530,13 +5531,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="15"/>
@@ -5545,13 +5546,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="15"/>
@@ -5560,13 +5561,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
@@ -5575,13 +5576,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="15"/>
@@ -5590,13 +5591,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="15"/>
@@ -5605,13 +5606,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="15"/>
@@ -5620,13 +5621,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="15"/>
@@ -5635,13 +5636,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="15"/>
@@ -5650,13 +5651,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="15"/>
@@ -5665,13 +5666,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
@@ -5686,7 +5687,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="15"/>
@@ -5698,10 +5699,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="15"/>
@@ -5716,7 +5717,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
@@ -5731,7 +5732,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="15"/>
@@ -5746,7 +5747,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="15"/>
@@ -5761,7 +5762,7 @@
         <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="15"/>
@@ -5776,7 +5777,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="15"/>
@@ -5791,7 +5792,7 @@
         <v>22</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="15"/>
@@ -5806,7 +5807,7 @@
         <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="15"/>
@@ -5818,10 +5819,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="15"/>
@@ -5836,7 +5837,7 @@
         <v>24</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="15"/>
@@ -5851,7 +5852,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="15"/>
@@ -5866,7 +5867,7 @@
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="15"/>
@@ -5881,7 +5882,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="15"/>
@@ -5893,10 +5894,10 @@
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="15"/>
@@ -5911,7 +5912,7 @@
         <v>28</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="15"/>
@@ -5928,10 +5929,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C42" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="3"/>
@@ -5947,13 +5948,13 @@
     </row>
     <row r="44" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -5962,10 +5963,10 @@
     </row>
     <row r="45" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>

</xml_diff>

<commit_message>
add sql limit note
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0481755-7DED-4EA3-A17F-8DF2F8E39296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85B0C0D-2089-4563-AF26-E1B6C9571BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="164">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -624,6 +624,10 @@
   </si>
   <si>
     <t>B树与B+树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230415</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1113,7 +1117,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1698,7 +1702,7 @@
         <v>121</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="3"/>

</xml_diff>

<commit_message>
add window function note
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83B1913-D750-44E1-9B1A-FC26554D7F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545442A1-3240-4475-88F2-F39BB4035855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,7 +631,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230424</t>
+    <t>20230425</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1121,7 +1121,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add lead() and lag() window function
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545442A1-3240-4475-88F2-F39BB4035855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF58B75-69BF-4190-9302-FF43147E2003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,15 +623,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230421</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20230423</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230425</t>
+    <t>20230426</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230428</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1121,7 +1121,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1301,7 @@
         <v>106</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="15"/>
@@ -1709,7 +1709,7 @@
         <v>164</v>
       </c>
       <c r="L13" s="7"/>
-      <c r="M13" s="3"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="8"/>
       <c r="O13" s="3"/>
       <c r="P13" s="1"/>
@@ -1754,7 +1754,7 @@
         <v>153</v>
       </c>
       <c r="L14" s="7"/>
-      <c r="M14" s="3"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="8"/>
       <c r="O14" s="3"/>
       <c r="P14" s="1"/>
@@ -1976,7 +1976,7 @@
         <v>92</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="3"/>

</xml_diff>

<commit_message>
modify all files to regulate the use of titles
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF58B75-69BF-4190-9302-FF43147E2003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448BF9AB-9FE1-4BA4-B39E-FDF886EC6218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="134">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,9 +105,6 @@
     <t>软件设计模式（持续更新）</t>
   </si>
   <si>
-    <t>一些编程的好习惯（持续更新）</t>
-  </si>
-  <si>
     <t>Git自学笔记（本地操作）</t>
   </si>
   <si>
@@ -293,10 +290,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20220307</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C++常用数据结构及函数</t>
   </si>
   <si>
@@ -315,18 +308,10 @@
     <t>C指针使用笔记</t>
   </si>
   <si>
-    <t>20220412</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CSDN发布</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20220704</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GBase数据库系统操作</t>
   </si>
   <si>
@@ -334,10 +319,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20220707</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C编译报错原因汇总</t>
   </si>
   <si>
@@ -345,17 +326,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20220902</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>利用数学方法进行算法优化</t>
   </si>
   <si>
-    <t>20220913</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LeetCode中神奇的链表操作</t>
   </si>
   <si>
@@ -395,10 +368,6 @@
   </si>
   <si>
     <t>VS Code使用技巧及开发环境配置</t>
-  </si>
-  <si>
-    <t>20221013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>$("aside.blog_container_aside").remove();
@@ -427,14 +396,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20221018</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20221024</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://editor.csdn.net/md/?articleId=</t>
   </si>
   <si>
@@ -442,26 +403,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20221027</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20221102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20221108</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Linux系统命令（持续更新）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20221109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SQL笔记（DQL语句）</t>
   </si>
   <si>
@@ -472,29 +417,9 @@
     <t>经典动态规划算法合集</t>
   </si>
   <si>
-    <t>20221124</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20221205</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20221206</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一笔画问题（欧拉回路）</t>
   </si>
   <si>
-    <t>20221213</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>红黑树算法详解</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -510,39 +435,19 @@
     <t>简单高效的字符串匹配算法</t>
   </si>
   <si>
-    <t>20230201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>总计</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>发布39篇</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>堆的性质与应用</t>
   </si>
   <si>
-    <t>20230223</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230228</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C++ Primer Plus拾遗</t>
   </si>
   <si>
     <t>LeetCode贪心算法合集</t>
   </si>
   <si>
-    <t>20230301</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>函数模板（书8.5）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -555,46 +460,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230303</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Windows下PostgreSQL编译调试笔记</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230314</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230324</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>11.1-11.5运算符重载与友元函数暂时跳过</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230324</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20230325</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230329</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230330</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230404</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C（C++）字符串操作笔记</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -607,31 +484,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230407</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230412</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20230414</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>B树与B+树</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230423</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20230426</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230428</t>
+    <t>规范使用标题改造</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230510</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发布38篇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Python专栏</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1119,9 +996,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1155,16 +1032,16 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="5" t="s">
@@ -1177,16 +1054,16 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1213,24 +1090,24 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="15"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="L2" s="7"/>
-      <c r="M2" s="15"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="8"/>
       <c r="O2" s="9"/>
     </row>
@@ -1242,24 +1119,24 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="15"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
       <c r="H3" s="12"/>
       <c r="I3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="L3" s="7"/>
-      <c r="M3" s="15"/>
+      <c r="M3" s="3"/>
       <c r="N3" s="8"/>
       <c r="O3" s="9"/>
       <c r="P3" s="1"/>
@@ -1284,10 +1161,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="15"/>
@@ -1295,16 +1172,16 @@
       <c r="G4" s="9"/>
       <c r="H4" s="12"/>
       <c r="I4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="L4" s="7"/>
-      <c r="M4" s="15"/>
+      <c r="M4" s="3"/>
       <c r="N4" s="8"/>
       <c r="O4" s="9"/>
       <c r="P4" s="1"/>
@@ -1332,24 +1209,24 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="8"/>
       <c r="G5" s="3"/>
       <c r="H5" s="12"/>
       <c r="I5" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="L5" s="7"/>
-      <c r="M5" s="15"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="8"/>
       <c r="O5" s="9"/>
       <c r="P5" s="1"/>
@@ -1374,27 +1251,27 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="15"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
       <c r="H6" s="12"/>
       <c r="I6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="L6" s="7"/>
-      <c r="M6" s="15"/>
+      <c r="M6" s="3"/>
       <c r="N6" s="8"/>
       <c r="O6" s="9"/>
       <c r="P6" s="1"/>
@@ -1419,24 +1296,24 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="15"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
       <c r="H7" s="12"/>
       <c r="I7" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="15"/>
@@ -1464,24 +1341,24 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="15"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
       <c r="H8" s="12"/>
       <c r="I8" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="15"/>
@@ -1509,10 +1386,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
@@ -1520,16 +1397,16 @@
       <c r="G9" s="3"/>
       <c r="H9" s="12"/>
       <c r="I9" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="L9" s="7"/>
-      <c r="M9" s="15"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="8"/>
       <c r="O9" s="9"/>
       <c r="P9" s="1"/>
@@ -1554,10 +1431,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>
@@ -1565,16 +1442,16 @@
       <c r="G10" s="3"/>
       <c r="H10" s="12"/>
       <c r="I10" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="L10" s="7"/>
-      <c r="M10" s="15"/>
+      <c r="M10" s="3"/>
       <c r="N10" s="8"/>
       <c r="O10" s="9"/>
       <c r="P10" s="1"/>
@@ -1599,27 +1476,27 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="15"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="8"/>
       <c r="G11" s="3"/>
       <c r="H11" s="12"/>
       <c r="I11" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="L11" s="7"/>
-      <c r="M11" s="15"/>
+      <c r="M11" s="3"/>
       <c r="N11" s="8"/>
       <c r="O11" s="9"/>
       <c r="P11" s="1"/>
@@ -1644,10 +1521,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3"/>
@@ -1655,16 +1532,16 @@
       <c r="G12" s="3"/>
       <c r="H12" s="12"/>
       <c r="I12" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L12" s="7"/>
-      <c r="M12" s="15"/>
+      <c r="M12" s="3"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9"/>
       <c r="P12" s="1"/>
@@ -1689,10 +1566,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="3"/>
@@ -1703,13 +1580,13 @@
         <v>2</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="L13" s="7"/>
-      <c r="M13" s="15"/>
+      <c r="M13" s="3"/>
       <c r="N13" s="8"/>
       <c r="O13" s="3"/>
       <c r="P13" s="1"/>
@@ -1734,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
@@ -1748,13 +1625,13 @@
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="L14" s="7"/>
-      <c r="M14" s="15"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="8"/>
       <c r="O14" s="3"/>
       <c r="P14" s="1"/>
@@ -1779,13 +1656,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="15"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
       <c r="H15" s="12"/>
@@ -1796,10 +1673,10 @@
         <v>11</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="L15" s="7"/>
-      <c r="M15" s="15"/>
+      <c r="M15" s="3"/>
       <c r="N15" s="8"/>
       <c r="O15" s="9"/>
       <c r="P15" s="1"/>
@@ -1824,13 +1701,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="15"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="8"/>
       <c r="G16" s="9"/>
       <c r="H16" s="12"/>
@@ -1838,13 +1715,13 @@
         <v>2</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="L16" s="7"/>
-      <c r="M16" s="15"/>
+      <c r="M16" s="3"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
       <c r="P16" s="1"/>
@@ -1869,13 +1746,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="15"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
       <c r="H17" s="12"/>
@@ -1883,13 +1760,13 @@
         <v>2</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="L17" s="7"/>
-      <c r="M17" s="15"/>
+      <c r="M17" s="3"/>
       <c r="N17" s="8"/>
       <c r="O17" s="9"/>
       <c r="P17" s="1"/>
@@ -1911,16 +1788,16 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="15"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="8"/>
       <c r="G18" s="9"/>
       <c r="H18" s="12"/>
@@ -1928,13 +1805,13 @@
         <v>2</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L18" s="7"/>
-      <c r="M18" s="15"/>
+      <c r="M18" s="3"/>
       <c r="N18" s="8"/>
       <c r="O18" s="3"/>
       <c r="P18" s="1"/>
@@ -1959,10 +1836,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1973,10 +1850,10 @@
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="3"/>
@@ -2004,13 +1881,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="15"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
       <c r="H20" s="12"/>
@@ -2018,13 +1895,13 @@
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="L20" s="7"/>
-      <c r="M20" s="15"/>
+      <c r="M20" s="3"/>
       <c r="N20" s="8"/>
       <c r="O20" s="9"/>
       <c r="P20" s="1"/>
@@ -2046,13 +1923,13 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -2063,10 +1940,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="3"/>
@@ -2091,16 +1968,16 @@
     </row>
     <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="15"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="8"/>
       <c r="G22" s="3"/>
       <c r="H22" s="12"/>
@@ -2108,13 +1985,13 @@
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="L22" s="7"/>
-      <c r="M22" s="15"/>
+      <c r="M22" s="3"/>
       <c r="N22" s="8"/>
       <c r="O22" s="9"/>
       <c r="P22" s="1"/>
@@ -2136,13 +2013,13 @@
     </row>
     <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="15"/>
@@ -2153,10 +2030,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -2181,13 +2058,13 @@
     </row>
     <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
@@ -2198,10 +2075,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="L24" s="1"/>
       <c r="N24" s="8"/>
@@ -2229,13 +2106,13 @@
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="L25" s="7"/>
-      <c r="M25" s="15"/>
+      <c r="M25" s="1"/>
       <c r="N25" s="8"/>
       <c r="O25" s="9"/>
       <c r="P25" s="1"/>
@@ -2261,13 +2138,13 @@
         <v>1</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="L26" s="7"/>
-      <c r="M26" s="15"/>
+      <c r="M26" s="1"/>
       <c r="N26" s="8"/>
       <c r="O26" s="9"/>
       <c r="P26" s="1"/>
@@ -2289,20 +2166,20 @@
     </row>
     <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2327,7 +2204,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="10"/>
@@ -2356,7 +2233,7 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2421,7 +2298,7 @@
     <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2455,7 +2332,7 @@
     <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="1" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2580,7 +2457,9 @@
       <c r="AE35" s="1"/>
     </row>
     <row r="36" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+      <c r="A36" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -2611,7 +2490,12 @@
       <c r="AE36" s="1"/>
     </row>
     <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
+      <c r="A37" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -2643,6 +2527,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2674,6 +2559,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -2705,6 +2591,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2736,6 +2623,7 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -5302,10 +5190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G177"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -5330,27 +5218,27 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="15"/>
@@ -5359,13 +5247,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="15"/>
@@ -5374,13 +5262,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="15"/>
@@ -5389,13 +5277,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="15"/>
@@ -5404,13 +5292,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="15"/>
@@ -5419,13 +5307,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="15"/>
@@ -5434,13 +5322,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
@@ -5449,13 +5337,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="15"/>
@@ -5464,13 +5352,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="15"/>
@@ -5479,13 +5367,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="15"/>
@@ -5494,13 +5382,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="15"/>
@@ -5509,13 +5397,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="15"/>
@@ -5524,13 +5412,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="15"/>
@@ -5539,13 +5427,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="15"/>
@@ -5554,13 +5442,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="15"/>
@@ -5569,13 +5457,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
@@ -5584,13 +5472,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="15"/>
@@ -5599,13 +5487,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="15"/>
@@ -5614,13 +5502,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="15"/>
@@ -5629,13 +5517,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="15"/>
@@ -5644,13 +5532,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="15"/>
@@ -5659,13 +5547,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="15"/>
@@ -5674,13 +5562,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
@@ -5695,7 +5583,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="15"/>
@@ -5707,10 +5595,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="15"/>
@@ -5725,7 +5613,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
@@ -5740,7 +5628,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="15"/>
@@ -5755,7 +5643,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="15"/>
@@ -5770,7 +5658,7 @@
         <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="15"/>
@@ -5785,7 +5673,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="15"/>
@@ -5800,7 +5688,7 @@
         <v>22</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="15"/>
@@ -5815,10 +5703,10 @@
         <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="E33" s="15"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
     </row>
@@ -5827,10 +5715,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="15"/>
@@ -5845,10 +5733,10 @@
         <v>24</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="15"/>
+      <c r="E35" s="3"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
     </row>
@@ -5860,10 +5748,10 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="D36" s="7"/>
-      <c r="E36" s="15"/>
+      <c r="E36" s="3"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
     </row>
@@ -5875,10 +5763,10 @@
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="15"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
     </row>
@@ -5887,13 +5775,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="15"/>
+      <c r="E38" s="3"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
     </row>
@@ -5902,80 +5790,72 @@
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="15"/>
-      <c r="F39" s="8"/>
+      <c r="F39" s="3"/>
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="15"/>
+      <c r="A40" s="10"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="9"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="C41" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="E41" s="1"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="A42" s="10"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="3"/>
+      <c r="F42" s="1"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="C43" s="1"/>
+    <row r="43" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>113</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>109</v>
-      </c>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -5983,6 +5863,7 @@
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -5994,7 +5875,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="3"/>
+      <c r="F47" s="1"/>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -6002,7 +5883,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -6062,7 +5943,7 @@
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
+      <c r="A56" s="11"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -6070,7 +5951,7 @@
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="11"/>
+      <c r="A57" s="10"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -6086,12 +5967,9 @@
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
+      <c r="A59" s="5"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
@@ -6390,8 +6268,6 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
@@ -6563,9 +6439,6 @@
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update the reason of C compile error
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8E6308-73DB-44FB-9253-C3ED0B81BC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51805F9-1D40-4076-AA1C-D4A2A8E25774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,10 +488,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20230426</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>规范使用标题改造</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -529,6 +525,10 @@
   </si>
   <si>
     <t>20230531</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230608</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -694,9 +694,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -734,9 +734,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -769,26 +769,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -821,26 +804,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1018,7 +984,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1076,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="3"/>
@@ -1124,7 +1090,7 @@
         <v>53</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="3"/>
@@ -1139,7 +1105,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="3"/>
@@ -1153,7 +1119,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="3"/>
@@ -1198,7 +1164,7 @@
         <v>99</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="3"/>
@@ -1229,7 +1195,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="3"/>
@@ -1243,7 +1209,7 @@
         <v>50</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="3"/>
@@ -1274,7 +1240,7 @@
         <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="3"/>
@@ -1288,7 +1254,7 @@
         <v>9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="3"/>
@@ -1319,7 +1285,7 @@
         <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="3"/>
@@ -1364,7 +1330,7 @@
         <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="3"/>
@@ -1409,7 +1375,7 @@
         <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
@@ -1423,7 +1389,7 @@
         <v>72</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="3"/>
@@ -1468,7 +1434,7 @@
         <v>105</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="3"/>
@@ -1499,7 +1465,7 @@
         <v>96</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="3"/>
@@ -1513,7 +1479,7 @@
         <v>80</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="3"/>
@@ -1558,7 +1524,7 @@
         <v>69</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="3"/>
@@ -1603,7 +1569,7 @@
         <v>106</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="3"/>
@@ -1648,7 +1614,7 @@
         <v>107</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="3"/>
@@ -1679,7 +1645,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="3"/>
@@ -1693,7 +1659,7 @@
         <v>11</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="3"/>
@@ -1724,7 +1690,7 @@
         <v>95</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="15"/>
@@ -1738,7 +1704,7 @@
         <v>88</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="3"/>
@@ -1769,7 +1735,7 @@
         <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
@@ -1783,7 +1749,7 @@
         <v>121</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="3"/>
@@ -1814,7 +1780,7 @@
         <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="3"/>
@@ -1828,7 +1794,7 @@
         <v>85</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="3"/>
@@ -1873,9 +1839,9 @@
         <v>87</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="L19" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="8"/>
       <c r="O19" s="3"/>
@@ -1901,10 +1867,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1918,7 +1884,7 @@
         <v>83</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="3"/>
@@ -1949,7 +1915,7 @@
         <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="3"/>
@@ -1963,7 +1929,7 @@
         <v>116</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="3"/>
@@ -1994,7 +1960,7 @@
         <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -2008,7 +1974,7 @@
         <v>124</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="3"/>
@@ -2039,7 +2005,7 @@
         <v>117</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="3"/>
@@ -2053,7 +2019,7 @@
         <v>126</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -2098,7 +2064,7 @@
         <v>125</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L24" s="1"/>
       <c r="N24" s="8"/>
@@ -2142,7 +2108,7 @@
         <v>86</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L25" s="7"/>
       <c r="M25" s="1"/>
@@ -2174,7 +2140,7 @@
         <v>79</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="1"/>
@@ -2206,7 +2172,7 @@
         <v>120</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2516,7 +2482,7 @@
     </row>
     <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2549,10 +2515,10 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -5736,7 +5702,7 @@
         <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="3"/>
@@ -5766,7 +5732,7 @@
         <v>24</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="3"/>
@@ -5781,7 +5747,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="3"/>
@@ -5796,7 +5762,7 @@
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="3"/>
@@ -5811,7 +5777,7 @@
         <v>100</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="3"/>
@@ -5846,7 +5812,7 @@
         <v>114</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="3"/>

</xml_diff>

<commit_message>
Modify some articles' menu struct and add new article: C++ STL
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51805F9-1D40-4076-AA1C-D4A2A8E25774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDCCC4F-E801-4089-BCC6-5FF50C6D178C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,10 +488,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>规范使用标题改造</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20230510</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -500,14 +496,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>未完成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Python专栏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20230511</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -530,23 +518,32 @@
   <si>
     <t>20230608</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C++STL用法笔记</t>
+  </si>
+  <si>
+    <t>20230911</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -555,7 +552,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -564,7 +561,7 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -572,7 +569,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -983,11 +980,11 @@
   <dimension ref="A1:AE177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="36" style="1" customWidth="1"/>
@@ -1007,7 +1004,7 @@
     <col min="16" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -1068,7 +1065,7 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" s="1" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1073,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="3"/>
@@ -1090,14 +1087,14 @@
         <v>53</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="3"/>
       <c r="N2" s="8"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="3"/>
@@ -1119,7 +1116,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="3"/>
@@ -1142,7 +1139,7 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" s="4" customFormat="1">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -1164,7 +1161,7 @@
         <v>99</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="3"/>
@@ -1187,7 +1184,7 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31">
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1192,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="3"/>
@@ -1209,7 +1206,7 @@
         <v>50</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="3"/>
@@ -1232,7 +1229,7 @@
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31">
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1237,7 @@
         <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="3"/>
@@ -1254,7 +1251,7 @@
         <v>9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="3"/>
@@ -1277,7 +1274,7 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1285,7 +1282,7 @@
         <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="3"/>
@@ -1322,7 +1319,7 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="3"/>
@@ -1367,7 +1364,7 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31">
       <c r="A9" s="10" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1372,7 @@
         <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
@@ -1389,7 +1386,7 @@
         <v>72</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="3"/>
@@ -1412,7 +1409,7 @@
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31">
       <c r="A10" s="10" t="s">
         <v>0</v>
       </c>
@@ -1434,7 +1431,7 @@
         <v>105</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="3"/>
@@ -1457,7 +1454,7 @@
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31">
       <c r="A11" s="10" t="s">
         <v>0</v>
       </c>
@@ -1465,7 +1462,7 @@
         <v>96</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="3"/>
@@ -1479,7 +1476,7 @@
         <v>80</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="3"/>
@@ -1502,7 +1499,7 @@
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31">
       <c r="A12" s="10" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1521,7 @@
         <v>69</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="3"/>
@@ -1547,7 +1544,7 @@
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31">
       <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1566,7 @@
         <v>106</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="3"/>
@@ -1592,7 +1589,7 @@
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31">
       <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
@@ -1614,7 +1611,7 @@
         <v>107</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="3"/>
@@ -1637,7 +1634,7 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31">
       <c r="A15" s="10" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1642,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="3"/>
@@ -1659,7 +1656,7 @@
         <v>11</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="3"/>
@@ -1682,7 +1679,7 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31">
       <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
@@ -1690,7 +1687,7 @@
         <v>95</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="15"/>
@@ -1704,7 +1701,7 @@
         <v>88</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="3"/>
@@ -1727,7 +1724,7 @@
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31">
       <c r="A17" s="10" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +1732,7 @@
         <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
@@ -1749,7 +1746,7 @@
         <v>121</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="3"/>
@@ -1772,7 +1769,7 @@
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31">
       <c r="A18" s="10" t="s">
         <v>92</v>
       </c>
@@ -1780,7 +1777,7 @@
         <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="3"/>
@@ -1794,7 +1791,7 @@
         <v>85</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="3"/>
@@ -1817,7 +1814,7 @@
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31">
       <c r="A19" s="10" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +1836,7 @@
         <v>87</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1862,15 +1859,15 @@
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1884,7 +1881,7 @@
         <v>83</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="3"/>
@@ -1907,7 +1904,7 @@
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -1915,7 +1912,7 @@
         <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="3"/>
@@ -1929,7 +1926,7 @@
         <v>116</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="3"/>
@@ -1952,7 +1949,7 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A22" s="11" t="s">
         <v>82</v>
       </c>
@@ -1960,7 +1957,7 @@
         <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1974,7 +1971,7 @@
         <v>124</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="3"/>
@@ -1997,7 +1994,7 @@
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
     </row>
-    <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A23" s="11" t="s">
         <v>82</v>
       </c>
@@ -2005,7 +2002,7 @@
         <v>117</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="3"/>
@@ -2019,7 +2016,7 @@
         <v>126</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -2042,7 +2039,7 @@
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
     </row>
-    <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>82</v>
       </c>
@@ -2064,7 +2061,7 @@
         <v>125</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L24" s="1"/>
       <c r="N24" s="8"/>
@@ -2086,7 +2083,7 @@
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>82</v>
       </c>
@@ -2108,7 +2105,7 @@
         <v>86</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L25" s="7"/>
       <c r="M25" s="1"/>
@@ -2131,7 +2128,7 @@
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="H26" s="12"/>
       <c r="I26" s="10" t="s">
         <v>1</v>
@@ -2140,7 +2137,7 @@
         <v>79</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="1"/>
@@ -2163,7 +2160,7 @@
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
     </row>
-    <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="H27" s="12"/>
       <c r="I27" s="10" t="s">
         <v>1</v>
@@ -2172,7 +2169,7 @@
         <v>120</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2195,7 +2192,7 @@
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31">
       <c r="A28" s="11" t="s">
         <v>98</v>
       </c>
@@ -2203,11 +2200,18 @@
         <v>116</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="10"/>
-      <c r="K28" s="1"/>
+      <c r="I28" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="3"/>
+      <c r="N28" s="8"/>
       <c r="O28" s="3"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
@@ -2226,7 +2230,7 @@
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31">
       <c r="B29" s="1" t="s">
         <v>118</v>
       </c>
@@ -2254,7 +2258,7 @@
       <c r="AD29" s="1"/>
       <c r="AE29" s="1"/>
     </row>
-    <row r="30" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="1" t="s">
         <v>119</v>
@@ -2288,7 +2292,7 @@
       <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
     </row>
-    <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A31" s="10"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2319,7 +2323,7 @@
       <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
     </row>
-    <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="1" t="s">
         <v>120</v>
@@ -2353,7 +2357,7 @@
       <c r="AD32" s="1"/>
       <c r="AE32" s="1"/>
     </row>
-    <row r="33" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="1" t="s">
         <v>122</v>
@@ -2387,7 +2391,7 @@
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
     </row>
-    <row r="34" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A34" s="10"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2418,7 +2422,7 @@
       <c r="AD34" s="1"/>
       <c r="AE34" s="1"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31">
       <c r="A35" s="10"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2449,7 +2453,7 @@
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
     </row>
-    <row r="36" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" ht="17.399999999999999" customHeight="1">
       <c r="A36" s="10"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2480,10 +2484,8 @@
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
     </row>
-    <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>128</v>
-      </c>
+    <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1">
+      <c r="A37" s="10"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -2513,13 +2515,8 @@
       <c r="AD37" s="1"/>
       <c r="AE37" s="1"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>132</v>
-      </c>
+    <row r="38" spans="1:31">
+      <c r="A38" s="10"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2549,7 +2546,7 @@
       <c r="AD38" s="1"/>
       <c r="AE38" s="1"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="1"/>
@@ -2581,7 +2578,7 @@
       <c r="AD39" s="1"/>
       <c r="AE39" s="1"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="1"/>
@@ -2613,7 +2610,7 @@
       <c r="AD40" s="1"/>
       <c r="AE40" s="1"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="1"/>
@@ -2645,7 +2642,7 @@
       <c r="AD41" s="1"/>
       <c r="AE41" s="1"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="1"/>
@@ -2677,7 +2674,7 @@
       <c r="AD42" s="1"/>
       <c r="AE42" s="1"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31">
       <c r="A43" s="10"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2708,7 +2705,7 @@
       <c r="AD43" s="1"/>
       <c r="AE43" s="1"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31">
       <c r="A44" s="10"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2739,7 +2736,7 @@
       <c r="AD44" s="1"/>
       <c r="AE44" s="1"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31">
       <c r="A45" s="10"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2770,7 +2767,7 @@
       <c r="AD45" s="1"/>
       <c r="AE45" s="1"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31">
       <c r="A46" s="10"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2801,7 +2798,7 @@
       <c r="AD46" s="1"/>
       <c r="AE46" s="1"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31">
       <c r="A47" s="10"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2832,7 +2829,7 @@
       <c r="AD47" s="1"/>
       <c r="AE47" s="1"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31">
       <c r="A48" s="10"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2863,7 +2860,7 @@
       <c r="AD48" s="1"/>
       <c r="AE48" s="1"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31">
       <c r="A49" s="10"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2894,7 +2891,7 @@
       <c r="AD49" s="1"/>
       <c r="AE49" s="1"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31">
       <c r="A50" s="10"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2925,7 +2922,7 @@
       <c r="AD50" s="1"/>
       <c r="AE50" s="1"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31">
       <c r="A51" s="10"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2956,7 +2953,7 @@
       <c r="AD51" s="1"/>
       <c r="AE51" s="1"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31">
       <c r="A52" s="10"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2987,7 +2984,7 @@
       <c r="AD52" s="1"/>
       <c r="AE52" s="1"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31">
       <c r="A53" s="10"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3018,7 +3015,7 @@
       <c r="AD53" s="1"/>
       <c r="AE53" s="1"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31">
       <c r="A54" s="10"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -3049,7 +3046,7 @@
       <c r="AD54" s="1"/>
       <c r="AE54" s="1"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31">
       <c r="A55" s="10"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -3080,7 +3077,7 @@
       <c r="AD55" s="1"/>
       <c r="AE55" s="1"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31">
       <c r="A56" s="10"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -3111,7 +3108,7 @@
       <c r="AD56" s="1"/>
       <c r="AE56" s="1"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31">
       <c r="A57" s="11"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -3142,7 +3139,7 @@
       <c r="AD57" s="1"/>
       <c r="AE57" s="1"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31">
       <c r="A58" s="10"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -3173,7 +3170,7 @@
       <c r="AD58" s="1"/>
       <c r="AE58" s="1"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31">
       <c r="A59" s="10"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -3204,7 +3201,7 @@
       <c r="AD59" s="1"/>
       <c r="AE59" s="1"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31">
       <c r="A60" s="5"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -3232,7 +3229,7 @@
       <c r="AD60" s="1"/>
       <c r="AE60" s="1"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31">
       <c r="A61" s="5"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -3257,7 +3254,7 @@
       <c r="AD61" s="1"/>
       <c r="AE61" s="1"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31">
       <c r="A62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -3282,7 +3279,7 @@
       <c r="AD62" s="1"/>
       <c r="AE62" s="1"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31">
       <c r="A63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3307,7 +3304,7 @@
       <c r="AD63" s="1"/>
       <c r="AE63" s="1"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31">
       <c r="A64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -3332,7 +3329,7 @@
       <c r="AD64" s="1"/>
       <c r="AE64" s="1"/>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31">
       <c r="A65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -3357,7 +3354,7 @@
       <c r="AD65" s="1"/>
       <c r="AE65" s="1"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31">
       <c r="A66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -3382,7 +3379,7 @@
       <c r="AD66" s="1"/>
       <c r="AE66" s="1"/>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31">
       <c r="A67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -3407,7 +3404,7 @@
       <c r="AD67" s="1"/>
       <c r="AE67" s="1"/>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31">
       <c r="A68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -3432,7 +3429,7 @@
       <c r="AD68" s="1"/>
       <c r="AE68" s="1"/>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31">
       <c r="A69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3457,7 +3454,7 @@
       <c r="AD69" s="1"/>
       <c r="AE69" s="1"/>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31">
       <c r="A70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3482,7 +3479,7 @@
       <c r="AD70" s="1"/>
       <c r="AE70" s="1"/>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31">
       <c r="A71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3507,7 +3504,7 @@
       <c r="AD71" s="1"/>
       <c r="AE71" s="1"/>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31">
       <c r="A72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -3532,7 +3529,7 @@
       <c r="AD72" s="1"/>
       <c r="AE72" s="1"/>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31">
       <c r="A73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -3557,7 +3554,7 @@
       <c r="AD73" s="1"/>
       <c r="AE73" s="1"/>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31">
       <c r="A74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -3582,7 +3579,7 @@
       <c r="AD74" s="1"/>
       <c r="AE74" s="1"/>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31">
       <c r="A75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -3607,7 +3604,7 @@
       <c r="AD75" s="1"/>
       <c r="AE75" s="1"/>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31">
       <c r="A76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -3632,7 +3629,7 @@
       <c r="AD76" s="1"/>
       <c r="AE76" s="1"/>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31">
       <c r="A77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -3657,7 +3654,7 @@
       <c r="AD77" s="1"/>
       <c r="AE77" s="1"/>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31">
       <c r="A78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -3682,7 +3679,7 @@
       <c r="AD78" s="1"/>
       <c r="AE78" s="1"/>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31">
       <c r="A79" s="5"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3707,7 +3704,7 @@
       <c r="AD79" s="1"/>
       <c r="AE79" s="1"/>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31">
       <c r="A80" s="5"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3732,7 +3729,7 @@
       <c r="AD80" s="1"/>
       <c r="AE80" s="1"/>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31">
       <c r="A81" s="5"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -3757,7 +3754,7 @@
       <c r="AD81" s="1"/>
       <c r="AE81" s="1"/>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31">
       <c r="A82" s="5"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -3782,7 +3779,7 @@
       <c r="AD82" s="1"/>
       <c r="AE82" s="1"/>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31">
       <c r="A83" s="5"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -3807,7 +3804,7 @@
       <c r="AD83" s="1"/>
       <c r="AE83" s="1"/>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31">
       <c r="A84" s="5"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -3832,7 +3829,7 @@
       <c r="AD84" s="1"/>
       <c r="AE84" s="1"/>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31">
       <c r="A85" s="5"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -3857,7 +3854,7 @@
       <c r="AD85" s="1"/>
       <c r="AE85" s="1"/>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31">
       <c r="A86" s="5"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -3882,7 +3879,7 @@
       <c r="AD86" s="1"/>
       <c r="AE86" s="1"/>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31">
       <c r="A87" s="5"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -3907,7 +3904,7 @@
       <c r="AD87" s="1"/>
       <c r="AE87" s="1"/>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31">
       <c r="A88" s="5"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -3932,7 +3929,7 @@
       <c r="AD88" s="1"/>
       <c r="AE88" s="1"/>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31">
       <c r="A89" s="5"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -3957,7 +3954,7 @@
       <c r="AD89" s="1"/>
       <c r="AE89" s="1"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31">
       <c r="A90" s="5"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -3982,7 +3979,7 @@
       <c r="AD90" s="1"/>
       <c r="AE90" s="1"/>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31">
       <c r="A91" s="5"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -4007,7 +4004,7 @@
       <c r="AD91" s="1"/>
       <c r="AE91" s="1"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31">
       <c r="A92" s="5"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -4032,7 +4029,7 @@
       <c r="AD92" s="1"/>
       <c r="AE92" s="1"/>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31">
       <c r="A93" s="5"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -4057,7 +4054,7 @@
       <c r="AD93" s="1"/>
       <c r="AE93" s="1"/>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:31">
       <c r="A94" s="5"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -4082,7 +4079,7 @@
       <c r="AD94" s="1"/>
       <c r="AE94" s="1"/>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:31">
       <c r="A95" s="5"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -4107,7 +4104,7 @@
       <c r="AD95" s="1"/>
       <c r="AE95" s="1"/>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:31">
       <c r="A96" s="5"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -4132,7 +4129,7 @@
       <c r="AD96" s="1"/>
       <c r="AE96" s="1"/>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31">
       <c r="A97" s="5"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -4157,7 +4154,7 @@
       <c r="AD97" s="1"/>
       <c r="AE97" s="1"/>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31">
       <c r="A98" s="5"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -4182,7 +4179,7 @@
       <c r="AD98" s="1"/>
       <c r="AE98" s="1"/>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31">
       <c r="A99" s="5"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -4207,7 +4204,7 @@
       <c r="AD99" s="1"/>
       <c r="AE99" s="1"/>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31">
       <c r="A100" s="5"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -4232,7 +4229,7 @@
       <c r="AD100" s="1"/>
       <c r="AE100" s="1"/>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31">
       <c r="A101" s="5"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -4257,7 +4254,7 @@
       <c r="AD101" s="1"/>
       <c r="AE101" s="1"/>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31">
       <c r="A102" s="5"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -4282,7 +4279,7 @@
       <c r="AD102" s="1"/>
       <c r="AE102" s="1"/>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31">
       <c r="A103" s="5"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -4307,7 +4304,7 @@
       <c r="AD103" s="1"/>
       <c r="AE103" s="1"/>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31">
       <c r="A104" s="5"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -4332,7 +4329,7 @@
       <c r="AD104" s="1"/>
       <c r="AE104" s="1"/>
     </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31">
       <c r="A105" s="5"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -4357,7 +4354,7 @@
       <c r="AD105" s="1"/>
       <c r="AE105" s="1"/>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31">
       <c r="A106" s="5"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -4382,7 +4379,7 @@
       <c r="AD106" s="1"/>
       <c r="AE106" s="1"/>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31">
       <c r="A107" s="5"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -4407,7 +4404,7 @@
       <c r="AD107" s="1"/>
       <c r="AE107" s="1"/>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31">
       <c r="A108" s="5"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -4432,7 +4429,7 @@
       <c r="AD108" s="1"/>
       <c r="AE108" s="1"/>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31">
       <c r="A109" s="5"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -4457,7 +4454,7 @@
       <c r="AD109" s="1"/>
       <c r="AE109" s="1"/>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31">
       <c r="A110" s="5"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -4482,7 +4479,7 @@
       <c r="AD110" s="1"/>
       <c r="AE110" s="1"/>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31">
       <c r="A111" s="5"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -4507,7 +4504,7 @@
       <c r="AD111" s="1"/>
       <c r="AE111" s="1"/>
     </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31">
       <c r="A112" s="5"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -4532,7 +4529,7 @@
       <c r="AD112" s="1"/>
       <c r="AE112" s="1"/>
     </row>
-    <row r="113" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:31">
       <c r="A113" s="5"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -4557,7 +4554,7 @@
       <c r="AD113" s="1"/>
       <c r="AE113" s="1"/>
     </row>
-    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:31">
       <c r="A114" s="5"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -4582,7 +4579,7 @@
       <c r="AD114" s="1"/>
       <c r="AE114" s="1"/>
     </row>
-    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31">
       <c r="A115" s="5"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -4607,7 +4604,7 @@
       <c r="AD115" s="1"/>
       <c r="AE115" s="1"/>
     </row>
-    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:31">
       <c r="A116" s="5"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -4632,7 +4629,7 @@
       <c r="AD116" s="1"/>
       <c r="AE116" s="1"/>
     </row>
-    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:31">
       <c r="A117" s="5"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -4657,7 +4654,7 @@
       <c r="AD117" s="1"/>
       <c r="AE117" s="1"/>
     </row>
-    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:31">
       <c r="A118" s="5"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -4681,7 +4678,7 @@
       <c r="AD118" s="1"/>
       <c r="AE118" s="1"/>
     </row>
-    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:31">
       <c r="A119" s="5"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -4705,7 +4702,7 @@
       <c r="AD119" s="1"/>
       <c r="AE119" s="1"/>
     </row>
-    <row r="120" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:31">
       <c r="A120" s="5"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -4728,7 +4725,7 @@
       <c r="AD120" s="1"/>
       <c r="AE120" s="1"/>
     </row>
-    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:31">
       <c r="A121" s="5"/>
       <c r="H121" s="12"/>
       <c r="I121" s="5"/>
@@ -4749,7 +4746,7 @@
       <c r="AD121" s="1"/>
       <c r="AE121" s="1"/>
     </row>
-    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:31">
       <c r="A122" s="5"/>
       <c r="H122" s="12"/>
       <c r="I122" s="5"/>
@@ -4770,7 +4767,7 @@
       <c r="AD122" s="1"/>
       <c r="AE122" s="1"/>
     </row>
-    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:31">
       <c r="A123" s="5"/>
       <c r="H123" s="12"/>
       <c r="I123" s="5"/>
@@ -4791,7 +4788,7 @@
       <c r="AD123" s="1"/>
       <c r="AE123" s="1"/>
     </row>
-    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:31">
       <c r="A124" s="5"/>
       <c r="H124" s="12"/>
       <c r="I124" s="5"/>
@@ -4812,7 +4809,7 @@
       <c r="AD124" s="1"/>
       <c r="AE124" s="1"/>
     </row>
-    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:31">
       <c r="A125" s="5"/>
       <c r="H125" s="12"/>
       <c r="I125" s="5"/>
@@ -4833,7 +4830,7 @@
       <c r="AD125" s="1"/>
       <c r="AE125" s="1"/>
     </row>
-    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:31">
       <c r="A126" s="5"/>
       <c r="H126" s="12"/>
       <c r="I126" s="5"/>
@@ -4854,7 +4851,7 @@
       <c r="AD126" s="1"/>
       <c r="AE126" s="1"/>
     </row>
-    <row r="127" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:31">
       <c r="A127" s="5"/>
       <c r="H127" s="12"/>
       <c r="I127" s="5"/>
@@ -4875,7 +4872,7 @@
       <c r="AD127" s="1"/>
       <c r="AE127" s="1"/>
     </row>
-    <row r="128" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:31">
       <c r="A128" s="5"/>
       <c r="H128" s="12"/>
       <c r="I128" s="5"/>
@@ -4896,7 +4893,7 @@
       <c r="AD128" s="1"/>
       <c r="AE128" s="1"/>
     </row>
-    <row r="129" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:31">
       <c r="A129" s="5"/>
       <c r="H129" s="12"/>
       <c r="I129" s="5"/>
@@ -4917,7 +4914,7 @@
       <c r="AD129" s="1"/>
       <c r="AE129" s="1"/>
     </row>
-    <row r="130" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:31">
       <c r="A130" s="5"/>
       <c r="H130" s="12"/>
       <c r="I130" s="5"/>
@@ -4938,7 +4935,7 @@
       <c r="AD130" s="1"/>
       <c r="AE130" s="1"/>
     </row>
-    <row r="131" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:31">
       <c r="A131" s="5"/>
       <c r="H131" s="12"/>
       <c r="I131" s="5"/>
@@ -4959,7 +4956,7 @@
       <c r="AD131" s="1"/>
       <c r="AE131" s="1"/>
     </row>
-    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:31">
       <c r="A132" s="5"/>
       <c r="H132" s="12"/>
       <c r="I132" s="5"/>
@@ -4980,7 +4977,7 @@
       <c r="AD132" s="1"/>
       <c r="AE132" s="1"/>
     </row>
-    <row r="133" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:31">
       <c r="A133" s="5"/>
       <c r="H133" s="12"/>
       <c r="I133" s="5"/>
@@ -5001,179 +4998,179 @@
       <c r="AD133" s="1"/>
       <c r="AE133" s="1"/>
     </row>
-    <row r="134" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:31">
       <c r="A134" s="5"/>
       <c r="I134" s="5"/>
     </row>
-    <row r="135" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:31">
       <c r="A135" s="5"/>
       <c r="I135" s="5"/>
     </row>
-    <row r="136" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:31">
       <c r="A136" s="5"/>
       <c r="I136" s="5"/>
     </row>
-    <row r="137" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:31">
       <c r="A137" s="5"/>
       <c r="I137" s="5"/>
     </row>
-    <row r="138" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:31">
       <c r="A138" s="5"/>
       <c r="I138" s="5"/>
     </row>
-    <row r="139" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:31">
       <c r="A139" s="5"/>
       <c r="I139" s="5"/>
     </row>
-    <row r="140" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:31">
       <c r="A140" s="5"/>
       <c r="I140" s="5"/>
     </row>
-    <row r="141" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:31">
       <c r="A141" s="5"/>
       <c r="I141" s="5"/>
     </row>
-    <row r="142" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:31">
       <c r="A142" s="5"/>
       <c r="I142" s="5"/>
     </row>
-    <row r="143" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:31">
       <c r="A143" s="5"/>
       <c r="I143" s="5"/>
     </row>
-    <row r="144" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:31">
       <c r="A144" s="5"/>
       <c r="I144" s="5"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9">
       <c r="A145" s="5"/>
       <c r="I145" s="5"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9">
       <c r="A146" s="5"/>
       <c r="I146" s="5"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9">
       <c r="A147" s="5"/>
       <c r="I147" s="5"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9">
       <c r="A148" s="5"/>
       <c r="I148" s="5"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9">
       <c r="A149" s="5"/>
       <c r="I149" s="5"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9">
       <c r="A150" s="5"/>
       <c r="I150" s="5"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9">
       <c r="A151" s="5"/>
       <c r="I151" s="5"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9">
       <c r="A152" s="5"/>
       <c r="I152" s="5"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9">
       <c r="A153" s="5"/>
       <c r="I153" s="5"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9">
       <c r="A154" s="5"/>
       <c r="I154" s="5"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9">
       <c r="A155" s="5"/>
       <c r="I155" s="5"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9">
       <c r="A156" s="5"/>
       <c r="I156" s="5"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9">
       <c r="A157" s="5"/>
       <c r="I157" s="5"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9">
       <c r="A158" s="5"/>
       <c r="I158" s="5"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9">
       <c r="A159" s="5"/>
       <c r="I159" s="5"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9">
       <c r="A160" s="5"/>
       <c r="I160" s="5"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9">
       <c r="A161" s="5"/>
       <c r="I161" s="5"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9">
       <c r="A162" s="5"/>
       <c r="I162" s="5"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9">
       <c r="A163" s="5"/>
       <c r="I163" s="5"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9">
       <c r="A164" s="5"/>
       <c r="I164" s="5"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9">
       <c r="A165" s="5"/>
       <c r="I165" s="5"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9">
       <c r="A166" s="5"/>
       <c r="I166" s="5"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9">
       <c r="A167" s="5"/>
       <c r="I167" s="5"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9">
       <c r="A168" s="5"/>
       <c r="I168" s="5"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9">
       <c r="A169" s="5"/>
       <c r="I169" s="5"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9">
       <c r="A170" s="5"/>
       <c r="I170" s="5"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9">
       <c r="A171" s="5"/>
       <c r="I171" s="5"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9">
       <c r="A172" s="5"/>
       <c r="I172" s="5"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9">
       <c r="A173" s="5"/>
       <c r="I173" s="5"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9">
       <c r="A174" s="5"/>
       <c r="I174" s="5"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9">
       <c r="A175" s="5"/>
       <c r="I175" s="5"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9">
       <c r="A176" s="5"/>
       <c r="I176" s="5"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9">
       <c r="A177" s="5"/>
       <c r="I177" s="5"/>
     </row>
@@ -5192,10 +5189,10 @@
   <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="28" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" style="1" customWidth="1"/>
@@ -5206,7 +5203,7 @@
     <col min="7" max="7" width="13.109375" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -5229,7 +5226,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
         <v>66</v>
       </c>
@@ -5244,7 +5241,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="11" t="s">
         <v>66</v>
       </c>
@@ -5259,7 +5256,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="11" t="s">
         <v>66</v>
       </c>
@@ -5274,7 +5271,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
         <v>66</v>
       </c>
@@ -5289,7 +5286,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="11" t="s">
         <v>66</v>
       </c>
@@ -5304,7 +5301,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="11" t="s">
         <v>66</v>
       </c>
@@ -5319,7 +5316,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="11" t="s">
         <v>66</v>
       </c>
@@ -5334,7 +5331,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="11" t="s">
         <v>67</v>
       </c>
@@ -5349,7 +5346,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="11" t="s">
         <v>67</v>
       </c>
@@ -5364,7 +5361,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
@@ -5379,7 +5376,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5394,7 +5391,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="11" t="s">
         <v>67</v>
       </c>
@@ -5409,7 +5406,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="11" t="s">
         <v>67</v>
       </c>
@@ -5424,7 +5421,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="11" t="s">
         <v>67</v>
       </c>
@@ -5439,7 +5436,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="11" t="s">
         <v>67</v>
       </c>
@@ -5454,7 +5451,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="11" t="s">
         <v>67</v>
       </c>
@@ -5469,7 +5466,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="11" t="s">
         <v>67</v>
       </c>
@@ -5484,7 +5481,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="11" t="s">
         <v>67</v>
       </c>
@@ -5499,7 +5496,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="11" t="s">
         <v>67</v>
       </c>
@@ -5514,7 +5511,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="11" t="s">
         <v>67</v>
       </c>
@@ -5529,7 +5526,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="11" t="s">
         <v>68</v>
       </c>
@@ -5544,7 +5541,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="11" t="s">
         <v>68</v>
       </c>
@@ -5559,7 +5556,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="11" t="s">
         <v>68</v>
       </c>
@@ -5574,7 +5571,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="10" t="s">
         <v>6</v>
       </c>
@@ -5589,7 +5586,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="10" t="s">
         <v>6</v>
       </c>
@@ -5604,7 +5601,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="10" t="s">
         <v>6</v>
       </c>
@@ -5619,7 +5616,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="10" t="s">
         <v>6</v>
       </c>
@@ -5634,7 +5631,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="10" t="s">
         <v>6</v>
       </c>
@@ -5649,7 +5646,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="10" t="s">
         <v>6</v>
       </c>
@@ -5664,7 +5661,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="10" t="s">
         <v>3</v>
       </c>
@@ -5679,7 +5676,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="10" t="s">
         <v>3</v>
       </c>
@@ -5694,7 +5691,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="10" t="s">
         <v>3</v>
       </c>
@@ -5702,14 +5699,14 @@
         <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="3"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="10" t="s">
         <v>3</v>
       </c>
@@ -5724,7 +5721,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="10" t="s">
         <v>3</v>
       </c>
@@ -5732,14 +5729,14 @@
         <v>24</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="3"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="10" t="s">
         <v>3</v>
       </c>
@@ -5747,14 +5744,14 @@
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="3"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="10" t="s">
         <v>3</v>
       </c>
@@ -5762,14 +5759,14 @@
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="3"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="10" t="s">
         <v>3</v>
       </c>
@@ -5777,14 +5774,14 @@
         <v>100</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="3"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="10" t="s">
         <v>3</v>
       </c>
@@ -5799,7 +5796,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="10"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -5807,18 +5804,18 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="C41" s="10" t="s">
         <v>114</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="10"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -5826,7 +5823,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="36">
       <c r="A43" s="10" t="s">
         <v>97</v>
       </c>
@@ -5841,7 +5838,7 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="409.6">
       <c r="A44" s="10" t="s">
         <v>102</v>
       </c>
@@ -5854,14 +5851,14 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="10"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -5869,7 +5866,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="10"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -5877,7 +5874,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="10"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -5885,7 +5882,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="10"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -5893,7 +5890,7 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="10"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -5901,7 +5898,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" s="10"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -5909,7 +5906,7 @@
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="10"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -5917,7 +5914,7 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" s="10"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -5925,7 +5922,7 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" s="10"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -5933,7 +5930,7 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" s="10"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -5941,7 +5938,7 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" s="11"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -5949,7 +5946,7 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" s="10"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -5957,7 +5954,7 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" s="10"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -5965,478 +5962,478 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" s="5"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" s="5"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" s="5"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="5"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="5"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" s="5"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="5"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" s="5"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="5"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="5"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="5"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="5"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="5"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="5"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="5"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" s="5"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="5"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="5"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" s="5"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" s="5"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" s="5"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="5"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="5"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="5"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="5"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="5"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="5"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="5"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="5"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="5"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="5"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="5"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="5"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="5"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="5"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="5"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="5"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="5"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="5"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="5"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" s="5"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" s="5"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="5"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="5"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" s="5"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" s="5"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="5"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="5"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="5"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="5"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" s="5"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" s="5"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" s="5"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1">
       <c r="A129" s="5"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1">
       <c r="A130" s="5"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1">
       <c r="A131" s="5"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1">
       <c r="A132" s="5"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1">
       <c r="A133" s="5"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1">
       <c r="A134" s="5"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1">
       <c r="A135" s="5"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1">
       <c r="A136" s="5"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1">
       <c r="A137" s="5"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1">
       <c r="A138" s="5"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1">
       <c r="A139" s="5"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1">
       <c r="A140" s="5"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1">
       <c r="A141" s="5"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1">
       <c r="A142" s="5"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1">
       <c r="A143" s="5"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1">
       <c r="A144" s="5"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1">
       <c r="A145" s="5"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1">
       <c r="A146" s="5"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1">
       <c r="A147" s="5"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1">
       <c r="A148" s="5"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1">
       <c r="A149" s="5"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1">
       <c r="A150" s="5"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1">
       <c r="A151" s="5"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1">
       <c r="A152" s="5"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1">
       <c r="A153" s="5"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1">
       <c r="A154" s="5"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1">
       <c r="A155" s="5"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1">
       <c r="A156" s="5"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1">
       <c r="A157" s="5"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1">
       <c r="A158" s="5"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1">
       <c r="A159" s="5"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1">
       <c r="A160" s="5"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1">
       <c r="A161" s="5"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1">
       <c r="A162" s="5"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1">
       <c r="A163" s="5"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1">
       <c r="A164" s="5"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1">
       <c r="A165" s="5"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1">
       <c r="A166" s="5"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1">
       <c r="A167" s="5"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1">
       <c r="A168" s="5"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1">
       <c r="A169" s="5"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1">
       <c r="A170" s="5"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1">
       <c r="A171" s="5"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1">
       <c r="A172" s="5"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1">
       <c r="A173" s="5"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1">
       <c r="A174" s="5"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1">
       <c r="A175" s="5"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1">
       <c r="A176" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename column Web Development
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDCCC4F-E801-4089-BCC6-5FF50C6D178C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63CFFC4-D437-472F-A746-D473309367AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="140">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -244,10 +244,6 @@
   </si>
   <si>
     <t>Machine Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Web Development</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -528,22 +524,30 @@
   <si>
     <t>20230911</t>
   </si>
+  <si>
+    <t>Network and Web Development</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20230919</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -552,7 +556,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -561,7 +565,7 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -569,7 +573,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -980,11 +984,11 @@
   <dimension ref="A1:AE177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="36" style="1" customWidth="1"/>
@@ -1004,7 +1008,7 @@
     <col min="16" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -1015,16 +1019,16 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="5" t="s">
@@ -1037,16 +1041,16 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1065,7 +1069,7 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1">
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1073,7 +1077,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="3"/>
@@ -1087,14 +1091,14 @@
         <v>53</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="3"/>
       <c r="N2" s="8"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="3"/>
@@ -1116,7 +1120,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="3"/>
@@ -1139,7 +1143,7 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:31" s="4" customFormat="1">
+    <row r="4" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -1158,10 +1162,10 @@
         <v>65</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="3"/>
@@ -1184,7 +1188,7 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
@@ -1192,7 +1196,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="3"/>
@@ -1206,7 +1210,7 @@
         <v>50</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="3"/>
@@ -1229,15 +1233,15 @@
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="3"/>
@@ -1251,7 +1255,7 @@
         <v>9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="3"/>
@@ -1274,15 +1278,15 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="7" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="3"/>
@@ -1296,7 +1300,7 @@
         <v>10</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="15"/>
@@ -1319,15 +1323,15 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="3"/>
@@ -1338,10 +1342,10 @@
         <v>65</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="15"/>
@@ -1364,15 +1368,15 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
@@ -1383,10 +1387,10 @@
         <v>65</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="3"/>
@@ -1409,7 +1413,7 @@
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>0</v>
       </c>
@@ -1428,10 +1432,10 @@
         <v>65</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="3"/>
@@ -1454,15 +1458,15 @@
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="3"/>
@@ -1473,10 +1477,10 @@
         <v>65</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="3"/>
@@ -1499,7 +1503,7 @@
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +1511,7 @@
         <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3"/>
@@ -1518,10 +1522,10 @@
         <v>65</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="3"/>
@@ -1544,7 +1548,7 @@
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
@@ -1563,10 +1567,10 @@
         <v>2</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="3"/>
@@ -1589,7 +1593,7 @@
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
@@ -1608,10 +1612,10 @@
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="3"/>
@@ -1634,7 +1638,7 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1646,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="3"/>
@@ -1656,7 +1660,7 @@
         <v>11</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="3"/>
@@ -1679,15 +1683,15 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="15"/>
@@ -1698,10 +1702,10 @@
         <v>2</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="3"/>
@@ -1724,15 +1728,15 @@
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
@@ -1743,10 +1747,10 @@
         <v>2</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="3"/>
@@ -1769,15 +1773,15 @@
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="3"/>
@@ -1788,10 +1792,10 @@
         <v>2</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="3"/>
@@ -1814,15 +1818,15 @@
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1833,10 +1837,10 @@
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1859,15 +1863,15 @@
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1878,10 +1882,10 @@
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="3"/>
@@ -1904,15 +1908,15 @@
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="3"/>
@@ -1923,10 +1927,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="3"/>
@@ -1949,15 +1953,15 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1968,10 +1972,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="3"/>
@@ -1994,15 +1998,15 @@
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
     </row>
-    <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="3"/>
@@ -2013,10 +2017,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -2039,15 +2043,15 @@
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
     </row>
-    <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
@@ -2058,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L24" s="1"/>
       <c r="N24" s="8"/>
@@ -2083,15 +2087,15 @@
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="25" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="15"/>
@@ -2102,10 +2106,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L25" s="7"/>
       <c r="M25" s="1"/>
@@ -2128,16 +2132,16 @@
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="26" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H26" s="12"/>
       <c r="I26" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="1"/>
@@ -2160,16 +2164,16 @@
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
     </row>
-    <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H27" s="12"/>
       <c r="I27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2192,22 +2196,22 @@
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2230,9 +2234,9 @@
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="11"/>
@@ -2258,10 +2262,10 @@
       <c r="AD29" s="1"/>
       <c r="AE29" s="1"/>
     </row>
-    <row r="30" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="30" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2292,7 +2296,7 @@
       <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
     </row>
-    <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2323,10 +2327,10 @@
       <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
     </row>
-    <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2357,10 +2361,10 @@
       <c r="AD32" s="1"/>
       <c r="AE32" s="1"/>
     </row>
-    <row r="33" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="33" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2391,7 +2395,7 @@
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
     </row>
-    <row r="34" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="34" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2422,7 +2426,7 @@
       <c r="AD34" s="1"/>
       <c r="AE34" s="1"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2453,7 +2457,7 @@
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
     </row>
-    <row r="36" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="36" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2484,7 +2488,7 @@
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
     </row>
-    <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2515,7 +2519,7 @@
       <c r="AD37" s="1"/>
       <c r="AE37" s="1"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2546,7 +2550,7 @@
       <c r="AD38" s="1"/>
       <c r="AE38" s="1"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="1"/>
@@ -2578,7 +2582,7 @@
       <c r="AD39" s="1"/>
       <c r="AE39" s="1"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="1"/>
@@ -2610,7 +2614,7 @@
       <c r="AD40" s="1"/>
       <c r="AE40" s="1"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="1"/>
@@ -2642,7 +2646,7 @@
       <c r="AD41" s="1"/>
       <c r="AE41" s="1"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="1"/>
@@ -2674,7 +2678,7 @@
       <c r="AD42" s="1"/>
       <c r="AE42" s="1"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2705,7 +2709,7 @@
       <c r="AD43" s="1"/>
       <c r="AE43" s="1"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2736,7 +2740,7 @@
       <c r="AD44" s="1"/>
       <c r="AE44" s="1"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2767,7 +2771,7 @@
       <c r="AD45" s="1"/>
       <c r="AE45" s="1"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2798,7 +2802,7 @@
       <c r="AD46" s="1"/>
       <c r="AE46" s="1"/>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2829,7 +2833,7 @@
       <c r="AD47" s="1"/>
       <c r="AE47" s="1"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2860,7 +2864,7 @@
       <c r="AD48" s="1"/>
       <c r="AE48" s="1"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2891,7 +2895,7 @@
       <c r="AD49" s="1"/>
       <c r="AE49" s="1"/>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2922,7 +2926,7 @@
       <c r="AD50" s="1"/>
       <c r="AE50" s="1"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2953,7 +2957,7 @@
       <c r="AD51" s="1"/>
       <c r="AE51" s="1"/>
     </row>
-    <row r="52" spans="1:31">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2984,7 +2988,7 @@
       <c r="AD52" s="1"/>
       <c r="AE52" s="1"/>
     </row>
-    <row r="53" spans="1:31">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3015,7 +3019,7 @@
       <c r="AD53" s="1"/>
       <c r="AE53" s="1"/>
     </row>
-    <row r="54" spans="1:31">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -3046,7 +3050,7 @@
       <c r="AD54" s="1"/>
       <c r="AE54" s="1"/>
     </row>
-    <row r="55" spans="1:31">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -3077,7 +3081,7 @@
       <c r="AD55" s="1"/>
       <c r="AE55" s="1"/>
     </row>
-    <row r="56" spans="1:31">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -3108,7 +3112,7 @@
       <c r="AD56" s="1"/>
       <c r="AE56" s="1"/>
     </row>
-    <row r="57" spans="1:31">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -3139,7 +3143,7 @@
       <c r="AD57" s="1"/>
       <c r="AE57" s="1"/>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -3170,7 +3174,7 @@
       <c r="AD58" s="1"/>
       <c r="AE58" s="1"/>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -3201,7 +3205,7 @@
       <c r="AD59" s="1"/>
       <c r="AE59" s="1"/>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -3229,7 +3233,7 @@
       <c r="AD60" s="1"/>
       <c r="AE60" s="1"/>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -3254,7 +3258,7 @@
       <c r="AD61" s="1"/>
       <c r="AE61" s="1"/>
     </row>
-    <row r="62" spans="1:31">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -3279,7 +3283,7 @@
       <c r="AD62" s="1"/>
       <c r="AE62" s="1"/>
     </row>
-    <row r="63" spans="1:31">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3304,7 +3308,7 @@
       <c r="AD63" s="1"/>
       <c r="AE63" s="1"/>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -3329,7 +3333,7 @@
       <c r="AD64" s="1"/>
       <c r="AE64" s="1"/>
     </row>
-    <row r="65" spans="1:31">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -3354,7 +3358,7 @@
       <c r="AD65" s="1"/>
       <c r="AE65" s="1"/>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -3379,7 +3383,7 @@
       <c r="AD66" s="1"/>
       <c r="AE66" s="1"/>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -3404,7 +3408,7 @@
       <c r="AD67" s="1"/>
       <c r="AE67" s="1"/>
     </row>
-    <row r="68" spans="1:31">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -3429,7 +3433,7 @@
       <c r="AD68" s="1"/>
       <c r="AE68" s="1"/>
     </row>
-    <row r="69" spans="1:31">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3454,7 +3458,7 @@
       <c r="AD69" s="1"/>
       <c r="AE69" s="1"/>
     </row>
-    <row r="70" spans="1:31">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3479,7 +3483,7 @@
       <c r="AD70" s="1"/>
       <c r="AE70" s="1"/>
     </row>
-    <row r="71" spans="1:31">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3504,7 +3508,7 @@
       <c r="AD71" s="1"/>
       <c r="AE71" s="1"/>
     </row>
-    <row r="72" spans="1:31">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -3529,7 +3533,7 @@
       <c r="AD72" s="1"/>
       <c r="AE72" s="1"/>
     </row>
-    <row r="73" spans="1:31">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -3554,7 +3558,7 @@
       <c r="AD73" s="1"/>
       <c r="AE73" s="1"/>
     </row>
-    <row r="74" spans="1:31">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -3579,7 +3583,7 @@
       <c r="AD74" s="1"/>
       <c r="AE74" s="1"/>
     </row>
-    <row r="75" spans="1:31">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -3604,7 +3608,7 @@
       <c r="AD75" s="1"/>
       <c r="AE75" s="1"/>
     </row>
-    <row r="76" spans="1:31">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -3629,7 +3633,7 @@
       <c r="AD76" s="1"/>
       <c r="AE76" s="1"/>
     </row>
-    <row r="77" spans="1:31">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -3654,7 +3658,7 @@
       <c r="AD77" s="1"/>
       <c r="AE77" s="1"/>
     </row>
-    <row r="78" spans="1:31">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -3679,7 +3683,7 @@
       <c r="AD78" s="1"/>
       <c r="AE78" s="1"/>
     </row>
-    <row r="79" spans="1:31">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3704,7 +3708,7 @@
       <c r="AD79" s="1"/>
       <c r="AE79" s="1"/>
     </row>
-    <row r="80" spans="1:31">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3729,7 +3733,7 @@
       <c r="AD80" s="1"/>
       <c r="AE80" s="1"/>
     </row>
-    <row r="81" spans="1:31">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -3754,7 +3758,7 @@
       <c r="AD81" s="1"/>
       <c r="AE81" s="1"/>
     </row>
-    <row r="82" spans="1:31">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -3779,7 +3783,7 @@
       <c r="AD82" s="1"/>
       <c r="AE82" s="1"/>
     </row>
-    <row r="83" spans="1:31">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -3804,7 +3808,7 @@
       <c r="AD83" s="1"/>
       <c r="AE83" s="1"/>
     </row>
-    <row r="84" spans="1:31">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -3829,7 +3833,7 @@
       <c r="AD84" s="1"/>
       <c r="AE84" s="1"/>
     </row>
-    <row r="85" spans="1:31">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -3854,7 +3858,7 @@
       <c r="AD85" s="1"/>
       <c r="AE85" s="1"/>
     </row>
-    <row r="86" spans="1:31">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -3879,7 +3883,7 @@
       <c r="AD86" s="1"/>
       <c r="AE86" s="1"/>
     </row>
-    <row r="87" spans="1:31">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -3904,7 +3908,7 @@
       <c r="AD87" s="1"/>
       <c r="AE87" s="1"/>
     </row>
-    <row r="88" spans="1:31">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -3929,7 +3933,7 @@
       <c r="AD88" s="1"/>
       <c r="AE88" s="1"/>
     </row>
-    <row r="89" spans="1:31">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -3954,7 +3958,7 @@
       <c r="AD89" s="1"/>
       <c r="AE89" s="1"/>
     </row>
-    <row r="90" spans="1:31">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -3979,7 +3983,7 @@
       <c r="AD90" s="1"/>
       <c r="AE90" s="1"/>
     </row>
-    <row r="91" spans="1:31">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -4004,7 +4008,7 @@
       <c r="AD91" s="1"/>
       <c r="AE91" s="1"/>
     </row>
-    <row r="92" spans="1:31">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -4029,7 +4033,7 @@
       <c r="AD92" s="1"/>
       <c r="AE92" s="1"/>
     </row>
-    <row r="93" spans="1:31">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -4054,7 +4058,7 @@
       <c r="AD93" s="1"/>
       <c r="AE93" s="1"/>
     </row>
-    <row r="94" spans="1:31">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -4079,7 +4083,7 @@
       <c r="AD94" s="1"/>
       <c r="AE94" s="1"/>
     </row>
-    <row r="95" spans="1:31">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -4104,7 +4108,7 @@
       <c r="AD95" s="1"/>
       <c r="AE95" s="1"/>
     </row>
-    <row r="96" spans="1:31">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -4129,7 +4133,7 @@
       <c r="AD96" s="1"/>
       <c r="AE96" s="1"/>
     </row>
-    <row r="97" spans="1:31">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -4154,7 +4158,7 @@
       <c r="AD97" s="1"/>
       <c r="AE97" s="1"/>
     </row>
-    <row r="98" spans="1:31">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -4179,7 +4183,7 @@
       <c r="AD98" s="1"/>
       <c r="AE98" s="1"/>
     </row>
-    <row r="99" spans="1:31">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -4204,7 +4208,7 @@
       <c r="AD99" s="1"/>
       <c r="AE99" s="1"/>
     </row>
-    <row r="100" spans="1:31">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -4229,7 +4233,7 @@
       <c r="AD100" s="1"/>
       <c r="AE100" s="1"/>
     </row>
-    <row r="101" spans="1:31">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -4254,7 +4258,7 @@
       <c r="AD101" s="1"/>
       <c r="AE101" s="1"/>
     </row>
-    <row r="102" spans="1:31">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -4279,7 +4283,7 @@
       <c r="AD102" s="1"/>
       <c r="AE102" s="1"/>
     </row>
-    <row r="103" spans="1:31">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -4304,7 +4308,7 @@
       <c r="AD103" s="1"/>
       <c r="AE103" s="1"/>
     </row>
-    <row r="104" spans="1:31">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -4329,7 +4333,7 @@
       <c r="AD104" s="1"/>
       <c r="AE104" s="1"/>
     </row>
-    <row r="105" spans="1:31">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -4354,7 +4358,7 @@
       <c r="AD105" s="1"/>
       <c r="AE105" s="1"/>
     </row>
-    <row r="106" spans="1:31">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -4379,7 +4383,7 @@
       <c r="AD106" s="1"/>
       <c r="AE106" s="1"/>
     </row>
-    <row r="107" spans="1:31">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -4404,7 +4408,7 @@
       <c r="AD107" s="1"/>
       <c r="AE107" s="1"/>
     </row>
-    <row r="108" spans="1:31">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -4429,7 +4433,7 @@
       <c r="AD108" s="1"/>
       <c r="AE108" s="1"/>
     </row>
-    <row r="109" spans="1:31">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -4454,7 +4458,7 @@
       <c r="AD109" s="1"/>
       <c r="AE109" s="1"/>
     </row>
-    <row r="110" spans="1:31">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -4479,7 +4483,7 @@
       <c r="AD110" s="1"/>
       <c r="AE110" s="1"/>
     </row>
-    <row r="111" spans="1:31">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -4504,7 +4508,7 @@
       <c r="AD111" s="1"/>
       <c r="AE111" s="1"/>
     </row>
-    <row r="112" spans="1:31">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -4529,7 +4533,7 @@
       <c r="AD112" s="1"/>
       <c r="AE112" s="1"/>
     </row>
-    <row r="113" spans="1:31">
+    <row r="113" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -4554,7 +4558,7 @@
       <c r="AD113" s="1"/>
       <c r="AE113" s="1"/>
     </row>
-    <row r="114" spans="1:31">
+    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -4579,7 +4583,7 @@
       <c r="AD114" s="1"/>
       <c r="AE114" s="1"/>
     </row>
-    <row r="115" spans="1:31">
+    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -4604,7 +4608,7 @@
       <c r="AD115" s="1"/>
       <c r="AE115" s="1"/>
     </row>
-    <row r="116" spans="1:31">
+    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -4629,7 +4633,7 @@
       <c r="AD116" s="1"/>
       <c r="AE116" s="1"/>
     </row>
-    <row r="117" spans="1:31">
+    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -4654,7 +4658,7 @@
       <c r="AD117" s="1"/>
       <c r="AE117" s="1"/>
     </row>
-    <row r="118" spans="1:31">
+    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -4678,7 +4682,7 @@
       <c r="AD118" s="1"/>
       <c r="AE118" s="1"/>
     </row>
-    <row r="119" spans="1:31">
+    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -4702,7 +4706,7 @@
       <c r="AD119" s="1"/>
       <c r="AE119" s="1"/>
     </row>
-    <row r="120" spans="1:31">
+    <row r="120" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -4725,7 +4729,7 @@
       <c r="AD120" s="1"/>
       <c r="AE120" s="1"/>
     </row>
-    <row r="121" spans="1:31">
+    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="H121" s="12"/>
       <c r="I121" s="5"/>
@@ -4746,7 +4750,7 @@
       <c r="AD121" s="1"/>
       <c r="AE121" s="1"/>
     </row>
-    <row r="122" spans="1:31">
+    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="H122" s="12"/>
       <c r="I122" s="5"/>
@@ -4767,7 +4771,7 @@
       <c r="AD122" s="1"/>
       <c r="AE122" s="1"/>
     </row>
-    <row r="123" spans="1:31">
+    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="H123" s="12"/>
       <c r="I123" s="5"/>
@@ -4788,7 +4792,7 @@
       <c r="AD123" s="1"/>
       <c r="AE123" s="1"/>
     </row>
-    <row r="124" spans="1:31">
+    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="H124" s="12"/>
       <c r="I124" s="5"/>
@@ -4809,7 +4813,7 @@
       <c r="AD124" s="1"/>
       <c r="AE124" s="1"/>
     </row>
-    <row r="125" spans="1:31">
+    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="H125" s="12"/>
       <c r="I125" s="5"/>
@@ -4830,7 +4834,7 @@
       <c r="AD125" s="1"/>
       <c r="AE125" s="1"/>
     </row>
-    <row r="126" spans="1:31">
+    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="H126" s="12"/>
       <c r="I126" s="5"/>
@@ -4851,7 +4855,7 @@
       <c r="AD126" s="1"/>
       <c r="AE126" s="1"/>
     </row>
-    <row r="127" spans="1:31">
+    <row r="127" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="H127" s="12"/>
       <c r="I127" s="5"/>
@@ -4872,7 +4876,7 @@
       <c r="AD127" s="1"/>
       <c r="AE127" s="1"/>
     </row>
-    <row r="128" spans="1:31">
+    <row r="128" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="H128" s="12"/>
       <c r="I128" s="5"/>
@@ -4893,7 +4897,7 @@
       <c r="AD128" s="1"/>
       <c r="AE128" s="1"/>
     </row>
-    <row r="129" spans="1:31">
+    <row r="129" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="H129" s="12"/>
       <c r="I129" s="5"/>
@@ -4914,7 +4918,7 @@
       <c r="AD129" s="1"/>
       <c r="AE129" s="1"/>
     </row>
-    <row r="130" spans="1:31">
+    <row r="130" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="H130" s="12"/>
       <c r="I130" s="5"/>
@@ -4935,7 +4939,7 @@
       <c r="AD130" s="1"/>
       <c r="AE130" s="1"/>
     </row>
-    <row r="131" spans="1:31">
+    <row r="131" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="H131" s="12"/>
       <c r="I131" s="5"/>
@@ -4956,7 +4960,7 @@
       <c r="AD131" s="1"/>
       <c r="AE131" s="1"/>
     </row>
-    <row r="132" spans="1:31">
+    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="H132" s="12"/>
       <c r="I132" s="5"/>
@@ -4977,7 +4981,7 @@
       <c r="AD132" s="1"/>
       <c r="AE132" s="1"/>
     </row>
-    <row r="133" spans="1:31">
+    <row r="133" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="H133" s="12"/>
       <c r="I133" s="5"/>
@@ -4998,179 +5002,179 @@
       <c r="AD133" s="1"/>
       <c r="AE133" s="1"/>
     </row>
-    <row r="134" spans="1:31">
+    <row r="134" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="I134" s="5"/>
     </row>
-    <row r="135" spans="1:31">
+    <row r="135" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="I135" s="5"/>
     </row>
-    <row r="136" spans="1:31">
+    <row r="136" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="I136" s="5"/>
     </row>
-    <row r="137" spans="1:31">
+    <row r="137" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="I137" s="5"/>
     </row>
-    <row r="138" spans="1:31">
+    <row r="138" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="I138" s="5"/>
     </row>
-    <row r="139" spans="1:31">
+    <row r="139" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="I139" s="5"/>
     </row>
-    <row r="140" spans="1:31">
+    <row r="140" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="I140" s="5"/>
     </row>
-    <row r="141" spans="1:31">
+    <row r="141" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="I141" s="5"/>
     </row>
-    <row r="142" spans="1:31">
+    <row r="142" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="I142" s="5"/>
     </row>
-    <row r="143" spans="1:31">
+    <row r="143" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="I143" s="5"/>
     </row>
-    <row r="144" spans="1:31">
+    <row r="144" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="I144" s="5"/>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="I145" s="5"/>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="I146" s="5"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="I147" s="5"/>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
       <c r="I148" s="5"/>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
       <c r="I149" s="5"/>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
       <c r="I150" s="5"/>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
       <c r="I151" s="5"/>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="I152" s="5"/>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
       <c r="I153" s="5"/>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
       <c r="I154" s="5"/>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
       <c r="I155" s="5"/>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
       <c r="I156" s="5"/>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="I157" s="5"/>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
       <c r="I158" s="5"/>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
       <c r="I159" s="5"/>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
       <c r="I160" s="5"/>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="I161" s="5"/>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="I162" s="5"/>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="I163" s="5"/>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="I164" s="5"/>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="I165" s="5"/>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="I166" s="5"/>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="I167" s="5"/>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="I168" s="5"/>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="I169" s="5"/>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="I170" s="5"/>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="I171" s="5"/>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="I172" s="5"/>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="I173" s="5"/>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
       <c r="I174" s="5"/>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="I175" s="5"/>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="I176" s="5"/>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
       <c r="I177" s="5"/>
     </row>
@@ -5186,15 +5190,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" style="2" customWidth="1"/>
@@ -5203,7 +5207,7 @@
     <col min="7" max="7" width="13.109375" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -5214,19 +5218,19 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>66</v>
       </c>
@@ -5241,7 +5245,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>66</v>
       </c>
@@ -5256,7 +5260,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>66</v>
       </c>
@@ -5271,7 +5275,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>66</v>
       </c>
@@ -5286,7 +5290,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>66</v>
       </c>
@@ -5301,7 +5305,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>66</v>
       </c>
@@ -5316,7 +5320,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>66</v>
       </c>
@@ -5331,7 +5335,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>67</v>
       </c>
@@ -5346,7 +5350,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>67</v>
       </c>
@@ -5361,7 +5365,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
@@ -5376,7 +5380,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5391,7 +5395,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>67</v>
       </c>
@@ -5406,7 +5410,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>67</v>
       </c>
@@ -5421,7 +5425,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>67</v>
       </c>
@@ -5436,7 +5440,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>67</v>
       </c>
@@ -5451,7 +5455,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>67</v>
       </c>
@@ -5466,7 +5470,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>67</v>
       </c>
@@ -5481,7 +5485,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>67</v>
       </c>
@@ -5496,7 +5500,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>67</v>
       </c>
@@ -5511,7 +5515,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>67</v>
       </c>
@@ -5526,72 +5530,69 @@
       <c r="F21" s="3"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="15"/>
       <c r="F23" s="3"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
       <c r="F24" s="3"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="10" t="s">
-        <v>6</v>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>138</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="15"/>
-      <c r="F25" s="8"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>64</v>
@@ -5601,288 +5602,295 @@
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="15"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="8"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="8"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="15"/>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="8"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="3"/>
+      <c r="F32" s="1"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="8"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="1"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="8"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="8"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="1"/>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="3"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="3"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="3"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="9"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="9"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="10"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="15"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="C41" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="G40" s="9"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="10"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" ht="36">
-      <c r="A43" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>103</v>
-      </c>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="3"/>
+      <c r="F43" s="1"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="409.6">
+    <row r="44" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B44" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>100</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="10"/>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="3"/>
+      <c r="F48" s="1"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -5890,7 +5898,7 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -5898,7 +5906,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -5906,7 +5914,7 @@
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -5914,7 +5922,7 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -5922,7 +5930,7 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -5930,7 +5938,7 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -5938,23 +5946,23 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="11"/>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="10"/>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -5962,479 +5970,487 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="5"/>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="E59" s="1"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add new blog: LaTeX math sign
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC0FBF6-233D-4BBE-BC0C-9AE46BFAADC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709C2E98-6C4B-4B72-AB18-D673B677A5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="148">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -549,22 +549,30 @@
   <si>
     <t>20231010</t>
   </si>
+  <si>
+    <t>20231020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LaTeX公式与符号总结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -573,7 +581,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -582,7 +590,7 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -590,7 +598,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1005,7 +1013,7 @@
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="36" style="1" customWidth="1"/>
@@ -1025,7 +1033,7 @@
     <col min="16" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -1086,7 +1094,7 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1">
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1123,7 @@
       <c r="N2" s="8"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1168,7 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:31" s="4" customFormat="1">
+    <row r="4" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -1205,7 +1213,7 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
@@ -1250,7 +1258,7 @@
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
@@ -1295,7 +1303,7 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="7" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1348,7 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +1393,7 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>0</v>
       </c>
@@ -1430,7 +1438,7 @@
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1483,7 @@
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>0</v>
       </c>
@@ -1520,7 +1528,7 @@
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +1573,7 @@
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
@@ -1610,7 +1618,7 @@
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
@@ -1655,7 +1663,7 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>0</v>
       </c>
@@ -1700,7 +1708,7 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
@@ -1745,7 +1753,7 @@
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>0</v>
       </c>
@@ -1790,7 +1798,7 @@
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>91</v>
       </c>
@@ -1835,7 +1843,7 @@
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>0</v>
       </c>
@@ -1880,7 +1888,7 @@
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -1925,7 +1933,7 @@
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -1970,7 +1978,7 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="22" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>81</v>
       </c>
@@ -2015,7 +2023,7 @@
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
     </row>
-    <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="23" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>81</v>
       </c>
@@ -2060,7 +2068,7 @@
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
     </row>
-    <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="24" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>81</v>
       </c>
@@ -2104,7 +2112,7 @@
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="25" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>81</v>
       </c>
@@ -2149,7 +2157,7 @@
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="26" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H26" s="12"/>
       <c r="I26" s="10" t="s">
         <v>1</v>
@@ -2181,7 +2189,7 @@
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
     </row>
-    <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="27" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H27" s="12"/>
       <c r="I27" s="10" t="s">
         <v>1</v>
@@ -2213,7 +2221,7 @@
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>97</v>
       </c>
@@ -2251,7 +2259,7 @@
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>117</v>
       </c>
@@ -2279,7 +2287,7 @@
       <c r="AD29" s="1"/>
       <c r="AE29" s="1"/>
     </row>
-    <row r="30" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="30" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="1" t="s">
         <v>118</v>
@@ -2313,7 +2321,7 @@
       <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
     </row>
-    <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="31" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2344,7 +2352,7 @@
       <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
     </row>
-    <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="32" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="1" t="s">
         <v>119</v>
@@ -2378,7 +2386,7 @@
       <c r="AD32" s="1"/>
       <c r="AE32" s="1"/>
     </row>
-    <row r="33" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="33" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="1" t="s">
         <v>121</v>
@@ -2412,7 +2420,7 @@
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
     </row>
-    <row r="34" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="34" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2443,7 +2451,7 @@
       <c r="AD34" s="1"/>
       <c r="AE34" s="1"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2474,7 +2482,7 @@
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
     </row>
-    <row r="36" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="36" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2505,7 +2513,7 @@
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
     </row>
-    <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1">
+    <row r="37" spans="1:31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2536,7 +2544,7 @@
       <c r="AD37" s="1"/>
       <c r="AE37" s="1"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2567,7 +2575,7 @@
       <c r="AD38" s="1"/>
       <c r="AE38" s="1"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="1"/>
@@ -2599,7 +2607,7 @@
       <c r="AD39" s="1"/>
       <c r="AE39" s="1"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="1"/>
@@ -2631,7 +2639,7 @@
       <c r="AD40" s="1"/>
       <c r="AE40" s="1"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="1"/>
@@ -2663,7 +2671,7 @@
       <c r="AD41" s="1"/>
       <c r="AE41" s="1"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="1"/>
@@ -2695,7 +2703,7 @@
       <c r="AD42" s="1"/>
       <c r="AE42" s="1"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2726,7 +2734,7 @@
       <c r="AD43" s="1"/>
       <c r="AE43" s="1"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2757,7 +2765,7 @@
       <c r="AD44" s="1"/>
       <c r="AE44" s="1"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2788,7 +2796,7 @@
       <c r="AD45" s="1"/>
       <c r="AE45" s="1"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2819,7 +2827,7 @@
       <c r="AD46" s="1"/>
       <c r="AE46" s="1"/>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2850,7 +2858,7 @@
       <c r="AD47" s="1"/>
       <c r="AE47" s="1"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2881,7 +2889,7 @@
       <c r="AD48" s="1"/>
       <c r="AE48" s="1"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2912,7 +2920,7 @@
       <c r="AD49" s="1"/>
       <c r="AE49" s="1"/>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2943,7 +2951,7 @@
       <c r="AD50" s="1"/>
       <c r="AE50" s="1"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2974,7 +2982,7 @@
       <c r="AD51" s="1"/>
       <c r="AE51" s="1"/>
     </row>
-    <row r="52" spans="1:31">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -3005,7 +3013,7 @@
       <c r="AD52" s="1"/>
       <c r="AE52" s="1"/>
     </row>
-    <row r="53" spans="1:31">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3036,7 +3044,7 @@
       <c r="AD53" s="1"/>
       <c r="AE53" s="1"/>
     </row>
-    <row r="54" spans="1:31">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -3067,7 +3075,7 @@
       <c r="AD54" s="1"/>
       <c r="AE54" s="1"/>
     </row>
-    <row r="55" spans="1:31">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -3098,7 +3106,7 @@
       <c r="AD55" s="1"/>
       <c r="AE55" s="1"/>
     </row>
-    <row r="56" spans="1:31">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -3129,7 +3137,7 @@
       <c r="AD56" s="1"/>
       <c r="AE56" s="1"/>
     </row>
-    <row r="57" spans="1:31">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -3160,7 +3168,7 @@
       <c r="AD57" s="1"/>
       <c r="AE57" s="1"/>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -3191,7 +3199,7 @@
       <c r="AD58" s="1"/>
       <c r="AE58" s="1"/>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -3222,7 +3230,7 @@
       <c r="AD59" s="1"/>
       <c r="AE59" s="1"/>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -3250,7 +3258,7 @@
       <c r="AD60" s="1"/>
       <c r="AE60" s="1"/>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -3275,7 +3283,7 @@
       <c r="AD61" s="1"/>
       <c r="AE61" s="1"/>
     </row>
-    <row r="62" spans="1:31">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -3300,7 +3308,7 @@
       <c r="AD62" s="1"/>
       <c r="AE62" s="1"/>
     </row>
-    <row r="63" spans="1:31">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3325,7 +3333,7 @@
       <c r="AD63" s="1"/>
       <c r="AE63" s="1"/>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -3350,7 +3358,7 @@
       <c r="AD64" s="1"/>
       <c r="AE64" s="1"/>
     </row>
-    <row r="65" spans="1:31">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -3375,7 +3383,7 @@
       <c r="AD65" s="1"/>
       <c r="AE65" s="1"/>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -3400,7 +3408,7 @@
       <c r="AD66" s="1"/>
       <c r="AE66" s="1"/>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -3425,7 +3433,7 @@
       <c r="AD67" s="1"/>
       <c r="AE67" s="1"/>
     </row>
-    <row r="68" spans="1:31">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -3450,7 +3458,7 @@
       <c r="AD68" s="1"/>
       <c r="AE68" s="1"/>
     </row>
-    <row r="69" spans="1:31">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3475,7 +3483,7 @@
       <c r="AD69" s="1"/>
       <c r="AE69" s="1"/>
     </row>
-    <row r="70" spans="1:31">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3500,7 +3508,7 @@
       <c r="AD70" s="1"/>
       <c r="AE70" s="1"/>
     </row>
-    <row r="71" spans="1:31">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3525,7 +3533,7 @@
       <c r="AD71" s="1"/>
       <c r="AE71" s="1"/>
     </row>
-    <row r="72" spans="1:31">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -3550,7 +3558,7 @@
       <c r="AD72" s="1"/>
       <c r="AE72" s="1"/>
     </row>
-    <row r="73" spans="1:31">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -3575,7 +3583,7 @@
       <c r="AD73" s="1"/>
       <c r="AE73" s="1"/>
     </row>
-    <row r="74" spans="1:31">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -3600,7 +3608,7 @@
       <c r="AD74" s="1"/>
       <c r="AE74" s="1"/>
     </row>
-    <row r="75" spans="1:31">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -3625,7 +3633,7 @@
       <c r="AD75" s="1"/>
       <c r="AE75" s="1"/>
     </row>
-    <row r="76" spans="1:31">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -3650,7 +3658,7 @@
       <c r="AD76" s="1"/>
       <c r="AE76" s="1"/>
     </row>
-    <row r="77" spans="1:31">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -3675,7 +3683,7 @@
       <c r="AD77" s="1"/>
       <c r="AE77" s="1"/>
     </row>
-    <row r="78" spans="1:31">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -3700,7 +3708,7 @@
       <c r="AD78" s="1"/>
       <c r="AE78" s="1"/>
     </row>
-    <row r="79" spans="1:31">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3725,7 +3733,7 @@
       <c r="AD79" s="1"/>
       <c r="AE79" s="1"/>
     </row>
-    <row r="80" spans="1:31">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3750,7 +3758,7 @@
       <c r="AD80" s="1"/>
       <c r="AE80" s="1"/>
     </row>
-    <row r="81" spans="1:31">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -3775,7 +3783,7 @@
       <c r="AD81" s="1"/>
       <c r="AE81" s="1"/>
     </row>
-    <row r="82" spans="1:31">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -3800,7 +3808,7 @@
       <c r="AD82" s="1"/>
       <c r="AE82" s="1"/>
     </row>
-    <row r="83" spans="1:31">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -3825,7 +3833,7 @@
       <c r="AD83" s="1"/>
       <c r="AE83" s="1"/>
     </row>
-    <row r="84" spans="1:31">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -3850,7 +3858,7 @@
       <c r="AD84" s="1"/>
       <c r="AE84" s="1"/>
     </row>
-    <row r="85" spans="1:31">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -3875,7 +3883,7 @@
       <c r="AD85" s="1"/>
       <c r="AE85" s="1"/>
     </row>
-    <row r="86" spans="1:31">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -3900,7 +3908,7 @@
       <c r="AD86" s="1"/>
       <c r="AE86" s="1"/>
     </row>
-    <row r="87" spans="1:31">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -3925,7 +3933,7 @@
       <c r="AD87" s="1"/>
       <c r="AE87" s="1"/>
     </row>
-    <row r="88" spans="1:31">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -3950,7 +3958,7 @@
       <c r="AD88" s="1"/>
       <c r="AE88" s="1"/>
     </row>
-    <row r="89" spans="1:31">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -3975,7 +3983,7 @@
       <c r="AD89" s="1"/>
       <c r="AE89" s="1"/>
     </row>
-    <row r="90" spans="1:31">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -4000,7 +4008,7 @@
       <c r="AD90" s="1"/>
       <c r="AE90" s="1"/>
     </row>
-    <row r="91" spans="1:31">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -4025,7 +4033,7 @@
       <c r="AD91" s="1"/>
       <c r="AE91" s="1"/>
     </row>
-    <row r="92" spans="1:31">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -4050,7 +4058,7 @@
       <c r="AD92" s="1"/>
       <c r="AE92" s="1"/>
     </row>
-    <row r="93" spans="1:31">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -4075,7 +4083,7 @@
       <c r="AD93" s="1"/>
       <c r="AE93" s="1"/>
     </row>
-    <row r="94" spans="1:31">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -4100,7 +4108,7 @@
       <c r="AD94" s="1"/>
       <c r="AE94" s="1"/>
     </row>
-    <row r="95" spans="1:31">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -4125,7 +4133,7 @@
       <c r="AD95" s="1"/>
       <c r="AE95" s="1"/>
     </row>
-    <row r="96" spans="1:31">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -4150,7 +4158,7 @@
       <c r="AD96" s="1"/>
       <c r="AE96" s="1"/>
     </row>
-    <row r="97" spans="1:31">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -4175,7 +4183,7 @@
       <c r="AD97" s="1"/>
       <c r="AE97" s="1"/>
     </row>
-    <row r="98" spans="1:31">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -4200,7 +4208,7 @@
       <c r="AD98" s="1"/>
       <c r="AE98" s="1"/>
     </row>
-    <row r="99" spans="1:31">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -4225,7 +4233,7 @@
       <c r="AD99" s="1"/>
       <c r="AE99" s="1"/>
     </row>
-    <row r="100" spans="1:31">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -4250,7 +4258,7 @@
       <c r="AD100" s="1"/>
       <c r="AE100" s="1"/>
     </row>
-    <row r="101" spans="1:31">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -4275,7 +4283,7 @@
       <c r="AD101" s="1"/>
       <c r="AE101" s="1"/>
     </row>
-    <row r="102" spans="1:31">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -4300,7 +4308,7 @@
       <c r="AD102" s="1"/>
       <c r="AE102" s="1"/>
     </row>
-    <row r="103" spans="1:31">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -4325,7 +4333,7 @@
       <c r="AD103" s="1"/>
       <c r="AE103" s="1"/>
     </row>
-    <row r="104" spans="1:31">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -4350,7 +4358,7 @@
       <c r="AD104" s="1"/>
       <c r="AE104" s="1"/>
     </row>
-    <row r="105" spans="1:31">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -4375,7 +4383,7 @@
       <c r="AD105" s="1"/>
       <c r="AE105" s="1"/>
     </row>
-    <row r="106" spans="1:31">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -4400,7 +4408,7 @@
       <c r="AD106" s="1"/>
       <c r="AE106" s="1"/>
     </row>
-    <row r="107" spans="1:31">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -4425,7 +4433,7 @@
       <c r="AD107" s="1"/>
       <c r="AE107" s="1"/>
     </row>
-    <row r="108" spans="1:31">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -4450,7 +4458,7 @@
       <c r="AD108" s="1"/>
       <c r="AE108" s="1"/>
     </row>
-    <row r="109" spans="1:31">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -4475,7 +4483,7 @@
       <c r="AD109" s="1"/>
       <c r="AE109" s="1"/>
     </row>
-    <row r="110" spans="1:31">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -4500,7 +4508,7 @@
       <c r="AD110" s="1"/>
       <c r="AE110" s="1"/>
     </row>
-    <row r="111" spans="1:31">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -4525,7 +4533,7 @@
       <c r="AD111" s="1"/>
       <c r="AE111" s="1"/>
     </row>
-    <row r="112" spans="1:31">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -4550,7 +4558,7 @@
       <c r="AD112" s="1"/>
       <c r="AE112" s="1"/>
     </row>
-    <row r="113" spans="1:31">
+    <row r="113" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -4575,7 +4583,7 @@
       <c r="AD113" s="1"/>
       <c r="AE113" s="1"/>
     </row>
-    <row r="114" spans="1:31">
+    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -4600,7 +4608,7 @@
       <c r="AD114" s="1"/>
       <c r="AE114" s="1"/>
     </row>
-    <row r="115" spans="1:31">
+    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -4625,7 +4633,7 @@
       <c r="AD115" s="1"/>
       <c r="AE115" s="1"/>
     </row>
-    <row r="116" spans="1:31">
+    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -4650,7 +4658,7 @@
       <c r="AD116" s="1"/>
       <c r="AE116" s="1"/>
     </row>
-    <row r="117" spans="1:31">
+    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -4675,7 +4683,7 @@
       <c r="AD117" s="1"/>
       <c r="AE117" s="1"/>
     </row>
-    <row r="118" spans="1:31">
+    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -4699,7 +4707,7 @@
       <c r="AD118" s="1"/>
       <c r="AE118" s="1"/>
     </row>
-    <row r="119" spans="1:31">
+    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -4723,7 +4731,7 @@
       <c r="AD119" s="1"/>
       <c r="AE119" s="1"/>
     </row>
-    <row r="120" spans="1:31">
+    <row r="120" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -4746,7 +4754,7 @@
       <c r="AD120" s="1"/>
       <c r="AE120" s="1"/>
     </row>
-    <row r="121" spans="1:31">
+    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="H121" s="12"/>
       <c r="I121" s="5"/>
@@ -4767,7 +4775,7 @@
       <c r="AD121" s="1"/>
       <c r="AE121" s="1"/>
     </row>
-    <row r="122" spans="1:31">
+    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="H122" s="12"/>
       <c r="I122" s="5"/>
@@ -4788,7 +4796,7 @@
       <c r="AD122" s="1"/>
       <c r="AE122" s="1"/>
     </row>
-    <row r="123" spans="1:31">
+    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="H123" s="12"/>
       <c r="I123" s="5"/>
@@ -4809,7 +4817,7 @@
       <c r="AD123" s="1"/>
       <c r="AE123" s="1"/>
     </row>
-    <row r="124" spans="1:31">
+    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="H124" s="12"/>
       <c r="I124" s="5"/>
@@ -4830,7 +4838,7 @@
       <c r="AD124" s="1"/>
       <c r="AE124" s="1"/>
     </row>
-    <row r="125" spans="1:31">
+    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="H125" s="12"/>
       <c r="I125" s="5"/>
@@ -4851,7 +4859,7 @@
       <c r="AD125" s="1"/>
       <c r="AE125" s="1"/>
     </row>
-    <row r="126" spans="1:31">
+    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="H126" s="12"/>
       <c r="I126" s="5"/>
@@ -4872,7 +4880,7 @@
       <c r="AD126" s="1"/>
       <c r="AE126" s="1"/>
     </row>
-    <row r="127" spans="1:31">
+    <row r="127" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="H127" s="12"/>
       <c r="I127" s="5"/>
@@ -4893,7 +4901,7 @@
       <c r="AD127" s="1"/>
       <c r="AE127" s="1"/>
     </row>
-    <row r="128" spans="1:31">
+    <row r="128" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="H128" s="12"/>
       <c r="I128" s="5"/>
@@ -4914,7 +4922,7 @@
       <c r="AD128" s="1"/>
       <c r="AE128" s="1"/>
     </row>
-    <row r="129" spans="1:31">
+    <row r="129" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="H129" s="12"/>
       <c r="I129" s="5"/>
@@ -4935,7 +4943,7 @@
       <c r="AD129" s="1"/>
       <c r="AE129" s="1"/>
     </row>
-    <row r="130" spans="1:31">
+    <row r="130" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="H130" s="12"/>
       <c r="I130" s="5"/>
@@ -4956,7 +4964,7 @@
       <c r="AD130" s="1"/>
       <c r="AE130" s="1"/>
     </row>
-    <row r="131" spans="1:31">
+    <row r="131" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="H131" s="12"/>
       <c r="I131" s="5"/>
@@ -4977,7 +4985,7 @@
       <c r="AD131" s="1"/>
       <c r="AE131" s="1"/>
     </row>
-    <row r="132" spans="1:31">
+    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="H132" s="12"/>
       <c r="I132" s="5"/>
@@ -4998,7 +5006,7 @@
       <c r="AD132" s="1"/>
       <c r="AE132" s="1"/>
     </row>
-    <row r="133" spans="1:31">
+    <row r="133" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="H133" s="12"/>
       <c r="I133" s="5"/>
@@ -5019,179 +5027,179 @@
       <c r="AD133" s="1"/>
       <c r="AE133" s="1"/>
     </row>
-    <row r="134" spans="1:31">
+    <row r="134" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="I134" s="5"/>
     </row>
-    <row r="135" spans="1:31">
+    <row r="135" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="I135" s="5"/>
     </row>
-    <row r="136" spans="1:31">
+    <row r="136" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="I136" s="5"/>
     </row>
-    <row r="137" spans="1:31">
+    <row r="137" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="I137" s="5"/>
     </row>
-    <row r="138" spans="1:31">
+    <row r="138" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="I138" s="5"/>
     </row>
-    <row r="139" spans="1:31">
+    <row r="139" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="I139" s="5"/>
     </row>
-    <row r="140" spans="1:31">
+    <row r="140" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="I140" s="5"/>
     </row>
-    <row r="141" spans="1:31">
+    <row r="141" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="I141" s="5"/>
     </row>
-    <row r="142" spans="1:31">
+    <row r="142" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="I142" s="5"/>
     </row>
-    <row r="143" spans="1:31">
+    <row r="143" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="I143" s="5"/>
     </row>
-    <row r="144" spans="1:31">
+    <row r="144" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="I144" s="5"/>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="I145" s="5"/>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="I146" s="5"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="I147" s="5"/>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
       <c r="I148" s="5"/>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
       <c r="I149" s="5"/>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
       <c r="I150" s="5"/>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
       <c r="I151" s="5"/>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="I152" s="5"/>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
       <c r="I153" s="5"/>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
       <c r="I154" s="5"/>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
       <c r="I155" s="5"/>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
       <c r="I156" s="5"/>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="I157" s="5"/>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
       <c r="I158" s="5"/>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
       <c r="I159" s="5"/>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
       <c r="I160" s="5"/>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="I161" s="5"/>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="I162" s="5"/>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="I163" s="5"/>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="I164" s="5"/>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="I165" s="5"/>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="I166" s="5"/>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="I167" s="5"/>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="I168" s="5"/>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="I169" s="5"/>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="I170" s="5"/>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="I171" s="5"/>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="I172" s="5"/>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="I173" s="5"/>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
       <c r="I174" s="5"/>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="I175" s="5"/>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="I176" s="5"/>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
       <c r="I177" s="5"/>
     </row>
@@ -5207,13 +5215,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.44140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" style="1" customWidth="1"/>
@@ -5224,7 +5232,7 @@
     <col min="7" max="7" width="13.109375" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -5247,7 +5255,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>66</v>
       </c>
@@ -5262,7 +5270,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>66</v>
       </c>
@@ -5277,7 +5285,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>66</v>
       </c>
@@ -5292,7 +5300,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>66</v>
       </c>
@@ -5307,7 +5315,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>66</v>
       </c>
@@ -5322,7 +5330,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>66</v>
       </c>
@@ -5337,7 +5345,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>66</v>
       </c>
@@ -5352,7 +5360,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>67</v>
       </c>
@@ -5367,7 +5375,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>67</v>
       </c>
@@ -5382,7 +5390,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
@@ -5397,7 +5405,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5412,7 +5420,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>67</v>
       </c>
@@ -5427,7 +5435,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>67</v>
       </c>
@@ -5442,7 +5450,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>67</v>
       </c>
@@ -5457,7 +5465,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>67</v>
       </c>
@@ -5472,7 +5480,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>67</v>
       </c>
@@ -5487,7 +5495,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>67</v>
       </c>
@@ -5502,7 +5510,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>67</v>
       </c>
@@ -5517,7 +5525,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>67</v>
       </c>
@@ -5532,7 +5540,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>67</v>
       </c>
@@ -5547,7 +5555,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>138</v>
       </c>
@@ -5562,7 +5570,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>138</v>
       </c>
@@ -5577,7 +5585,7 @@
       <c r="F23" s="8"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>138</v>
       </c>
@@ -5592,7 +5600,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>138</v>
       </c>
@@ -5607,7 +5615,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>138</v>
       </c>
@@ -5622,7 +5630,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>138</v>
       </c>
@@ -5637,7 +5645,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>138</v>
       </c>
@@ -5652,7 +5660,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>6</v>
       </c>
@@ -5667,7 +5675,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>6</v>
       </c>
@@ -5682,7 +5690,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>6</v>
       </c>
@@ -5697,7 +5705,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>6</v>
       </c>
@@ -5712,7 +5720,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>6</v>
       </c>
@@ -5727,7 +5735,7 @@
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>6</v>
       </c>
@@ -5742,7 +5750,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>3</v>
       </c>
@@ -5757,7 +5765,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>3</v>
       </c>
@@ -5772,7 +5780,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>3</v>
       </c>
@@ -5787,42 +5795,42 @@
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>60</v>
+        <v>147</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="1:7">
+        <v>146</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="8"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="1"/>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>127</v>
@@ -5832,12 +5840,12 @@
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>127</v>
@@ -5847,12 +5855,12 @@
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>127</v>
@@ -5862,108 +5870,115 @@
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="9"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="9"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="10"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="15"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="C45" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="G44" s="9"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="10"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" ht="36">
-      <c r="A47" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>102</v>
-      </c>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="3"/>
+      <c r="F47" s="1"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7" ht="409.6">
+    <row r="48" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>100</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="10"/>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="3"/>
+      <c r="F52" s="1"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -5971,7 +5986,7 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -5979,7 +5994,7 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -5987,7 +6002,7 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -5995,7 +6010,7 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -6003,7 +6018,7 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -6011,7 +6026,7 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -6019,23 +6034,23 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="11"/>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="10"/>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -6043,479 +6058,487 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="5"/>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="E63" s="1"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="5"/>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="5"/>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="5"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Nov 9 before class
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF23C042-013F-45E2-8E54-E5DEE05A31FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3222D1-81DE-4B5E-B164-2CB25CE69EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t>TCP拥塞控制机制</t>
+  </si>
+  <si>
+    <t>IP协议极简笔记</t>
   </si>
 </sst>
 </file>
@@ -884,7 +887,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1061,8 +1064,8 @@
       <c r="G5" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>113</v>
+      <c r="H5" s="15" t="s">
+        <v>120</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="14" t="s">
@@ -1099,7 +1102,7 @@
         <v>109</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="14" t="s">
@@ -1135,8 +1138,8 @@
       <c r="G7" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>120</v>
+      <c r="H7" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="14" t="s">
@@ -1172,8 +1175,8 @@
       <c r="G8" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>46</v>
+      <c r="H8" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="14" t="s">
@@ -1210,7 +1213,7 @@
         <v>109</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="14" t="s">
@@ -1247,7 +1250,7 @@
         <v>109</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="14" t="s">
@@ -1280,11 +1283,11 @@
         <v>67</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="4" t="s">
-        <v>6</v>
+      <c r="G11" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="14" t="s">
@@ -1321,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="14" t="s">
@@ -1358,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="14" t="s">
@@ -1395,7 +1398,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="14" t="s">
@@ -1432,7 +1435,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="14" t="s">
@@ -1469,7 +1472,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="14" t="s">
@@ -1503,10 +1506,10 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="14" t="s">
@@ -1540,10 +1543,10 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>20</v>
+        <v>118</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="14" t="s">
@@ -1579,8 +1582,8 @@
       <c r="G19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>21</v>
+      <c r="H19" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="14" t="s">
@@ -1616,8 +1619,8 @@
       <c r="G20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>114</v>
+      <c r="H20" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="14" t="s">
@@ -1653,8 +1656,8 @@
       <c r="G21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="10" t="s">
-        <v>55</v>
+      <c r="H21" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="14" t="s">
@@ -1690,8 +1693,8 @@
       <c r="G22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="11" t="s">
-        <v>22</v>
+      <c r="H22" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="2"/>
@@ -1724,7 +1727,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="2"/>
@@ -1757,7 +1760,7 @@
         <v>3</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="2"/>
@@ -1790,7 +1793,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="2"/>
@@ -1816,8 +1819,8 @@
       <c r="G26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="10" t="s">
-        <v>25</v>
+      <c r="H26" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="2"/>
@@ -1840,8 +1843,12 @@
         <v>100</v>
       </c>
       <c r="F27" s="7"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="G27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="I27" s="7"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1882,7 +1889,7 @@
       <c r="D29" s="6"/>
       <c r="F29" s="7"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="15"/>
+      <c r="H29" s="2"/>
       <c r="I29" s="7"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -1903,7 +1910,7 @@
       <c r="D30" s="2"/>
       <c r="F30" s="7"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="H30" s="15"/>
       <c r="I30" s="7"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -2233,8 +2240,8 @@
       <c r="C47" s="7"/>
       <c r="D47" s="2"/>
       <c r="F47" s="7"/>
-      <c r="G47"/>
-      <c r="H47"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
       <c r="I47" s="7"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -2271,8 +2278,8 @@
       <c r="C49" s="7"/>
       <c r="D49" s="2"/>
       <c r="F49" s="7"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="G49"/>
+      <c r="H49"/>
       <c r="I49" s="7"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -3544,6 +3551,8 @@
       <c r="C116" s="7"/>
       <c r="D116" s="2"/>
       <c r="F116" s="7"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
       <c r="I116" s="7"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>

</xml_diff>

<commit_message>
Nov 23 before class
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3222D1-81DE-4B5E-B164-2CB25CE69EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADE0117-64CE-4316-ADA5-A94985F4F0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="123">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>IP协议极简笔记</t>
+  </si>
+  <si>
+    <t>Tor与洋葱路由的技术原理</t>
   </si>
 </sst>
 </file>
@@ -887,7 +890,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1212,8 +1215,8 @@
       <c r="G9" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>46</v>
+      <c r="H9" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="14" t="s">
@@ -1250,7 +1253,7 @@
         <v>109</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="14" t="s">
@@ -1287,7 +1290,7 @@
         <v>109</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="14" t="s">
@@ -1320,11 +1323,11 @@
         <v>61</v>
       </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="4" t="s">
-        <v>6</v>
+      <c r="G12" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="14" t="s">
@@ -1361,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="14" t="s">
@@ -1398,7 +1401,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="14" t="s">
@@ -1435,7 +1438,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="14" t="s">
@@ -1472,7 +1475,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="14" t="s">
@@ -1509,7 +1512,7 @@
         <v>6</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="14" t="s">
@@ -1543,10 +1546,10 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="14" t="s">
@@ -1580,10 +1583,10 @@
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>20</v>
+        <v>118</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="14" t="s">
@@ -1619,8 +1622,8 @@
       <c r="G20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="11" t="s">
-        <v>21</v>
+      <c r="H20" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="14" t="s">
@@ -1656,8 +1659,8 @@
       <c r="G21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>114</v>
+      <c r="H21" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="14" t="s">
@@ -1693,8 +1696,8 @@
       <c r="G22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>55</v>
+      <c r="H22" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="2"/>
@@ -1726,8 +1729,8 @@
       <c r="G23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>22</v>
+      <c r="H23" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="2"/>
@@ -1760,7 +1763,7 @@
         <v>3</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="2"/>
@@ -1793,7 +1796,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="2"/>
@@ -1820,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="2"/>
@@ -1846,8 +1849,8 @@
       <c r="G27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="10" t="s">
-        <v>25</v>
+      <c r="H27" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="2"/>
@@ -1870,8 +1873,12 @@
         <v>108</v>
       </c>
       <c r="F28" s="7"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="I28" s="7"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -1910,7 +1917,7 @@
       <c r="D30" s="2"/>
       <c r="F30" s="7"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="15"/>
+      <c r="H30" s="2"/>
       <c r="I30" s="7"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1931,7 +1938,7 @@
       <c r="D31" s="2"/>
       <c r="F31" s="7"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="H31" s="15"/>
       <c r="I31" s="7"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -2259,8 +2266,8 @@
       <c r="C48" s="7"/>
       <c r="D48" s="2"/>
       <c r="F48" s="7"/>
-      <c r="G48"/>
-      <c r="H48"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
       <c r="I48" s="7"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -2297,8 +2304,8 @@
       <c r="C50" s="7"/>
       <c r="D50" s="2"/>
       <c r="F50" s="7"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="G50"/>
+      <c r="H50"/>
       <c r="I50" s="7"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -3570,6 +3577,8 @@
       <c r="C117" s="7"/>
       <c r="D117" s="2"/>
       <c r="F117" s="7"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
       <c r="I117" s="7"/>
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>

</xml_diff>

<commit_message>
Finish Network Layer blog
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADE0117-64CE-4316-ADA5-A94985F4F0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D53B96-630C-4DEB-A4BD-6AB6B02D90F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="124">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>Tor与洋葱路由的技术原理</t>
+  </si>
+  <si>
+    <t>PostgreSQL操作笔记</t>
   </si>
 </sst>
 </file>
@@ -886,11 +889,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S177"/>
+  <dimension ref="A1:S178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1541,8 +1544,8 @@
       <c r="D18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>70</v>
+      <c r="E18" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="4" t="s">
@@ -1576,10 +1579,10 @@
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>72</v>
+        <v>2</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="4" t="s">
@@ -1615,8 +1618,8 @@
       <c r="D20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>69</v>
+      <c r="E20" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="4" t="s">
@@ -1653,7 +1656,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="4" t="s">
@@ -1690,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="4" t="s">
@@ -1722,8 +1725,8 @@
       <c r="D23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>105</v>
+      <c r="E23" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="4" t="s">
@@ -1756,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="4" t="s">
@@ -1788,8 +1791,8 @@
       <c r="D25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>71</v>
+      <c r="E25" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="4" t="s">
@@ -1816,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="4" t="s">
@@ -1842,8 +1845,8 @@
       <c r="D27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>100</v>
+      <c r="E27" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="4" t="s">
@@ -1870,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="4" t="s">
@@ -1893,7 +1896,12 @@
     </row>
     <row r="29" spans="1:19">
       <c r="C29" s="7"/>
-      <c r="D29" s="6"/>
+      <c r="D29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1914,7 +1922,7 @@
         <v>116</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="6"/>
       <c r="F30" s="7"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -2226,7 +2234,8 @@
       <c r="C45" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
@@ -2245,7 +2254,8 @@
     <row r="47" spans="1:19">
       <c r="A47" s="2"/>
       <c r="C47" s="7"/>
-      <c r="D47" s="2"/>
+      <c r="D47" s="1"/>
+      <c r="E47"/>
       <c r="F47" s="7"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2435,7 +2445,7 @@
     <row r="57" spans="1:19">
       <c r="A57" s="6"/>
       <c r="C57" s="7"/>
-      <c r="D57" s="6"/>
+      <c r="D57" s="2"/>
       <c r="F57" s="7"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -2454,7 +2464,7 @@
     <row r="58" spans="1:19">
       <c r="A58" s="2"/>
       <c r="C58" s="7"/>
-      <c r="D58" s="2"/>
+      <c r="D58" s="6"/>
       <c r="F58" s="7"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -4039,6 +4049,9 @@
       <c r="A177" s="2"/>
       <c r="D177" s="2"/>
     </row>
+    <row r="178" spans="1:4">
+      <c r="D178" s="2"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B41">
     <sortCondition ref="A2:A41"/>

</xml_diff>

<commit_message>
Add blog: Python Pandas
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D53B96-630C-4DEB-A4BD-6AB6B02D90F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E1AFAD-252B-4315-85C4-2680C4FA64FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="125">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -455,6 +455,9 @@
   </si>
   <si>
     <t>PostgreSQL操作笔记</t>
+  </si>
+  <si>
+    <t>Pandas笔记</t>
   </si>
 </sst>
 </file>
@@ -893,7 +896,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1551,8 +1554,8 @@
       <c r="G18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>16</v>
+      <c r="H18" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="14" t="s">
@@ -1586,10 +1589,10 @@
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="14" t="s">
@@ -1623,10 +1626,10 @@
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>20</v>
+        <v>118</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="14" t="s">
@@ -1662,8 +1665,8 @@
       <c r="G21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>21</v>
+      <c r="H21" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="14" t="s">
@@ -1699,8 +1702,8 @@
       <c r="G22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>114</v>
+      <c r="H22" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="2"/>
@@ -1732,8 +1735,8 @@
       <c r="G23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="10" t="s">
-        <v>55</v>
+      <c r="H23" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="2"/>
@@ -1765,8 +1768,8 @@
       <c r="G24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="11" t="s">
-        <v>22</v>
+      <c r="H24" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="2"/>
@@ -1799,7 +1802,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="2"/>
@@ -1826,7 +1829,7 @@
         <v>3</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="2"/>
@@ -1853,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="2"/>
@@ -1879,8 +1882,8 @@
       <c r="G28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="10" t="s">
-        <v>25</v>
+      <c r="H28" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="2"/>
@@ -1903,8 +1906,12 @@
         <v>108</v>
       </c>
       <c r="F29" s="7"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="G29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="I29" s="7"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -1946,7 +1953,7 @@
       <c r="D31" s="2"/>
       <c r="F31" s="7"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="15"/>
+      <c r="H31" s="2"/>
       <c r="I31" s="7"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1967,7 +1974,7 @@
       <c r="D32" s="2"/>
       <c r="F32" s="7"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="15"/>
       <c r="I32" s="7"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -2295,8 +2302,8 @@
       <c r="C49" s="7"/>
       <c r="D49" s="2"/>
       <c r="F49" s="7"/>
-      <c r="G49"/>
-      <c r="H49"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
       <c r="I49" s="7"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -2333,8 +2340,8 @@
       <c r="C51" s="7"/>
       <c r="D51" s="2"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
+      <c r="G51"/>
+      <c r="H51"/>
       <c r="I51" s="7"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -3606,6 +3613,8 @@
       <c r="C118" s="7"/>
       <c r="D118" s="2"/>
       <c r="F118" s="7"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
       <c r="I118" s="7"/>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>

</xml_diff>

<commit_message>
Finish Image Classification and Format
</commit_message>
<xml_diff>
--- a/进度表.xlsx
+++ b/进度表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407A508E-E7DE-4CA4-B895-BB7BD2F1D22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63C3E08-5B7A-4436-8034-A1A630579AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="912" yWindow="-108" windowWidth="22236" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="127">
   <si>
     <t>Algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -463,6 +463,9 @@
   <si>
     <t>前缀和算法优化合集</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像格式与分类</t>
   </si>
 </sst>
 </file>
@@ -899,9 +902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1717,9 @@
       <c r="J22" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K22" s="2"/>
+      <c r="K22" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>

</xml_diff>